<commit_message>
Site updated: 2022-04-18 22:16:30
</commit_message>
<xml_diff>
--- a/file/personal/roleImportant/角色要事记录表_2022.xlsx
+++ b/file/personal/roleImportant/角色要事记录表_2022.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="67">
   <si>
     <t>角色</t>
   </si>
@@ -2972,7 +2972,7 @@
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection/>
-      <selection pane="topRight" activeCell="G6" sqref="G6"/>
+      <selection pane="topRight" activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3365384615385" defaultRowHeight="13" customHeight="1" outlineLevelCol="7"/>
@@ -3085,7 +3085,9 @@
       <c r="D7" s="14"/>
       <c r="E7" s="14"/>
       <c r="F7" s="14"/>
-      <c r="G7" s="14"/>
+      <c r="G7" s="23" t="s">
+        <v>34</v>
+      </c>
       <c r="H7" s="14"/>
     </row>
     <row r="8" ht="13.65" customHeight="1" spans="1:8">
@@ -3212,7 +3214,7 @@
     <mergeCell ref="A15:A17"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G5 G6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G5 G6 G7">
       <formula1>"未进行,进行中,已暂停,已完成"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Site updated: 2022-05-01 23:30:20
</commit_message>
<xml_diff>
--- a/file/personal/roleImportant/角色要事记录表_2022.xlsx
+++ b/file/personal/roleImportant/角色要事记录表_2022.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="16860" activeTab="2"/>
+    <workbookView windowHeight="14660" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="角色目录" sheetId="2" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="68">
   <si>
     <t>角色</t>
   </si>
@@ -198,22 +198,25 @@
     <t>第一周</t>
   </si>
   <si>
+    <t>家庭保险资料整理</t>
+  </si>
+  <si>
+    <t>保险知识简单整理</t>
+  </si>
+  <si>
+    <t>国家经济转型重点会发展哪些行业？</t>
+  </si>
+  <si>
+    <t>第二周</t>
+  </si>
+  <si>
+    <t>第三周</t>
+  </si>
+  <si>
     <t>面试准备计划</t>
   </si>
   <si>
-    <t>家庭保险资料整理</t>
-  </si>
-  <si>
-    <t>保险知识简单整理</t>
-  </si>
-  <si>
-    <t>国家经济转型重点会发展哪些行业？</t>
-  </si>
-  <si>
-    <t>第二周</t>
-  </si>
-  <si>
-    <t>第三周</t>
+    <t>养老行业/大健康行业的常青藤职业是什么</t>
   </si>
   <si>
     <t>第四周</t>
@@ -224,10 +227,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -235,6 +238,13 @@
       <color indexed="8"/>
       <name val="SimSun"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -246,17 +256,24 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Helvetica Neue"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color theme="3"/>
       <name val="Helvetica Neue"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -267,8 +284,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="Helvetica Neue"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -282,10 +300,34 @@
     </font>
     <font>
       <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Helvetica Neue"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF800080"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Helvetica Neue"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -299,14 +341,15 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="1"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF0000FF"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -327,41 +370,10 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Helvetica Neue"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Helvetica Neue"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Helvetica Neue"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -372,17 +384,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C0006"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -458,60 +461,174 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -519,120 +636,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -704,21 +707,6 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="13"/>
-      </left>
-      <right style="thin">
-        <color indexed="17"/>
-      </right>
-      <top style="thin">
-        <color indexed="13"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="17"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color indexed="17"/>
       </left>
       <right style="thin">
@@ -783,6 +771,21 @@
       <top/>
       <bottom style="thin">
         <color indexed="13"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="13"/>
+      </left>
+      <right style="thin">
+        <color indexed="17"/>
+      </right>
+      <top style="thin">
+        <color indexed="13"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="17"/>
       </bottom>
       <diagonal/>
     </border>
@@ -945,8 +948,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -966,17 +969,20 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -992,24 +998,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1039,153 +1027,168 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="40" borderId="24" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="24" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="30" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="25" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="18" borderId="29" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="28" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="24" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="24" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="29" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="30" borderId="30" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="28" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="26" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="26" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="28" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="27" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="27" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="26" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="25" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1220,26 +1223,26 @@
     <xf numFmtId="49" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -2946,7 +2949,7 @@
     <row r="18" ht="13.35" customHeight="1" spans="1:3">
       <c r="A18" s="36"/>
       <c r="B18" s="34"/>
-      <c r="C18" s="14"/>
+      <c r="C18" s="13"/>
     </row>
   </sheetData>
   <dataValidations count="1">
@@ -2972,7 +2975,7 @@
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection/>
-      <selection pane="topRight" activeCell="H6" sqref="H6"/>
+      <selection pane="topRight" activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3365384615385" defaultRowHeight="13" customHeight="1" outlineLevelCol="7"/>
@@ -3038,173 +3041,174 @@
       <c r="A4" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+    </row>
+    <row r="5" ht="13.35" customHeight="1" spans="1:8">
+      <c r="A5" s="11"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="11"/>
-    </row>
-    <row r="5" ht="13.35" customHeight="1" spans="1:8">
-      <c r="A5" s="12"/>
-      <c r="B5" s="13"/>
-      <c r="C5" s="14"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="F5" s="14"/>
+      <c r="F5" s="13"/>
       <c r="G5" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="H5" s="14"/>
+      <c r="H5" s="13"/>
     </row>
     <row r="6" ht="13.35" customHeight="1" spans="1:8">
-      <c r="A6" s="12"/>
-      <c r="B6" s="15"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14" t="s">
-        <v>62</v>
-      </c>
-      <c r="F6" s="14"/>
+      <c r="A6" s="11"/>
+      <c r="B6" s="14"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="F6" s="13"/>
       <c r="G6" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="H6" s="14"/>
+      <c r="H6" s="13"/>
     </row>
     <row r="7" ht="13.35" customHeight="1" spans="1:8">
-      <c r="A7" s="12"/>
-      <c r="B7" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="C7" s="14"/>
-      <c r="D7" s="14"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
+      <c r="A7" s="11"/>
+      <c r="B7" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
       <c r="G7" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="H7" s="14"/>
+      <c r="H7" s="13"/>
     </row>
     <row r="8" ht="13.65" customHeight="1" spans="1:8">
-      <c r="A8" s="16"/>
-      <c r="B8" s="15"/>
-      <c r="C8" s="14"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="14"/>
-      <c r="H8" s="14"/>
+      <c r="A8" s="15"/>
+      <c r="B8" s="14"/>
+      <c r="C8" s="13"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="13"/>
     </row>
     <row r="9" ht="13.65" customHeight="1" spans="1:8">
       <c r="A9" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="B9" s="13"/>
-      <c r="C9" s="14"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="14"/>
-      <c r="H9" s="14"/>
+        <v>63</v>
+      </c>
+      <c r="B9" s="12"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="13"/>
     </row>
     <row r="10" ht="13.35" customHeight="1" spans="1:8">
-      <c r="A10" s="12"/>
-      <c r="B10" s="15"/>
-      <c r="C10" s="14"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="14"/>
-      <c r="H10" s="14"/>
+      <c r="A10" s="11"/>
+      <c r="B10" s="14"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="13"/>
     </row>
     <row r="11" ht="13.65" customHeight="1" spans="1:8">
-      <c r="A11" s="16"/>
-      <c r="B11" s="15"/>
-      <c r="C11" s="14"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="14"/>
-      <c r="H11" s="14"/>
+      <c r="A11" s="15"/>
+      <c r="B11" s="14"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
+      <c r="H11" s="13"/>
     </row>
     <row r="12" ht="13.65" customHeight="1" spans="1:8">
       <c r="A12" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="B12" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="B12" s="13"/>
-      <c r="C12" s="14"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="14"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
+      <c r="H12" s="13"/>
     </row>
     <row r="13" ht="13.65" customHeight="1" spans="1:8">
-      <c r="A13" s="12"/>
-      <c r="B13" s="15"/>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="14"/>
+      <c r="A13" s="11"/>
+      <c r="B13" s="14"/>
+      <c r="C13" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="13"/>
     </row>
     <row r="14" ht="14" customHeight="1" spans="1:8">
-      <c r="A14" s="16"/>
-      <c r="B14" s="15"/>
-      <c r="C14" s="14"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="14"/>
-      <c r="G14" s="14"/>
-      <c r="H14" s="14"/>
+      <c r="A14" s="15"/>
+      <c r="B14" s="14"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="13"/>
     </row>
     <row r="15" ht="13.65" customHeight="1" spans="1:8">
       <c r="A15" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="B15" s="13"/>
-      <c r="C15" s="14"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="14"/>
-      <c r="H15" s="14"/>
+        <v>67</v>
+      </c>
+      <c r="B15" s="12"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
+      <c r="H15" s="13"/>
     </row>
     <row r="16" ht="13.35" customHeight="1" spans="1:8">
-      <c r="A16" s="12"/>
-      <c r="B16" s="13"/>
-      <c r="C16" s="14"/>
-      <c r="D16" s="14"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="14"/>
-      <c r="G16" s="14"/>
-      <c r="H16" s="14"/>
+      <c r="A16" s="11"/>
+      <c r="B16" s="12"/>
+      <c r="C16" s="13"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="13"/>
+      <c r="H16" s="13"/>
     </row>
     <row r="17" ht="13.65" customHeight="1" spans="1:8">
-      <c r="A17" s="16"/>
-      <c r="B17" s="15"/>
-      <c r="C17" s="14"/>
-      <c r="D17" s="14"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="14"/>
-      <c r="G17" s="14"/>
-      <c r="H17" s="14"/>
+      <c r="A17" s="15"/>
+      <c r="B17" s="14"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
+      <c r="H17" s="13"/>
     </row>
     <row r="18" ht="13.65" customHeight="1" spans="1:8">
       <c r="A18" s="17"/>
       <c r="B18" s="18"/>
-      <c r="C18" s="14"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="14"/>
-      <c r="G18" s="14"/>
-      <c r="H18" s="14"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="13"/>
+      <c r="H18" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>

<commit_message>
Site updated: 2022-05-04 00:27:31
</commit_message>
<xml_diff>
--- a/file/personal/roleImportant/角色要事记录表_2022.xlsx
+++ b/file/personal/roleImportant/角色要事记录表_2022.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="14660" activeTab="2"/>
+    <workbookView windowWidth="27500" windowHeight="11860" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="角色目录" sheetId="2" r:id="rId1"/>
     <sheet name="待办任务" sheetId="3" r:id="rId2"/>
     <sheet name="四月" sheetId="10" r:id="rId3"/>
+    <sheet name="五月" sheetId="11" r:id="rId4"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="76">
   <si>
     <t>角色</t>
   </si>
@@ -180,6 +181,18 @@
     <t>招聘、学习、考试、岗位</t>
   </si>
   <si>
+    <t>行业职业</t>
+  </si>
+  <si>
+    <t>养老行业/大健康行业的常青藤职业是什么</t>
+  </si>
+  <si>
+    <t>研究第二副业</t>
+  </si>
+  <si>
+    <t>比如做投资人/up主，最好是自己感兴趣的。感兴趣的不一定能做好，但是不感兴趣的一定做不好</t>
+  </si>
+  <si>
     <t>开始时间:</t>
   </si>
   <si>
@@ -216,10 +229,22 @@
     <t>面试准备计划</t>
   </si>
   <si>
-    <t>养老行业/大健康行业的常青藤职业是什么</t>
+    <t>已暂停</t>
+  </si>
+  <si>
+    <t>先进入行业，现在调研太早</t>
   </si>
   <si>
     <t>第四周</t>
+  </si>
+  <si>
+    <t>面试计划</t>
+  </si>
+  <si>
+    <t>家庭事务梳理</t>
+  </si>
+  <si>
+    <t>养生计划梳理</t>
   </si>
 </sst>
 </file>
@@ -227,10 +252,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -248,7 +273,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="1"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -256,7 +281,37 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="3"/>
+      <name val="Helvetica Neue"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Helvetica Neue"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -271,29 +326,53 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Helvetica Neue"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Helvetica Neue"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF9C6500"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -307,27 +386,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF9C0006"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF3F3F76"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Helvetica Neue"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -346,52 +415,8 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="41">
+  <fills count="43">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -419,6 +444,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -455,25 +492,103 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -485,25 +600,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -515,127 +660,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -954,21 +991,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -988,16 +1010,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </right>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1017,17 +1039,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -1042,170 +1053,193 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="33" borderId="24" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="42" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="38" borderId="26" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="26" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="30" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="21" borderId="28" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="27" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="25" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="34" borderId="29" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="24" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="29" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="30" borderId="30" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="28" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="26" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="27" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="26" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="25" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="23" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1223,6 +1257,9 @@
     <xf numFmtId="49" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1250,7 +1287,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1263,30 +1300,36 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="6" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="6" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="8" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="8" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="7" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="9" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="7" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="9" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1298,7 +1341,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1371,7 +1414,7 @@
     <cellStyle name="40% - 强调文字颜色 1" xfId="47" builtinId="31"/>
     <cellStyle name="链接单元格" xfId="48" builtinId="24"/>
   </cellStyles>
-  <tableStyles count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -2525,210 +2568,210 @@
       <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6" defaultRowHeight="13.5" customHeight="1" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9.90384615384615" defaultRowHeight="13.5" customHeight="1" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="9" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="6" style="1" customWidth="1"/>
+    <col min="1" max="1" width="9" style="9" customWidth="1"/>
+    <col min="2" max="16384" width="6" style="9" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="14" customHeight="1" spans="1:5">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
+      <c r="B1" s="39"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
     </row>
     <row r="2" ht="14" customHeight="1" spans="1:5">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="37"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
+      <c r="B2" s="39"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="40"/>
     </row>
     <row r="3" ht="14" customHeight="1" spans="1:5">
-      <c r="A3" s="39" t="s">
+      <c r="A3" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="37"/>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
+      <c r="B3" s="39"/>
+      <c r="C3" s="40"/>
+      <c r="D3" s="40"/>
+      <c r="E3" s="40"/>
     </row>
     <row r="4" ht="14" customHeight="1" spans="1:5">
-      <c r="A4" s="40" t="s">
+      <c r="A4" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="37"/>
-      <c r="C4" s="38"/>
-      <c r="D4" s="38"/>
-      <c r="E4" s="38"/>
+      <c r="B4" s="39"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
     </row>
     <row r="5" ht="14" customHeight="1" spans="1:5">
-      <c r="A5" s="41"/>
-      <c r="B5" s="37"/>
-      <c r="C5" s="38"/>
-      <c r="D5" s="38"/>
-      <c r="E5" s="38"/>
+      <c r="A5" s="43"/>
+      <c r="B5" s="39"/>
+      <c r="C5" s="40"/>
+      <c r="D5" s="40"/>
+      <c r="E5" s="40"/>
     </row>
     <row r="6" ht="14" customHeight="1" spans="1:5">
-      <c r="A6" s="41"/>
-      <c r="B6" s="37"/>
-      <c r="C6" s="38"/>
-      <c r="D6" s="38"/>
-      <c r="E6" s="38"/>
+      <c r="A6" s="43"/>
+      <c r="B6" s="39"/>
+      <c r="C6" s="40"/>
+      <c r="D6" s="40"/>
+      <c r="E6" s="40"/>
     </row>
     <row r="7" ht="14" customHeight="1" spans="1:5">
-      <c r="A7" s="40" t="s">
+      <c r="A7" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="37"/>
-      <c r="C7" s="38"/>
-      <c r="D7" s="38"/>
-      <c r="E7" s="38"/>
+      <c r="B7" s="39"/>
+      <c r="C7" s="40"/>
+      <c r="D7" s="40"/>
+      <c r="E7" s="40"/>
     </row>
     <row r="8" ht="14" customHeight="1" spans="1:5">
-      <c r="A8" s="41"/>
-      <c r="B8" s="37"/>
-      <c r="C8" s="38"/>
-      <c r="D8" s="38"/>
-      <c r="E8" s="38"/>
+      <c r="A8" s="43"/>
+      <c r="B8" s="39"/>
+      <c r="C8" s="40"/>
+      <c r="D8" s="40"/>
+      <c r="E8" s="40"/>
     </row>
     <row r="9" ht="14" customHeight="1" spans="1:5">
-      <c r="A9" s="41"/>
-      <c r="B9" s="37"/>
-      <c r="C9" s="38"/>
-      <c r="D9" s="38"/>
-      <c r="E9" s="38"/>
+      <c r="A9" s="43"/>
+      <c r="B9" s="39"/>
+      <c r="C9" s="40"/>
+      <c r="D9" s="40"/>
+      <c r="E9" s="40"/>
     </row>
     <row r="10" ht="14" customHeight="1" spans="1:5">
-      <c r="A10" s="40" t="s">
+      <c r="A10" s="42" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="37"/>
-      <c r="C10" s="38"/>
-      <c r="D10" s="38"/>
-      <c r="E10" s="38"/>
+      <c r="B10" s="39"/>
+      <c r="C10" s="40"/>
+      <c r="D10" s="40"/>
+      <c r="E10" s="40"/>
     </row>
     <row r="11" ht="14" customHeight="1" spans="1:5">
-      <c r="A11" s="40" t="s">
+      <c r="A11" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="37"/>
-      <c r="C11" s="38"/>
-      <c r="D11" s="38"/>
-      <c r="E11" s="38"/>
+      <c r="B11" s="39"/>
+      <c r="C11" s="40"/>
+      <c r="D11" s="40"/>
+      <c r="E11" s="40"/>
     </row>
     <row r="12" ht="14" customHeight="1" spans="1:5">
-      <c r="A12" s="40" t="s">
+      <c r="A12" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="B12" s="37"/>
-      <c r="C12" s="38"/>
-      <c r="D12" s="38"/>
-      <c r="E12" s="38"/>
+      <c r="B12" s="39"/>
+      <c r="C12" s="40"/>
+      <c r="D12" s="40"/>
+      <c r="E12" s="40"/>
     </row>
     <row r="13" ht="14" customHeight="1" spans="1:5">
-      <c r="A13" s="40" t="s">
+      <c r="A13" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="B13" s="37"/>
-      <c r="C13" s="38"/>
-      <c r="D13" s="38"/>
-      <c r="E13" s="38"/>
+      <c r="B13" s="39"/>
+      <c r="C13" s="40"/>
+      <c r="D13" s="40"/>
+      <c r="E13" s="40"/>
     </row>
     <row r="14" ht="14" customHeight="1" spans="1:5">
-      <c r="A14" s="40" t="s">
+      <c r="A14" s="42" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="37"/>
-      <c r="C14" s="38"/>
-      <c r="D14" s="38"/>
-      <c r="E14" s="38"/>
+      <c r="B14" s="39"/>
+      <c r="C14" s="40"/>
+      <c r="D14" s="40"/>
+      <c r="E14" s="40"/>
     </row>
     <row r="15" ht="14" customHeight="1" spans="1:5">
-      <c r="A15" s="40" t="s">
+      <c r="A15" s="42" t="s">
         <v>10</v>
       </c>
-      <c r="B15" s="37"/>
-      <c r="C15" s="38"/>
-      <c r="D15" s="38"/>
-      <c r="E15" s="38"/>
+      <c r="B15" s="39"/>
+      <c r="C15" s="40"/>
+      <c r="D15" s="40"/>
+      <c r="E15" s="40"/>
     </row>
     <row r="16" ht="14" customHeight="1" spans="1:5">
-      <c r="A16" s="40" t="s">
+      <c r="A16" s="42" t="s">
         <v>11</v>
       </c>
-      <c r="B16" s="37"/>
-      <c r="C16" s="38"/>
-      <c r="D16" s="38"/>
-      <c r="E16" s="38"/>
+      <c r="B16" s="39"/>
+      <c r="C16" s="40"/>
+      <c r="D16" s="40"/>
+      <c r="E16" s="40"/>
     </row>
     <row r="17" ht="14" customHeight="1" spans="1:5">
-      <c r="A17" s="40" t="s">
+      <c r="A17" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="B17" s="37"/>
-      <c r="C17" s="38"/>
-      <c r="D17" s="38"/>
-      <c r="E17" s="38"/>
+      <c r="B17" s="39"/>
+      <c r="C17" s="40"/>
+      <c r="D17" s="40"/>
+      <c r="E17" s="40"/>
     </row>
     <row r="18" ht="14" customHeight="1" spans="1:5">
-      <c r="A18" s="40" t="s">
+      <c r="A18" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="B18" s="37"/>
-      <c r="C18" s="38"/>
-      <c r="D18" s="38"/>
-      <c r="E18" s="38"/>
+      <c r="B18" s="39"/>
+      <c r="C18" s="40"/>
+      <c r="D18" s="40"/>
+      <c r="E18" s="40"/>
     </row>
     <row r="19" ht="14" customHeight="1" spans="1:5">
-      <c r="A19" s="40" t="s">
+      <c r="A19" s="42" t="s">
         <v>14</v>
       </c>
-      <c r="B19" s="37"/>
-      <c r="C19" s="38"/>
-      <c r="D19" s="38"/>
-      <c r="E19" s="38"/>
+      <c r="B19" s="39"/>
+      <c r="C19" s="40"/>
+      <c r="D19" s="40"/>
+      <c r="E19" s="40"/>
     </row>
     <row r="20" ht="14" customHeight="1" spans="1:5">
-      <c r="A20" s="40" t="s">
+      <c r="A20" s="42" t="s">
         <v>15</v>
       </c>
-      <c r="B20" s="37"/>
-      <c r="C20" s="38"/>
-      <c r="D20" s="38"/>
-      <c r="E20" s="38"/>
+      <c r="B20" s="39"/>
+      <c r="C20" s="40"/>
+      <c r="D20" s="40"/>
+      <c r="E20" s="40"/>
     </row>
     <row r="21" ht="14" customHeight="1" spans="1:5">
-      <c r="A21" s="40" t="s">
+      <c r="A21" s="42" t="s">
         <v>16</v>
       </c>
-      <c r="B21" s="37"/>
-      <c r="C21" s="38"/>
-      <c r="D21" s="38"/>
-      <c r="E21" s="38"/>
+      <c r="B21" s="39"/>
+      <c r="C21" s="40"/>
+      <c r="D21" s="40"/>
+      <c r="E21" s="40"/>
     </row>
     <row r="22" ht="14" customHeight="1" spans="1:5">
-      <c r="A22" s="40" t="s">
+      <c r="A22" s="42" t="s">
         <v>17</v>
       </c>
-      <c r="B22" s="37"/>
-      <c r="C22" s="38"/>
-      <c r="D22" s="38"/>
-      <c r="E22" s="38"/>
+      <c r="B22" s="39"/>
+      <c r="C22" s="40"/>
+      <c r="D22" s="40"/>
+      <c r="E22" s="40"/>
     </row>
     <row r="23" ht="14" customHeight="1" spans="1:5">
-      <c r="A23" s="39" t="s">
+      <c r="A23" s="41" t="s">
         <v>18</v>
       </c>
-      <c r="B23" s="37"/>
-      <c r="C23" s="38"/>
-      <c r="D23" s="38"/>
-      <c r="E23" s="38"/>
+      <c r="B23" s="39"/>
+      <c r="C23" s="40"/>
+      <c r="D23" s="40"/>
+      <c r="E23" s="40"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2738,7 +2781,7 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="1" orientation="portrait" useFirstPageNumber="1"/>
   <headerFooter>
-    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -2748,110 +2791,110 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C8" sqref="C8"/>
+      <selection pane="bottomRight" activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.3365384615385" defaultRowHeight="13" customHeight="1" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9.90384615384615" defaultRowHeight="13" customHeight="1" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="1" width="16.3557692307692" style="1" customWidth="1"/>
-    <col min="2" max="2" width="99.1153846153846" style="24" customWidth="1"/>
-    <col min="3" max="16384" width="16.3557692307692" style="1" customWidth="1"/>
+    <col min="1" max="1" width="16.3557692307692" style="9" customWidth="1"/>
+    <col min="2" max="2" width="99.1153846153846" style="26" customWidth="1"/>
+    <col min="3" max="16384" width="16.3557692307692" style="9" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.55" customHeight="1" spans="1:3">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="27" t="s">
+      <c r="C1" s="29" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="2" ht="13.55" customHeight="1" spans="1:3">
-      <c r="A2" s="28" t="s">
+      <c r="A2" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="30" t="s">
+      <c r="C2" s="32" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="3" ht="13.35" customHeight="1" spans="1:3">
-      <c r="A3" s="31" t="s">
+      <c r="A3" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="32" t="s">
+      <c r="B3" s="34" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="30" t="s">
+      <c r="C3" s="32" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="4" ht="13.35" customHeight="1" spans="1:3">
-      <c r="A4" s="33" t="s">
+      <c r="A4" s="35" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="32" t="s">
+      <c r="B4" s="34" t="s">
         <v>28</v>
       </c>
-      <c r="C4" s="30" t="s">
+      <c r="C4" s="32" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="5" ht="13.35" customHeight="1" spans="1:3">
-      <c r="A5" s="33" t="s">
+      <c r="A5" s="35" t="s">
         <v>29</v>
       </c>
-      <c r="B5" s="32" t="s">
+      <c r="B5" s="34" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="30" t="s">
+      <c r="C5" s="32" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="6" ht="13.35" customHeight="1" spans="1:3">
-      <c r="A6" s="33" t="s">
+      <c r="A6" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="B6" s="34"/>
-      <c r="C6" s="30" t="s">
+      <c r="B6" s="36"/>
+      <c r="C6" s="32" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="7" ht="13.35" customHeight="1" spans="1:3">
-      <c r="A7" s="33" t="s">
+      <c r="A7" s="35" t="s">
         <v>32</v>
       </c>
-      <c r="B7" s="34"/>
-      <c r="C7" s="30" t="s">
+      <c r="B7" s="36"/>
+      <c r="C7" s="32" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="8" ht="13.35" customHeight="1" spans="1:3">
-      <c r="A8" s="33" t="s">
+      <c r="A8" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="B8" s="34"/>
+      <c r="B8" s="36"/>
       <c r="C8" s="23" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="9" ht="13.35" customHeight="1" spans="1:3">
-      <c r="A9" s="33" t="s">
+      <c r="A9" s="35" t="s">
         <v>35</v>
       </c>
-      <c r="B9" s="32" t="s">
+      <c r="B9" s="34" t="s">
         <v>36</v>
       </c>
       <c r="C9" s="23" t="s">
@@ -2859,65 +2902,65 @@
       </c>
     </row>
     <row r="10" ht="13.35" customHeight="1" spans="1:3">
-      <c r="A10" s="33" t="s">
+      <c r="A10" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="B10" s="32" t="s">
+      <c r="B10" s="34" t="s">
         <v>38</v>
       </c>
-      <c r="C10" s="30" t="s">
+      <c r="C10" s="32" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="11" ht="13.35" customHeight="1" spans="1:3">
-      <c r="A11" s="31" t="s">
+      <c r="A11" s="33" t="s">
         <v>39</v>
       </c>
-      <c r="B11" s="32" t="s">
+      <c r="B11" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="C11" s="35" t="s">
+      <c r="C11" s="37" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="12" ht="13.35" customHeight="1" spans="1:3">
-      <c r="A12" s="33" t="s">
+      <c r="A12" s="35" t="s">
         <v>42</v>
       </c>
-      <c r="B12" s="32" t="s">
+      <c r="B12" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="C12" s="30" t="s">
+      <c r="C12" s="32" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="13" ht="13.35" customHeight="1" spans="1:3">
-      <c r="A13" s="33" t="s">
+      <c r="A13" s="35" t="s">
         <v>44</v>
       </c>
-      <c r="B13" s="32" t="s">
+      <c r="B13" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="C13" s="30" t="s">
+      <c r="C13" s="32" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="14" ht="13.35" customHeight="1" spans="1:3">
-      <c r="A14" s="31" t="s">
+      <c r="A14" s="33" t="s">
         <v>46</v>
       </c>
-      <c r="B14" s="32" t="s">
+      <c r="B14" s="34" t="s">
         <v>47</v>
       </c>
-      <c r="C14" s="35" t="s">
+      <c r="C14" s="37" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="15" ht="13.35" customHeight="1" spans="1:3">
-      <c r="A15" s="31" t="s">
+      <c r="A15" s="33" t="s">
         <v>48</v>
       </c>
-      <c r="B15" s="32" t="s">
+      <c r="B15" s="34" t="s">
         <v>49</v>
       </c>
       <c r="C15" s="23" t="s">
@@ -2925,31 +2968,43 @@
       </c>
     </row>
     <row r="16" ht="13.35" customHeight="1" spans="1:3">
-      <c r="A16" s="31" t="s">
+      <c r="A16" s="33" t="s">
         <v>50</v>
       </c>
-      <c r="B16" s="32" t="s">
+      <c r="B16" s="34" t="s">
         <v>51</v>
       </c>
-      <c r="C16" s="35" t="s">
+      <c r="C16" s="37" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="17" ht="13.35" customHeight="1" spans="1:3">
-      <c r="A17" s="31" t="s">
+      <c r="A17" s="33" t="s">
         <v>52</v>
       </c>
-      <c r="B17" s="32" t="s">
+      <c r="B17" s="34" t="s">
         <v>53</v>
       </c>
-      <c r="C17" s="30" t="s">
+      <c r="C17" s="32" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="18" ht="13.35" customHeight="1" spans="1:3">
-      <c r="A18" s="36"/>
-      <c r="B18" s="34"/>
+      <c r="A18" s="38" t="s">
+        <v>54</v>
+      </c>
+      <c r="B18" s="13" t="s">
+        <v>55</v>
+      </c>
       <c r="C18" s="13"/>
+    </row>
+    <row r="19" customHeight="1" spans="1:2">
+      <c r="A19" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="B19" s="26" t="s">
+        <v>57</v>
+      </c>
     </row>
   </sheetData>
   <dataValidations count="1">
@@ -2960,7 +3015,7 @@
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
   <pageSetup paperSize="1" orientation="portrait" useFirstPageNumber="1"/>
   <headerFooter>
-    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -2972,74 +3027,74 @@
   </sheetPr>
   <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A5" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection/>
-      <selection pane="topRight" activeCell="E16" sqref="E16"/>
+      <selection pane="topRight" activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.3365384615385" defaultRowHeight="13" customHeight="1" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="9.90384615384615" defaultRowHeight="13" customHeight="1" outlineLevelCol="7"/>
   <cols>
-    <col min="1" max="16384" width="16.3557692307692" style="1" customWidth="1"/>
+    <col min="1" max="16384" width="16.3557692307692" style="9" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="14" customHeight="1" spans="1:8">
-      <c r="A1" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="B1" s="3">
-        <v>20210901</v>
-      </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
+      <c r="A1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B1" s="2">
+        <v>20220401</v>
+      </c>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
       <c r="G1" s="19"/>
       <c r="H1" s="20"/>
     </row>
     <row r="2" ht="14" customHeight="1" spans="1:8">
-      <c r="A2" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="B2" s="6">
-        <v>20210930</v>
-      </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
+      <c r="A2" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2" s="5">
+        <v>20220430</v>
+      </c>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
       <c r="G2" s="21"/>
       <c r="H2" s="22"/>
     </row>
     <row r="3" ht="14" customHeight="1" spans="1:8">
-      <c r="A3" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="B3" s="8" t="s">
+      <c r="A3" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B3" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="F3" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="H3" s="8" t="s">
-        <v>58</v>
+      <c r="G3" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="4" ht="13.65" customHeight="1" spans="1:8">
-      <c r="A4" s="9" t="s">
-        <v>59</v>
+      <c r="A4" s="8" t="s">
+        <v>63</v>
       </c>
       <c r="C4" s="10"/>
       <c r="D4" s="10"/>
@@ -3054,7 +3109,7 @@
       <c r="C5" s="13"/>
       <c r="D5" s="13"/>
       <c r="E5" s="13" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="F5" s="13"/>
       <c r="G5" s="23" t="s">
@@ -3068,7 +3123,7 @@
       <c r="C6" s="13"/>
       <c r="D6" s="13"/>
       <c r="E6" s="13" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="F6" s="13"/>
       <c r="G6" s="23" t="s">
@@ -3079,7 +3134,7 @@
     <row r="7" ht="13.35" customHeight="1" spans="1:8">
       <c r="A7" s="11"/>
       <c r="B7" s="14" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="C7" s="13"/>
       <c r="D7" s="13"/>
@@ -3101,8 +3156,8 @@
       <c r="H8" s="13"/>
     </row>
     <row r="9" ht="13.65" customHeight="1" spans="1:8">
-      <c r="A9" s="9" t="s">
-        <v>63</v>
+      <c r="A9" s="8" t="s">
+        <v>67</v>
       </c>
       <c r="B9" s="12"/>
       <c r="C9" s="13"/>
@@ -3133,30 +3188,36 @@
       <c r="H11" s="13"/>
     </row>
     <row r="12" ht="13.65" customHeight="1" spans="1:8">
-      <c r="A12" s="9" t="s">
-        <v>64</v>
+      <c r="A12" s="8" t="s">
+        <v>68</v>
       </c>
       <c r="B12" s="16" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="C12" s="13"/>
       <c r="D12" s="13"/>
       <c r="E12" s="13"/>
       <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
+      <c r="G12" s="24" t="s">
+        <v>24</v>
+      </c>
       <c r="H12" s="13"/>
     </row>
     <row r="13" ht="13.65" customHeight="1" spans="1:8">
       <c r="A13" s="11"/>
       <c r="B13" s="14"/>
       <c r="C13" s="13" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="D13" s="13"/>
       <c r="E13" s="13"/>
       <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
-      <c r="H13" s="13"/>
+      <c r="G13" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="H13" s="13" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="14" ht="14" customHeight="1" spans="1:8">
       <c r="A14" s="15"/>
@@ -3169,8 +3230,8 @@
       <c r="H14" s="13"/>
     </row>
     <row r="15" ht="13.65" customHeight="1" spans="1:8">
-      <c r="A15" s="9" t="s">
-        <v>67</v>
+      <c r="A15" s="8" t="s">
+        <v>72</v>
       </c>
       <c r="B15" s="12"/>
       <c r="C15" s="13"/>
@@ -3218,14 +3279,261 @@
     <mergeCell ref="A15:A17"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G5 G6 G7">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G5 G6 G7 G12 G13">
       <formula1>"未进行,进行中,已暂停,已完成"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
   <pageSetup paperSize="1" orientation="portrait" useFirstPageNumber="1"/>
   <headerFooter>
-    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:H18"/>
+  <sheetViews>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.90384615384615" defaultRowHeight="16.8" outlineLevelCol="7"/>
+  <cols>
+    <col min="1" max="1" width="11.7307692307692" customWidth="1"/>
+    <col min="2" max="2" width="17.9711538461538" customWidth="1"/>
+    <col min="3" max="3" width="12.0288461538462" customWidth="1"/>
+    <col min="4" max="4" width="15" customWidth="1"/>
+    <col min="8" max="8" width="15.4903846153846" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B1" s="2">
+        <v>20220501</v>
+      </c>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="20"/>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2" s="5">
+        <v>20220531</v>
+      </c>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="22"/>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="H4" s="10"/>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="11"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
+      <c r="H5" s="13"/>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="11"/>
+      <c r="B6" s="14"/>
+      <c r="C6" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
+      <c r="H6" s="13"/>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="11"/>
+      <c r="B7" s="14"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+      <c r="H7" s="13"/>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="15"/>
+      <c r="B8" s="14"/>
+      <c r="C8" s="13"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+      <c r="H8" s="13"/>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="B9" s="12"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="H9" s="13"/>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="11"/>
+      <c r="B10" s="14"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="H10" s="13"/>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="15"/>
+      <c r="B11" s="14"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+      <c r="H11" s="13"/>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="B12" s="16"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+      <c r="H12" s="13"/>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="11"/>
+      <c r="B13" s="14"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="H13" s="13"/>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="15"/>
+      <c r="B14" s="14"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="13"/>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="B15" s="12"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
+      <c r="H15" s="13"/>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" s="11"/>
+      <c r="B16" s="12"/>
+      <c r="C16" s="13"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="13"/>
+      <c r="H16" s="13"/>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" s="15"/>
+      <c r="B17" s="14"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
+      <c r="H17" s="13"/>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" s="17"/>
+      <c r="B18" s="18"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="13"/>
+      <c r="H18" s="13"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A4:A8"/>
+    <mergeCell ref="A9:A11"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="A15:A17"/>
+  </mergeCells>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G4 G5 G6 G7 G12 G13">
+      <formula1>"未进行,进行中,已暂停,已完成"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Site updated: 2022-05-19 00:12:57
</commit_message>
<xml_diff>
--- a/file/personal/roleImportant/角色要事记录表_2022.xlsx
+++ b/file/personal/roleImportant/角色要事记录表_2022.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27500" windowHeight="11860" activeTab="1"/>
+    <workbookView windowWidth="27500" windowHeight="11860" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="角色目录" sheetId="2" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87">
   <si>
     <t>角色</t>
   </si>
@@ -91,21 +91,24 @@
     <t>身体锻炼/眼袋/皮肤/睡眠/作息等等</t>
   </si>
   <si>
+    <t>已完成</t>
+  </si>
+  <si>
+    <t>家庭</t>
+  </si>
+  <si>
+    <t>梳理出家庭需要处理的事情/问题，将事情分分工，借助项目管理的思路来管理</t>
+  </si>
+  <si>
+    <t>工作思考总结</t>
+  </si>
+  <si>
+    <t>思考/总结现有工作节奏、理想的工作节奏、能够达到的工作节奏，让工作不在成为自身成长和家庭的障碍，要成为助推器</t>
+  </si>
+  <si>
     <t>未进行</t>
   </si>
   <si>
-    <t>家庭</t>
-  </si>
-  <si>
-    <t>梳理出家庭需要处理的事情/问题，将事情分分工，借助项目管理的思路来管理</t>
-  </si>
-  <si>
-    <t>工作思考总结</t>
-  </si>
-  <si>
-    <t>思考/总结现有工作节奏、理想的工作节奏、能够达到的工作节奏，让工作不在成为自身成长和家庭的障碍，要成为助推器</t>
-  </si>
-  <si>
     <t>调研理财途径</t>
   </si>
   <si>
@@ -121,9 +124,6 @@
     <t>总结/了解保险</t>
   </si>
   <si>
-    <t>已完成</t>
-  </si>
-  <si>
     <t>筛选购买保险</t>
   </si>
   <si>
@@ -193,6 +193,27 @@
     <t>比如做投资人/up主，最好是自己感兴趣的。感兴趣的不一定能做好，但是不感兴趣的一定做不好</t>
   </si>
   <si>
+    <t>面部保养</t>
+  </si>
+  <si>
+    <t>消除脸上的斑</t>
+  </si>
+  <si>
+    <t>男性如何做好面部保养？</t>
+  </si>
+  <si>
+    <t>上海落户</t>
+  </si>
+  <si>
+    <t>如何完成上海落户？</t>
+  </si>
+  <si>
+    <t>房贷相关</t>
+  </si>
+  <si>
+    <t>如何转贷？提前还款利率是否变化？</t>
+  </si>
+  <si>
     <t>开始时间:</t>
   </si>
   <si>
@@ -245,6 +266,18 @@
   </si>
   <si>
     <t>养生计划梳理</t>
+  </si>
+  <si>
+    <t>业务互联业务梳理</t>
+  </si>
+  <si>
+    <t>业务互联技术梳理</t>
+  </si>
+  <si>
+    <t>业务互联管理梳理</t>
+  </si>
+  <si>
+    <t>Spring+java笔记整理温习</t>
   </si>
 </sst>
 </file>
@@ -253,9 +286,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -279,11 +312,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color theme="0"/>
       <name val="Helvetica Neue"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -296,7 +328,92 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="1"/>
+      <name val="Helvetica Neue"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Helvetica Neue"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Helvetica Neue"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -311,60 +428,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Helvetica Neue"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Helvetica Neue"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF9C6500"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
@@ -372,7 +435,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF3F3F76"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -385,38 +448,8 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="43">
+  <fills count="44">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -444,6 +477,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -498,19 +537,109 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -522,85 +651,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -624,49 +705,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -995,7 +1034,22 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1004,7 +1058,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1039,6 +1093,17 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -1053,183 +1118,157 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="42" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="38" borderId="26" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="42" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="43" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="38" borderId="27" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="27" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="26" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="30" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="21" borderId="28" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="18" borderId="27" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="25" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="29" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="23" borderId="30" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="28" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="24" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="25" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="34" borderId="29" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="41" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="26" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="23" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1302,34 +1341,34 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="8" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="8" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="9" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="9" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="9" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="10" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="9" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="10" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1338,10 +1377,13 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1483,11 +1525,6 @@
       <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -2556,11 +2593,12 @@
       </a:style>
     </a:txDef>
   </a:objectDefaults>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
   <dimension ref="A1:E23"/>
   <sheetViews>
@@ -2568,7 +2606,7 @@
       <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.90384615384615" defaultRowHeight="13.5" customHeight="1" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9.90825688073394" defaultRowHeight="13.5" customHeight="1" outlineLevelCol="4"/>
   <cols>
     <col min="1" max="1" width="9" style="9" customWidth="1"/>
     <col min="2" max="16384" width="6" style="9" customWidth="1"/>
@@ -2578,200 +2616,200 @@
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="39"/>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40"/>
+      <c r="B1" s="40"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
     </row>
     <row r="2" ht="14" customHeight="1" spans="1:5">
-      <c r="A2" s="41" t="s">
+      <c r="A2" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="39"/>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
+      <c r="B2" s="40"/>
+      <c r="C2" s="41"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="41"/>
     </row>
     <row r="3" ht="14" customHeight="1" spans="1:5">
-      <c r="A3" s="41" t="s">
+      <c r="A3" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="39"/>
-      <c r="C3" s="40"/>
-      <c r="D3" s="40"/>
-      <c r="E3" s="40"/>
+      <c r="B3" s="40"/>
+      <c r="C3" s="41"/>
+      <c r="D3" s="41"/>
+      <c r="E3" s="41"/>
     </row>
     <row r="4" ht="14" customHeight="1" spans="1:5">
-      <c r="A4" s="42" t="s">
+      <c r="A4" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="39"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="40"/>
+      <c r="B4" s="40"/>
+      <c r="C4" s="41"/>
+      <c r="D4" s="41"/>
+      <c r="E4" s="41"/>
     </row>
     <row r="5" ht="14" customHeight="1" spans="1:5">
-      <c r="A5" s="43"/>
-      <c r="B5" s="39"/>
-      <c r="C5" s="40"/>
-      <c r="D5" s="40"/>
-      <c r="E5" s="40"/>
+      <c r="A5" s="44"/>
+      <c r="B5" s="40"/>
+      <c r="C5" s="41"/>
+      <c r="D5" s="41"/>
+      <c r="E5" s="41"/>
     </row>
     <row r="6" ht="14" customHeight="1" spans="1:5">
-      <c r="A6" s="43"/>
-      <c r="B6" s="39"/>
-      <c r="C6" s="40"/>
-      <c r="D6" s="40"/>
-      <c r="E6" s="40"/>
+      <c r="A6" s="44"/>
+      <c r="B6" s="40"/>
+      <c r="C6" s="41"/>
+      <c r="D6" s="41"/>
+      <c r="E6" s="41"/>
     </row>
     <row r="7" ht="14" customHeight="1" spans="1:5">
-      <c r="A7" s="42" t="s">
+      <c r="A7" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="39"/>
-      <c r="C7" s="40"/>
-      <c r="D7" s="40"/>
-      <c r="E7" s="40"/>
+      <c r="B7" s="40"/>
+      <c r="C7" s="41"/>
+      <c r="D7" s="41"/>
+      <c r="E7" s="41"/>
     </row>
     <row r="8" ht="14" customHeight="1" spans="1:5">
-      <c r="A8" s="43"/>
-      <c r="B8" s="39"/>
-      <c r="C8" s="40"/>
-      <c r="D8" s="40"/>
-      <c r="E8" s="40"/>
+      <c r="A8" s="44"/>
+      <c r="B8" s="40"/>
+      <c r="C8" s="41"/>
+      <c r="D8" s="41"/>
+      <c r="E8" s="41"/>
     </row>
     <row r="9" ht="14" customHeight="1" spans="1:5">
-      <c r="A9" s="43"/>
-      <c r="B9" s="39"/>
-      <c r="C9" s="40"/>
-      <c r="D9" s="40"/>
-      <c r="E9" s="40"/>
+      <c r="A9" s="44"/>
+      <c r="B9" s="40"/>
+      <c r="C9" s="41"/>
+      <c r="D9" s="41"/>
+      <c r="E9" s="41"/>
     </row>
     <row r="10" ht="14" customHeight="1" spans="1:5">
-      <c r="A10" s="42" t="s">
+      <c r="A10" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="39"/>
-      <c r="C10" s="40"/>
-      <c r="D10" s="40"/>
-      <c r="E10" s="40"/>
+      <c r="B10" s="40"/>
+      <c r="C10" s="41"/>
+      <c r="D10" s="41"/>
+      <c r="E10" s="41"/>
     </row>
     <row r="11" ht="14" customHeight="1" spans="1:5">
-      <c r="A11" s="42" t="s">
+      <c r="A11" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="39"/>
-      <c r="C11" s="40"/>
-      <c r="D11" s="40"/>
-      <c r="E11" s="40"/>
+      <c r="B11" s="40"/>
+      <c r="C11" s="41"/>
+      <c r="D11" s="41"/>
+      <c r="E11" s="41"/>
     </row>
     <row r="12" ht="14" customHeight="1" spans="1:5">
-      <c r="A12" s="42" t="s">
+      <c r="A12" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="B12" s="39"/>
-      <c r="C12" s="40"/>
-      <c r="D12" s="40"/>
-      <c r="E12" s="40"/>
+      <c r="B12" s="40"/>
+      <c r="C12" s="41"/>
+      <c r="D12" s="41"/>
+      <c r="E12" s="41"/>
     </row>
     <row r="13" ht="14" customHeight="1" spans="1:5">
-      <c r="A13" s="42" t="s">
+      <c r="A13" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="B13" s="39"/>
-      <c r="C13" s="40"/>
-      <c r="D13" s="40"/>
-      <c r="E13" s="40"/>
+      <c r="B13" s="40"/>
+      <c r="C13" s="41"/>
+      <c r="D13" s="41"/>
+      <c r="E13" s="41"/>
     </row>
     <row r="14" ht="14" customHeight="1" spans="1:5">
-      <c r="A14" s="42" t="s">
+      <c r="A14" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="39"/>
-      <c r="C14" s="40"/>
-      <c r="D14" s="40"/>
-      <c r="E14" s="40"/>
+      <c r="B14" s="40"/>
+      <c r="C14" s="41"/>
+      <c r="D14" s="41"/>
+      <c r="E14" s="41"/>
     </row>
     <row r="15" ht="14" customHeight="1" spans="1:5">
-      <c r="A15" s="42" t="s">
+      <c r="A15" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="B15" s="39"/>
-      <c r="C15" s="40"/>
-      <c r="D15" s="40"/>
-      <c r="E15" s="40"/>
+      <c r="B15" s="40"/>
+      <c r="C15" s="41"/>
+      <c r="D15" s="41"/>
+      <c r="E15" s="41"/>
     </row>
     <row r="16" ht="14" customHeight="1" spans="1:5">
-      <c r="A16" s="42" t="s">
+      <c r="A16" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="B16" s="39"/>
-      <c r="C16" s="40"/>
-      <c r="D16" s="40"/>
-      <c r="E16" s="40"/>
+      <c r="B16" s="40"/>
+      <c r="C16" s="41"/>
+      <c r="D16" s="41"/>
+      <c r="E16" s="41"/>
     </row>
     <row r="17" ht="14" customHeight="1" spans="1:5">
-      <c r="A17" s="42" t="s">
+      <c r="A17" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="B17" s="39"/>
-      <c r="C17" s="40"/>
-      <c r="D17" s="40"/>
-      <c r="E17" s="40"/>
+      <c r="B17" s="40"/>
+      <c r="C17" s="41"/>
+      <c r="D17" s="41"/>
+      <c r="E17" s="41"/>
     </row>
     <row r="18" ht="14" customHeight="1" spans="1:5">
-      <c r="A18" s="42" t="s">
+      <c r="A18" s="43" t="s">
         <v>13</v>
       </c>
-      <c r="B18" s="39"/>
-      <c r="C18" s="40"/>
-      <c r="D18" s="40"/>
-      <c r="E18" s="40"/>
+      <c r="B18" s="40"/>
+      <c r="C18" s="41"/>
+      <c r="D18" s="41"/>
+      <c r="E18" s="41"/>
     </row>
     <row r="19" ht="14" customHeight="1" spans="1:5">
-      <c r="A19" s="42" t="s">
+      <c r="A19" s="43" t="s">
         <v>14</v>
       </c>
-      <c r="B19" s="39"/>
-      <c r="C19" s="40"/>
-      <c r="D19" s="40"/>
-      <c r="E19" s="40"/>
+      <c r="B19" s="40"/>
+      <c r="C19" s="41"/>
+      <c r="D19" s="41"/>
+      <c r="E19" s="41"/>
     </row>
     <row r="20" ht="14" customHeight="1" spans="1:5">
-      <c r="A20" s="42" t="s">
+      <c r="A20" s="43" t="s">
         <v>15</v>
       </c>
-      <c r="B20" s="39"/>
-      <c r="C20" s="40"/>
-      <c r="D20" s="40"/>
-      <c r="E20" s="40"/>
+      <c r="B20" s="40"/>
+      <c r="C20" s="41"/>
+      <c r="D20" s="41"/>
+      <c r="E20" s="41"/>
     </row>
     <row r="21" ht="14" customHeight="1" spans="1:5">
-      <c r="A21" s="42" t="s">
+      <c r="A21" s="43" t="s">
         <v>16</v>
       </c>
-      <c r="B21" s="39"/>
-      <c r="C21" s="40"/>
-      <c r="D21" s="40"/>
-      <c r="E21" s="40"/>
+      <c r="B21" s="40"/>
+      <c r="C21" s="41"/>
+      <c r="D21" s="41"/>
+      <c r="E21" s="41"/>
     </row>
     <row r="22" ht="14" customHeight="1" spans="1:5">
-      <c r="A22" s="42" t="s">
+      <c r="A22" s="43" t="s">
         <v>17</v>
       </c>
-      <c r="B22" s="39"/>
-      <c r="C22" s="40"/>
-      <c r="D22" s="40"/>
-      <c r="E22" s="40"/>
+      <c r="B22" s="40"/>
+      <c r="C22" s="41"/>
+      <c r="D22" s="41"/>
+      <c r="E22" s="41"/>
     </row>
     <row r="23" ht="14" customHeight="1" spans="1:5">
-      <c r="A23" s="41" t="s">
+      <c r="A23" s="42" t="s">
         <v>18</v>
       </c>
-      <c r="B23" s="39"/>
-      <c r="C23" s="40"/>
-      <c r="D23" s="40"/>
-      <c r="E23" s="40"/>
+      <c r="B23" s="40"/>
+      <c r="C23" s="41"/>
+      <c r="D23" s="41"/>
+      <c r="E23" s="41"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2787,46 +2825,46 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B9" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="B22" sqref="B22"/>
+      <selection pane="bottomRight" activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.90384615384615" defaultRowHeight="13" customHeight="1" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9.90825688073394" defaultRowHeight="13" customHeight="1" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="1" width="16.3557692307692" style="9" customWidth="1"/>
-    <col min="2" max="2" width="99.1153846153846" style="26" customWidth="1"/>
-    <col min="3" max="16384" width="16.3557692307692" style="9" customWidth="1"/>
+    <col min="1" max="1" width="16.3577981651376" style="9" customWidth="1"/>
+    <col min="2" max="2" width="99.1192660550459" style="27" customWidth="1"/>
+    <col min="3" max="16384" width="16.3577981651376" style="9" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.55" customHeight="1" spans="1:3">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="29" t="s">
+      <c r="C1" s="30" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="2" ht="13.55" customHeight="1" spans="1:3">
-      <c r="A2" s="30" t="s">
+      <c r="A2" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="31" t="s">
+      <c r="B2" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="32" t="s">
+      <c r="C2" s="23" t="s">
         <v>24</v>
       </c>
     </row>
@@ -2837,7 +2875,7 @@
       <c r="B3" s="34" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="32" t="s">
+      <c r="C3" s="23" t="s">
         <v>24</v>
       </c>
     </row>
@@ -2848,46 +2886,46 @@
       <c r="B4" s="34" t="s">
         <v>28</v>
       </c>
-      <c r="C4" s="32" t="s">
-        <v>24</v>
+      <c r="C4" s="36" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="5" ht="13.35" customHeight="1" spans="1:3">
       <c r="A5" s="35" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" s="34" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" s="36" t="s">
         <v>29</v>
-      </c>
-      <c r="B5" s="34" t="s">
-        <v>30</v>
-      </c>
-      <c r="C5" s="32" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="6" ht="13.35" customHeight="1" spans="1:3">
       <c r="A6" s="35" t="s">
-        <v>31</v>
-      </c>
-      <c r="B6" s="36"/>
-      <c r="C6" s="32" t="s">
-        <v>24</v>
+        <v>32</v>
+      </c>
+      <c r="B6" s="37"/>
+      <c r="C6" s="36" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="7" ht="13.35" customHeight="1" spans="1:3">
       <c r="A7" s="35" t="s">
-        <v>32</v>
-      </c>
-      <c r="B7" s="36"/>
-      <c r="C7" s="32" t="s">
-        <v>24</v>
+        <v>33</v>
+      </c>
+      <c r="B7" s="37"/>
+      <c r="C7" s="36" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="8" ht="13.35" customHeight="1" spans="1:3">
       <c r="A8" s="35" t="s">
-        <v>33</v>
-      </c>
-      <c r="B8" s="36"/>
+        <v>34</v>
+      </c>
+      <c r="B8" s="37"/>
       <c r="C8" s="23" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" ht="13.35" customHeight="1" spans="1:3">
@@ -2898,7 +2936,7 @@
         <v>36</v>
       </c>
       <c r="C9" s="23" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" ht="13.35" customHeight="1" spans="1:3">
@@ -2908,8 +2946,8 @@
       <c r="B10" s="34" t="s">
         <v>38</v>
       </c>
-      <c r="C10" s="32" t="s">
-        <v>24</v>
+      <c r="C10" s="36" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="11" ht="13.35" customHeight="1" spans="1:3">
@@ -2919,7 +2957,7 @@
       <c r="B11" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="C11" s="37" t="s">
+      <c r="C11" s="38" t="s">
         <v>41</v>
       </c>
     </row>
@@ -2930,8 +2968,8 @@
       <c r="B12" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="C12" s="32" t="s">
-        <v>24</v>
+      <c r="C12" s="36" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="13" ht="13.35" customHeight="1" spans="1:3">
@@ -2941,8 +2979,8 @@
       <c r="B13" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="C13" s="32" t="s">
-        <v>24</v>
+      <c r="C13" s="36" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="14" ht="13.35" customHeight="1" spans="1:3">
@@ -2952,7 +2990,7 @@
       <c r="B14" s="34" t="s">
         <v>47</v>
       </c>
-      <c r="C14" s="37" t="s">
+      <c r="C14" s="38" t="s">
         <v>41</v>
       </c>
     </row>
@@ -2964,7 +3002,7 @@
         <v>49</v>
       </c>
       <c r="C15" s="23" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
     </row>
     <row r="16" ht="13.35" customHeight="1" spans="1:3">
@@ -2974,7 +3012,7 @@
       <c r="B16" s="34" t="s">
         <v>51</v>
       </c>
-      <c r="C16" s="37" t="s">
+      <c r="C16" s="38" t="s">
         <v>41</v>
       </c>
     </row>
@@ -2985,12 +3023,12 @@
       <c r="B17" s="34" t="s">
         <v>53</v>
       </c>
-      <c r="C17" s="32" t="s">
-        <v>24</v>
+      <c r="C17" s="36" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="18" ht="13.35" customHeight="1" spans="1:3">
-      <c r="A18" s="38" t="s">
+      <c r="A18" s="39" t="s">
         <v>54</v>
       </c>
       <c r="B18" s="13" t="s">
@@ -3002,8 +3040,40 @@
       <c r="A19" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="B19" s="26" t="s">
+      <c r="B19" s="27" t="s">
         <v>57</v>
+      </c>
+    </row>
+    <row r="20" customHeight="1" spans="1:2">
+      <c r="A20" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="B20" s="27" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="21" customHeight="1" spans="1:2">
+      <c r="A21" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="B21" s="27" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="22" customHeight="1" spans="1:2">
+      <c r="A22" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="B22" s="27" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="23" customHeight="1" spans="1:2">
+      <c r="A23" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="B23" s="27" t="s">
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -3021,26 +3091,26 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A5" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection/>
       <selection pane="topRight" activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.90384615384615" defaultRowHeight="13" customHeight="1" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="9.90825688073394" defaultRowHeight="13" customHeight="1" outlineLevelCol="7"/>
   <cols>
-    <col min="1" max="16384" width="16.3557692307692" style="9" customWidth="1"/>
+    <col min="1" max="16384" width="16.3577981651376" style="9" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="14" customHeight="1" spans="1:8">
       <c r="A1" s="1" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="B1" s="2">
         <v>20220401</v>
@@ -3054,7 +3124,7 @@
     </row>
     <row r="2" ht="14" customHeight="1" spans="1:8">
       <c r="A2" s="4" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="B2" s="5">
         <v>20220430</v>
@@ -3068,7 +3138,7 @@
     </row>
     <row r="3" ht="14" customHeight="1" spans="1:8">
       <c r="A3" s="7" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>1</v>
@@ -3086,15 +3156,15 @@
         <v>14</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" ht="13.65" customHeight="1" spans="1:8">
       <c r="A4" s="8" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="C4" s="10"/>
       <c r="D4" s="10"/>
@@ -3109,11 +3179,11 @@
       <c r="C5" s="13"/>
       <c r="D5" s="13"/>
       <c r="E5" s="13" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="F5" s="13"/>
       <c r="G5" s="23" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="H5" s="13"/>
     </row>
@@ -3123,25 +3193,25 @@
       <c r="C6" s="13"/>
       <c r="D6" s="13"/>
       <c r="E6" s="13" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="F6" s="13"/>
       <c r="G6" s="23" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="H6" s="13"/>
     </row>
     <row r="7" ht="13.35" customHeight="1" spans="1:8">
       <c r="A7" s="11"/>
       <c r="B7" s="14" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="C7" s="13"/>
       <c r="D7" s="13"/>
       <c r="E7" s="13"/>
       <c r="F7" s="13"/>
       <c r="G7" s="23" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="H7" s="13"/>
     </row>
@@ -3157,7 +3227,7 @@
     </row>
     <row r="9" ht="13.65" customHeight="1" spans="1:8">
       <c r="A9" s="8" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="B9" s="12"/>
       <c r="C9" s="13"/>
@@ -3189,17 +3259,17 @@
     </row>
     <row r="12" ht="13.65" customHeight="1" spans="1:8">
       <c r="A12" s="8" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="B12" s="16" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="C12" s="13"/>
       <c r="D12" s="13"/>
       <c r="E12" s="13"/>
       <c r="F12" s="13"/>
-      <c r="G12" s="24" t="s">
-        <v>24</v>
+      <c r="G12" s="25" t="s">
+        <v>29</v>
       </c>
       <c r="H12" s="13"/>
     </row>
@@ -3212,11 +3282,11 @@
       <c r="D13" s="13"/>
       <c r="E13" s="13"/>
       <c r="F13" s="13"/>
-      <c r="G13" s="25" t="s">
-        <v>70</v>
+      <c r="G13" s="26" t="s">
+        <v>77</v>
       </c>
       <c r="H13" s="13" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
     </row>
     <row r="14" ht="14" customHeight="1" spans="1:8">
@@ -3231,7 +3301,7 @@
     </row>
     <row r="15" ht="13.65" customHeight="1" spans="1:8">
       <c r="A15" s="8" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="B15" s="12"/>
       <c r="C15" s="13"/>
@@ -3292,26 +3362,26 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
   <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.90384615384615" defaultRowHeight="16.8" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="9.90825688073394" defaultRowHeight="13.35" outlineLevelCol="7"/>
   <cols>
-    <col min="1" max="1" width="11.7307692307692" customWidth="1"/>
-    <col min="2" max="2" width="17.9711538461538" customWidth="1"/>
-    <col min="3" max="3" width="12.0288461538462" customWidth="1"/>
+    <col min="1" max="1" width="11.7339449541284" customWidth="1"/>
+    <col min="2" max="2" width="17.9724770642202" customWidth="1"/>
+    <col min="3" max="3" width="12.0275229357798" customWidth="1"/>
     <col min="4" max="4" width="15" customWidth="1"/>
-    <col min="8" max="8" width="15.4903846153846" customWidth="1"/>
+    <col min="8" max="8" width="15.4862385321101" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="B1" s="2">
         <v>20220501</v>
@@ -3325,7 +3395,7 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="4" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="B2" s="5">
         <v>20220531</v>
@@ -3339,7 +3409,7 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="7" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>1</v>
@@ -3357,25 +3427,25 @@
         <v>14</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="8" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>73</v>
+        <v>80</v>
       </c>
       <c r="C4" s="10"/>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
       <c r="G4" s="23" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="H4" s="10"/>
     </row>
@@ -3384,30 +3454,41 @@
       <c r="B5" s="12"/>
       <c r="C5" s="13"/>
       <c r="D5" s="13" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="E5" s="13"/>
       <c r="F5" s="13"/>
+      <c r="G5" s="23" t="s">
+        <v>24</v>
+      </c>
       <c r="H5" s="13"/>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="11"/>
       <c r="B6" s="14"/>
       <c r="C6" s="13" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="D6" s="13"/>
       <c r="E6" s="13"/>
       <c r="F6" s="13"/>
+      <c r="G6" s="23" t="s">
+        <v>24</v>
+      </c>
       <c r="H6" s="13"/>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="11"/>
-      <c r="B7" s="14"/>
+      <c r="B7" s="14" t="s">
+        <v>83</v>
+      </c>
       <c r="C7" s="13"/>
       <c r="D7" s="13"/>
       <c r="E7" s="13"/>
       <c r="F7" s="13"/>
+      <c r="G7" s="23" t="s">
+        <v>24</v>
+      </c>
       <c r="H7" s="13"/>
     </row>
     <row r="8" spans="1:8">
@@ -3421,22 +3502,32 @@
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="B9" s="12"/>
+        <v>74</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>84</v>
+      </c>
       <c r="C9" s="13"/>
       <c r="D9" s="13"/>
       <c r="E9" s="13"/>
       <c r="F9" s="13"/>
+      <c r="G9" s="24" t="s">
+        <v>24</v>
+      </c>
       <c r="H9" s="13"/>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="11"/>
-      <c r="B10" s="14"/>
+      <c r="B10" s="14" t="s">
+        <v>85</v>
+      </c>
       <c r="C10" s="13"/>
       <c r="D10" s="13"/>
       <c r="E10" s="13"/>
       <c r="F10" s="13"/>
+      <c r="G10" s="24" t="s">
+        <v>24</v>
+      </c>
       <c r="H10" s="13"/>
     </row>
     <row r="11" spans="1:8">
@@ -3450,9 +3541,11 @@
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="B12" s="16"/>
+        <v>75</v>
+      </c>
+      <c r="B12" s="16" t="s">
+        <v>86</v>
+      </c>
       <c r="C12" s="13"/>
       <c r="D12" s="13"/>
       <c r="E12" s="13"/>
@@ -3480,9 +3573,11 @@
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="B15" s="12"/>
+        <v>79</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>86</v>
+      </c>
       <c r="C15" s="13"/>
       <c r="D15" s="13"/>
       <c r="E15" s="13"/>

</xml_diff>

<commit_message>
Site updated: 2022-06-06 23:54:05
</commit_message>
<xml_diff>
--- a/file/personal/roleImportant/角色要事记录表_2022.xlsx
+++ b/file/personal/roleImportant/角色要事记录表_2022.xlsx
@@ -4,20 +4,21 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27500" windowHeight="11860" activeTab="3"/>
+    <workbookView windowWidth="27500" windowHeight="11860" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="角色目录" sheetId="2" r:id="rId1"/>
     <sheet name="待办任务" sheetId="3" r:id="rId2"/>
     <sheet name="四月" sheetId="10" r:id="rId3"/>
     <sheet name="五月" sheetId="11" r:id="rId4"/>
+    <sheet name="六月" sheetId="12" r:id="rId5"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="89">
   <si>
     <t>角色</t>
   </si>
@@ -277,7 +278,13 @@
     <t>业务互联管理梳理</t>
   </si>
   <si>
-    <t>Spring+java笔记整理温习</t>
+    <t>java笔记查漏补缺</t>
+  </si>
+  <si>
+    <t>未完成</t>
+  </si>
+  <si>
+    <t>印象笔记技术文档整理</t>
   </si>
 </sst>
 </file>
@@ -285,9 +292,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
@@ -299,16 +306,17 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
       <name val="Helvetica Neue"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -320,7 +328,7 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Helvetica Neue"/>
       <charset val="134"/>
@@ -334,9 +342,85 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF800080"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Helvetica Neue"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Helvetica Neue"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -351,21 +435,12 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Helvetica Neue"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Helvetica Neue"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Helvetica Neue"/>
@@ -373,81 +448,13 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF0000FF"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Helvetica Neue"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="44">
     <fill>
@@ -488,13 +495,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -531,187 +538,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -783,21 +790,6 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="17"/>
-      </left>
-      <right style="thin">
-        <color indexed="17"/>
-      </right>
-      <top style="thin">
-        <color indexed="13"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="17"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color indexed="13"/>
       </left>
       <right style="thin">
@@ -812,56 +804,11 @@
         <color indexed="13"/>
       </left>
       <right style="thin">
-        <color indexed="17"/>
-      </right>
-      <top style="thin">
-        <color indexed="17"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="17"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="17"/>
-      </left>
-      <right style="thin">
-        <color indexed="17"/>
-      </right>
-      <top style="thin">
-        <color indexed="17"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="17"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="13"/>
-      </left>
-      <right style="thin">
         <color indexed="13"/>
       </right>
       <top/>
       <bottom style="thin">
         <color indexed="13"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="13"/>
-      </left>
-      <right style="thin">
-        <color indexed="17"/>
-      </right>
-      <top style="thin">
-        <color indexed="13"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="17"/>
       </bottom>
       <diagonal/>
     </border>
@@ -896,6 +843,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color indexed="17"/>
+      </left>
+      <right style="thin">
+        <color indexed="17"/>
+      </right>
+      <top style="thin">
+        <color indexed="17"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="17"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right style="thin">
         <color indexed="17"/>
@@ -912,6 +874,51 @@
       <top/>
       <bottom style="thin">
         <color indexed="13"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="17"/>
+      </left>
+      <right style="thin">
+        <color indexed="17"/>
+      </right>
+      <top style="thin">
+        <color indexed="13"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="17"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="13"/>
+      </left>
+      <right style="thin">
+        <color indexed="17"/>
+      </right>
+      <top style="thin">
+        <color indexed="17"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="17"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="13"/>
+      </left>
+      <right style="thin">
+        <color indexed="17"/>
+      </right>
+      <top style="thin">
+        <color indexed="13"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="17"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1024,17 +1031,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1054,15 +1052,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -1074,6 +1063,41 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1095,26 +1119,9 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1123,152 +1130,152 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="34" borderId="25" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="43" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="42" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="43" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="38" borderId="27" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="25" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="26" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="31" borderId="28" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="29" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="27" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="27" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="29" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="23" borderId="30" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="28" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="24" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="24" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="25" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="41" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="27" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="26" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="42" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="30" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1296,46 +1303,46 @@
     <xf numFmtId="49" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1344,10 +1351,13 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -1371,7 +1381,7 @@
     <xf numFmtId="49" fontId="0" fillId="10" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1380,7 +1390,7 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1525,6 +1535,11 @@
       <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -2593,12 +2608,11 @@
       </a:style>
     </a:txDef>
   </a:objectDefaults>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:E23"/>
   <sheetViews>
@@ -2606,210 +2620,210 @@
       <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.90825688073394" defaultRowHeight="13.5" customHeight="1" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9.90384615384615" defaultRowHeight="13.5" customHeight="1" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="9" style="9" customWidth="1"/>
-    <col min="2" max="16384" width="6" style="9" customWidth="1"/>
+    <col min="1" max="1" width="9" style="18" customWidth="1"/>
+    <col min="2" max="16384" width="6" style="18" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="14" customHeight="1" spans="1:5">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
+      <c r="B1" s="41"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
     </row>
     <row r="2" ht="14" customHeight="1" spans="1:5">
-      <c r="A2" s="42" t="s">
+      <c r="A2" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="40"/>
-      <c r="C2" s="41"/>
-      <c r="D2" s="41"/>
-      <c r="E2" s="41"/>
+      <c r="B2" s="41"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
     </row>
     <row r="3" ht="14" customHeight="1" spans="1:5">
-      <c r="A3" s="42" t="s">
+      <c r="A3" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="40"/>
-      <c r="C3" s="41"/>
-      <c r="D3" s="41"/>
-      <c r="E3" s="41"/>
+      <c r="B3" s="41"/>
+      <c r="C3" s="42"/>
+      <c r="D3" s="42"/>
+      <c r="E3" s="42"/>
     </row>
     <row r="4" ht="14" customHeight="1" spans="1:5">
-      <c r="A4" s="43" t="s">
+      <c r="A4" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="40"/>
-      <c r="C4" s="41"/>
-      <c r="D4" s="41"/>
-      <c r="E4" s="41"/>
+      <c r="B4" s="41"/>
+      <c r="C4" s="42"/>
+      <c r="D4" s="42"/>
+      <c r="E4" s="42"/>
     </row>
     <row r="5" ht="14" customHeight="1" spans="1:5">
-      <c r="A5" s="44"/>
-      <c r="B5" s="40"/>
-      <c r="C5" s="41"/>
-      <c r="D5" s="41"/>
-      <c r="E5" s="41"/>
+      <c r="A5" s="45"/>
+      <c r="B5" s="41"/>
+      <c r="C5" s="42"/>
+      <c r="D5" s="42"/>
+      <c r="E5" s="42"/>
     </row>
     <row r="6" ht="14" customHeight="1" spans="1:5">
-      <c r="A6" s="44"/>
-      <c r="B6" s="40"/>
-      <c r="C6" s="41"/>
-      <c r="D6" s="41"/>
-      <c r="E6" s="41"/>
+      <c r="A6" s="45"/>
+      <c r="B6" s="41"/>
+      <c r="C6" s="42"/>
+      <c r="D6" s="42"/>
+      <c r="E6" s="42"/>
     </row>
     <row r="7" ht="14" customHeight="1" spans="1:5">
-      <c r="A7" s="43" t="s">
+      <c r="A7" s="44" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="40"/>
-      <c r="C7" s="41"/>
-      <c r="D7" s="41"/>
-      <c r="E7" s="41"/>
+      <c r="B7" s="41"/>
+      <c r="C7" s="42"/>
+      <c r="D7" s="42"/>
+      <c r="E7" s="42"/>
     </row>
     <row r="8" ht="14" customHeight="1" spans="1:5">
-      <c r="A8" s="44"/>
-      <c r="B8" s="40"/>
-      <c r="C8" s="41"/>
-      <c r="D8" s="41"/>
-      <c r="E8" s="41"/>
+      <c r="A8" s="45"/>
+      <c r="B8" s="41"/>
+      <c r="C8" s="42"/>
+      <c r="D8" s="42"/>
+      <c r="E8" s="42"/>
     </row>
     <row r="9" ht="14" customHeight="1" spans="1:5">
-      <c r="A9" s="44"/>
-      <c r="B9" s="40"/>
-      <c r="C9" s="41"/>
-      <c r="D9" s="41"/>
-      <c r="E9" s="41"/>
+      <c r="A9" s="45"/>
+      <c r="B9" s="41"/>
+      <c r="C9" s="42"/>
+      <c r="D9" s="42"/>
+      <c r="E9" s="42"/>
     </row>
     <row r="10" ht="14" customHeight="1" spans="1:5">
-      <c r="A10" s="43" t="s">
+      <c r="A10" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="40"/>
-      <c r="C10" s="41"/>
-      <c r="D10" s="41"/>
-      <c r="E10" s="41"/>
+      <c r="B10" s="41"/>
+      <c r="C10" s="42"/>
+      <c r="D10" s="42"/>
+      <c r="E10" s="42"/>
     </row>
     <row r="11" ht="14" customHeight="1" spans="1:5">
-      <c r="A11" s="43" t="s">
+      <c r="A11" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="40"/>
-      <c r="C11" s="41"/>
-      <c r="D11" s="41"/>
-      <c r="E11" s="41"/>
+      <c r="B11" s="41"/>
+      <c r="C11" s="42"/>
+      <c r="D11" s="42"/>
+      <c r="E11" s="42"/>
     </row>
     <row r="12" ht="14" customHeight="1" spans="1:5">
-      <c r="A12" s="43" t="s">
+      <c r="A12" s="44" t="s">
         <v>7</v>
       </c>
-      <c r="B12" s="40"/>
-      <c r="C12" s="41"/>
-      <c r="D12" s="41"/>
-      <c r="E12" s="41"/>
+      <c r="B12" s="41"/>
+      <c r="C12" s="42"/>
+      <c r="D12" s="42"/>
+      <c r="E12" s="42"/>
     </row>
     <row r="13" ht="14" customHeight="1" spans="1:5">
-      <c r="A13" s="43" t="s">
+      <c r="A13" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="B13" s="40"/>
-      <c r="C13" s="41"/>
-      <c r="D13" s="41"/>
-      <c r="E13" s="41"/>
+      <c r="B13" s="41"/>
+      <c r="C13" s="42"/>
+      <c r="D13" s="42"/>
+      <c r="E13" s="42"/>
     </row>
     <row r="14" ht="14" customHeight="1" spans="1:5">
-      <c r="A14" s="43" t="s">
+      <c r="A14" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="40"/>
-      <c r="C14" s="41"/>
-      <c r="D14" s="41"/>
-      <c r="E14" s="41"/>
+      <c r="B14" s="41"/>
+      <c r="C14" s="42"/>
+      <c r="D14" s="42"/>
+      <c r="E14" s="42"/>
     </row>
     <row r="15" ht="14" customHeight="1" spans="1:5">
-      <c r="A15" s="43" t="s">
+      <c r="A15" s="44" t="s">
         <v>10</v>
       </c>
-      <c r="B15" s="40"/>
-      <c r="C15" s="41"/>
-      <c r="D15" s="41"/>
-      <c r="E15" s="41"/>
+      <c r="B15" s="41"/>
+      <c r="C15" s="42"/>
+      <c r="D15" s="42"/>
+      <c r="E15" s="42"/>
     </row>
     <row r="16" ht="14" customHeight="1" spans="1:5">
-      <c r="A16" s="43" t="s">
+      <c r="A16" s="44" t="s">
         <v>11</v>
       </c>
-      <c r="B16" s="40"/>
-      <c r="C16" s="41"/>
-      <c r="D16" s="41"/>
-      <c r="E16" s="41"/>
+      <c r="B16" s="41"/>
+      <c r="C16" s="42"/>
+      <c r="D16" s="42"/>
+      <c r="E16" s="42"/>
     </row>
     <row r="17" ht="14" customHeight="1" spans="1:5">
-      <c r="A17" s="43" t="s">
+      <c r="A17" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="B17" s="40"/>
-      <c r="C17" s="41"/>
-      <c r="D17" s="41"/>
-      <c r="E17" s="41"/>
+      <c r="B17" s="41"/>
+      <c r="C17" s="42"/>
+      <c r="D17" s="42"/>
+      <c r="E17" s="42"/>
     </row>
     <row r="18" ht="14" customHeight="1" spans="1:5">
-      <c r="A18" s="43" t="s">
+      <c r="A18" s="44" t="s">
         <v>13</v>
       </c>
-      <c r="B18" s="40"/>
-      <c r="C18" s="41"/>
-      <c r="D18" s="41"/>
-      <c r="E18" s="41"/>
+      <c r="B18" s="41"/>
+      <c r="C18" s="42"/>
+      <c r="D18" s="42"/>
+      <c r="E18" s="42"/>
     </row>
     <row r="19" ht="14" customHeight="1" spans="1:5">
-      <c r="A19" s="43" t="s">
+      <c r="A19" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="B19" s="40"/>
-      <c r="C19" s="41"/>
-      <c r="D19" s="41"/>
-      <c r="E19" s="41"/>
+      <c r="B19" s="41"/>
+      <c r="C19" s="42"/>
+      <c r="D19" s="42"/>
+      <c r="E19" s="42"/>
     </row>
     <row r="20" ht="14" customHeight="1" spans="1:5">
-      <c r="A20" s="43" t="s">
+      <c r="A20" s="44" t="s">
         <v>15</v>
       </c>
-      <c r="B20" s="40"/>
-      <c r="C20" s="41"/>
-      <c r="D20" s="41"/>
-      <c r="E20" s="41"/>
+      <c r="B20" s="41"/>
+      <c r="C20" s="42"/>
+      <c r="D20" s="42"/>
+      <c r="E20" s="42"/>
     </row>
     <row r="21" ht="14" customHeight="1" spans="1:5">
-      <c r="A21" s="43" t="s">
+      <c r="A21" s="44" t="s">
         <v>16</v>
       </c>
-      <c r="B21" s="40"/>
-      <c r="C21" s="41"/>
-      <c r="D21" s="41"/>
-      <c r="E21" s="41"/>
+      <c r="B21" s="41"/>
+      <c r="C21" s="42"/>
+      <c r="D21" s="42"/>
+      <c r="E21" s="42"/>
     </row>
     <row r="22" ht="14" customHeight="1" spans="1:5">
-      <c r="A22" s="43" t="s">
+      <c r="A22" s="44" t="s">
         <v>17</v>
       </c>
-      <c r="B22" s="40"/>
-      <c r="C22" s="41"/>
-      <c r="D22" s="41"/>
-      <c r="E22" s="41"/>
+      <c r="B22" s="41"/>
+      <c r="C22" s="42"/>
+      <c r="D22" s="42"/>
+      <c r="E22" s="42"/>
     </row>
     <row r="23" ht="14" customHeight="1" spans="1:5">
-      <c r="A23" s="42" t="s">
+      <c r="A23" s="43" t="s">
         <v>18</v>
       </c>
-      <c r="B23" s="40"/>
-      <c r="C23" s="41"/>
-      <c r="D23" s="41"/>
-      <c r="E23" s="41"/>
+      <c r="B23" s="41"/>
+      <c r="C23" s="42"/>
+      <c r="D23" s="42"/>
+      <c r="E23" s="42"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2825,7 +2839,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -2839,29 +2853,29 @@
       <selection pane="bottomRight" activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.90825688073394" defaultRowHeight="13" customHeight="1" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9.90384615384615" defaultRowHeight="13" customHeight="1" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="1" width="16.3577981651376" style="9" customWidth="1"/>
-    <col min="2" max="2" width="99.1192660550459" style="27" customWidth="1"/>
-    <col min="3" max="16384" width="16.3577981651376" style="9" customWidth="1"/>
+    <col min="1" max="1" width="16.3557692307692" style="18" customWidth="1"/>
+    <col min="2" max="2" width="99.1153846153846" style="28" customWidth="1"/>
+    <col min="3" max="16384" width="16.3557692307692" style="18" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.55" customHeight="1" spans="1:3">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="30" t="s">
+      <c r="C1" s="31" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="2" ht="13.55" customHeight="1" spans="1:3">
-      <c r="A2" s="31" t="s">
+      <c r="A2" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="33" t="s">
         <v>23</v>
       </c>
       <c r="C2" s="23" t="s">
@@ -2869,10 +2883,10 @@
       </c>
     </row>
     <row r="3" ht="13.35" customHeight="1" spans="1:3">
-      <c r="A3" s="33" t="s">
+      <c r="A3" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="34" t="s">
+      <c r="B3" s="35" t="s">
         <v>26</v>
       </c>
       <c r="C3" s="23" t="s">
@@ -2880,59 +2894,59 @@
       </c>
     </row>
     <row r="4" ht="13.35" customHeight="1" spans="1:3">
-      <c r="A4" s="35" t="s">
+      <c r="A4" s="36" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="34" t="s">
+      <c r="B4" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="C4" s="36" t="s">
+      <c r="C4" s="37" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="5" ht="13.35" customHeight="1" spans="1:3">
-      <c r="A5" s="35" t="s">
+      <c r="A5" s="36" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="34" t="s">
+      <c r="B5" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="C5" s="36" t="s">
+      <c r="C5" s="37" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="6" ht="13.35" customHeight="1" spans="1:3">
-      <c r="A6" s="35" t="s">
+      <c r="A6" s="36" t="s">
         <v>32</v>
       </c>
-      <c r="B6" s="37"/>
-      <c r="C6" s="36" t="s">
+      <c r="B6" s="38"/>
+      <c r="C6" s="37" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="7" ht="13.35" customHeight="1" spans="1:3">
-      <c r="A7" s="35" t="s">
+      <c r="A7" s="36" t="s">
         <v>33</v>
       </c>
-      <c r="B7" s="37"/>
-      <c r="C7" s="36" t="s">
+      <c r="B7" s="38"/>
+      <c r="C7" s="37" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="8" ht="13.35" customHeight="1" spans="1:3">
-      <c r="A8" s="35" t="s">
+      <c r="A8" s="36" t="s">
         <v>34</v>
       </c>
-      <c r="B8" s="37"/>
+      <c r="B8" s="38"/>
       <c r="C8" s="23" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="9" ht="13.35" customHeight="1" spans="1:3">
-      <c r="A9" s="35" t="s">
+      <c r="A9" s="36" t="s">
         <v>35</v>
       </c>
-      <c r="B9" s="34" t="s">
+      <c r="B9" s="35" t="s">
         <v>36</v>
       </c>
       <c r="C9" s="23" t="s">
@@ -2940,65 +2954,65 @@
       </c>
     </row>
     <row r="10" ht="13.35" customHeight="1" spans="1:3">
-      <c r="A10" s="35" t="s">
+      <c r="A10" s="36" t="s">
         <v>37</v>
       </c>
-      <c r="B10" s="34" t="s">
+      <c r="B10" s="35" t="s">
         <v>38</v>
       </c>
-      <c r="C10" s="36" t="s">
+      <c r="C10" s="37" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="11" ht="13.35" customHeight="1" spans="1:3">
-      <c r="A11" s="33" t="s">
+      <c r="A11" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="B11" s="34" t="s">
+      <c r="B11" s="35" t="s">
         <v>40</v>
       </c>
-      <c r="C11" s="38" t="s">
+      <c r="C11" s="39" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="12" ht="13.35" customHeight="1" spans="1:3">
-      <c r="A12" s="35" t="s">
+      <c r="A12" s="36" t="s">
         <v>42</v>
       </c>
-      <c r="B12" s="34" t="s">
+      <c r="B12" s="35" t="s">
         <v>43</v>
       </c>
-      <c r="C12" s="36" t="s">
+      <c r="C12" s="37" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="13" ht="13.35" customHeight="1" spans="1:3">
-      <c r="A13" s="35" t="s">
+      <c r="A13" s="36" t="s">
         <v>44</v>
       </c>
-      <c r="B13" s="34" t="s">
+      <c r="B13" s="35" t="s">
         <v>45</v>
       </c>
-      <c r="C13" s="36" t="s">
+      <c r="C13" s="37" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="14" ht="13.35" customHeight="1" spans="1:3">
-      <c r="A14" s="33" t="s">
+      <c r="A14" s="34" t="s">
         <v>46</v>
       </c>
-      <c r="B14" s="34" t="s">
+      <c r="B14" s="35" t="s">
         <v>47</v>
       </c>
-      <c r="C14" s="38" t="s">
+      <c r="C14" s="39" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="15" ht="13.35" customHeight="1" spans="1:3">
-      <c r="A15" s="33" t="s">
+      <c r="A15" s="34" t="s">
         <v>48</v>
       </c>
-      <c r="B15" s="34" t="s">
+      <c r="B15" s="35" t="s">
         <v>49</v>
       </c>
       <c r="C15" s="23" t="s">
@@ -3006,29 +3020,29 @@
       </c>
     </row>
     <row r="16" ht="13.35" customHeight="1" spans="1:3">
-      <c r="A16" s="33" t="s">
+      <c r="A16" s="34" t="s">
         <v>50</v>
       </c>
-      <c r="B16" s="34" t="s">
+      <c r="B16" s="35" t="s">
         <v>51</v>
       </c>
-      <c r="C16" s="38" t="s">
+      <c r="C16" s="39" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="17" ht="13.35" customHeight="1" spans="1:3">
-      <c r="A17" s="33" t="s">
+      <c r="A17" s="34" t="s">
         <v>52</v>
       </c>
-      <c r="B17" s="34" t="s">
+      <c r="B17" s="35" t="s">
         <v>53</v>
       </c>
-      <c r="C17" s="36" t="s">
+      <c r="C17" s="37" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="18" ht="13.35" customHeight="1" spans="1:3">
-      <c r="A18" s="39" t="s">
+      <c r="A18" s="40" t="s">
         <v>54</v>
       </c>
       <c r="B18" s="13" t="s">
@@ -3037,42 +3051,42 @@
       <c r="C18" s="13"/>
     </row>
     <row r="19" customHeight="1" spans="1:2">
-      <c r="A19" s="9" t="s">
+      <c r="A19" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="B19" s="27" t="s">
+      <c r="B19" s="28" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="20" customHeight="1" spans="1:2">
-      <c r="A20" s="9" t="s">
+      <c r="A20" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="B20" s="27" t="s">
+      <c r="B20" s="28" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="21" customHeight="1" spans="1:2">
-      <c r="A21" s="9" t="s">
+      <c r="A21" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="B21" s="27" t="s">
+      <c r="B21" s="28" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="22" customHeight="1" spans="1:2">
-      <c r="A22" s="9" t="s">
+      <c r="A22" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="B22" s="27" t="s">
+      <c r="B22" s="28" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="23" customHeight="1" spans="1:2">
-      <c r="A23" s="9" t="s">
+      <c r="A23" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="B23" s="27" t="s">
+      <c r="B23" s="28" t="s">
         <v>64</v>
       </c>
     </row>
@@ -3091,7 +3105,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -3103,9 +3117,9 @@
       <selection pane="topRight" activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.90825688073394" defaultRowHeight="13" customHeight="1" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="9.90384615384615" defaultRowHeight="13" customHeight="1" outlineLevelCol="7"/>
   <cols>
-    <col min="1" max="16384" width="16.3577981651376" style="9" customWidth="1"/>
+    <col min="1" max="16384" width="16.3557692307692" style="18" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="14" customHeight="1" spans="1:8">
@@ -3119,8 +3133,8 @@
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="20"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="15"/>
     </row>
     <row r="2" ht="14" customHeight="1" spans="1:8">
       <c r="A2" s="4" t="s">
@@ -3133,8 +3147,8 @@
       <c r="D2" s="6"/>
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
-      <c r="G2" s="21"/>
-      <c r="H2" s="22"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="17"/>
     </row>
     <row r="3" ht="14" customHeight="1" spans="1:8">
       <c r="A3" s="7" t="s">
@@ -3166,16 +3180,16 @@
       <c r="A4" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="19"/>
+      <c r="H4" s="19"/>
     </row>
     <row r="5" ht="13.35" customHeight="1" spans="1:8">
-      <c r="A5" s="11"/>
-      <c r="B5" s="12"/>
+      <c r="A5" s="9"/>
+      <c r="B5" s="20"/>
       <c r="C5" s="13"/>
       <c r="D5" s="13"/>
       <c r="E5" s="13" t="s">
@@ -3188,8 +3202,8 @@
       <c r="H5" s="13"/>
     </row>
     <row r="6" ht="13.35" customHeight="1" spans="1:8">
-      <c r="A6" s="11"/>
-      <c r="B6" s="14"/>
+      <c r="A6" s="9"/>
+      <c r="B6" s="21"/>
       <c r="C6" s="13"/>
       <c r="D6" s="13"/>
       <c r="E6" s="13" t="s">
@@ -3202,8 +3216,8 @@
       <c r="H6" s="13"/>
     </row>
     <row r="7" ht="13.35" customHeight="1" spans="1:8">
-      <c r="A7" s="11"/>
-      <c r="B7" s="14" t="s">
+      <c r="A7" s="9"/>
+      <c r="B7" s="21" t="s">
         <v>73</v>
       </c>
       <c r="C7" s="13"/>
@@ -3216,8 +3230,8 @@
       <c r="H7" s="13"/>
     </row>
     <row r="8" ht="13.65" customHeight="1" spans="1:8">
-      <c r="A8" s="15"/>
-      <c r="B8" s="14"/>
+      <c r="A8" s="10"/>
+      <c r="B8" s="21"/>
       <c r="C8" s="13"/>
       <c r="D8" s="13"/>
       <c r="E8" s="13"/>
@@ -3229,7 +3243,7 @@
       <c r="A9" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="B9" s="12"/>
+      <c r="B9" s="20"/>
       <c r="C9" s="13"/>
       <c r="D9" s="13"/>
       <c r="E9" s="13"/>
@@ -3238,8 +3252,8 @@
       <c r="H9" s="13"/>
     </row>
     <row r="10" ht="13.35" customHeight="1" spans="1:8">
-      <c r="A10" s="11"/>
-      <c r="B10" s="14"/>
+      <c r="A10" s="9"/>
+      <c r="B10" s="21"/>
       <c r="C10" s="13"/>
       <c r="D10" s="13"/>
       <c r="E10" s="13"/>
@@ -3248,8 +3262,8 @@
       <c r="H10" s="13"/>
     </row>
     <row r="11" ht="13.65" customHeight="1" spans="1:8">
-      <c r="A11" s="15"/>
-      <c r="B11" s="14"/>
+      <c r="A11" s="10"/>
+      <c r="B11" s="21"/>
       <c r="C11" s="13"/>
       <c r="D11" s="13"/>
       <c r="E11" s="13"/>
@@ -3261,28 +3275,28 @@
       <c r="A12" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="B12" s="16" t="s">
+      <c r="B12" s="22" t="s">
         <v>76</v>
       </c>
       <c r="C12" s="13"/>
       <c r="D12" s="13"/>
       <c r="E12" s="13"/>
       <c r="F12" s="13"/>
-      <c r="G12" s="25" t="s">
+      <c r="G12" s="26" t="s">
         <v>29</v>
       </c>
       <c r="H12" s="13"/>
     </row>
     <row r="13" ht="13.65" customHeight="1" spans="1:8">
-      <c r="A13" s="11"/>
-      <c r="B13" s="14"/>
+      <c r="A13" s="9"/>
+      <c r="B13" s="21"/>
       <c r="C13" s="13" t="s">
         <v>55</v>
       </c>
       <c r="D13" s="13"/>
       <c r="E13" s="13"/>
       <c r="F13" s="13"/>
-      <c r="G13" s="26" t="s">
+      <c r="G13" s="27" t="s">
         <v>77</v>
       </c>
       <c r="H13" s="13" t="s">
@@ -3290,8 +3304,8 @@
       </c>
     </row>
     <row r="14" ht="14" customHeight="1" spans="1:8">
-      <c r="A14" s="15"/>
-      <c r="B14" s="14"/>
+      <c r="A14" s="10"/>
+      <c r="B14" s="21"/>
       <c r="C14" s="13"/>
       <c r="D14" s="13"/>
       <c r="E14" s="13"/>
@@ -3303,7 +3317,7 @@
       <c r="A15" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="B15" s="12"/>
+      <c r="B15" s="20"/>
       <c r="C15" s="13"/>
       <c r="D15" s="13"/>
       <c r="E15" s="13"/>
@@ -3312,8 +3326,8 @@
       <c r="H15" s="13"/>
     </row>
     <row r="16" ht="13.35" customHeight="1" spans="1:8">
-      <c r="A16" s="11"/>
-      <c r="B16" s="12"/>
+      <c r="A16" s="9"/>
+      <c r="B16" s="20"/>
       <c r="C16" s="13"/>
       <c r="D16" s="13"/>
       <c r="E16" s="13"/>
@@ -3322,8 +3336,8 @@
       <c r="H16" s="13"/>
     </row>
     <row r="17" ht="13.65" customHeight="1" spans="1:8">
-      <c r="A17" s="15"/>
-      <c r="B17" s="14"/>
+      <c r="A17" s="10"/>
+      <c r="B17" s="21"/>
       <c r="C17" s="13"/>
       <c r="D17" s="13"/>
       <c r="E17" s="13"/>
@@ -3332,8 +3346,8 @@
       <c r="H17" s="13"/>
     </row>
     <row r="18" ht="13.65" customHeight="1" spans="1:8">
-      <c r="A18" s="17"/>
-      <c r="B18" s="18"/>
+      <c r="A18" s="11"/>
+      <c r="B18" s="12"/>
       <c r="C18" s="13"/>
       <c r="D18" s="13"/>
       <c r="E18" s="13"/>
@@ -3362,21 +3376,21 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D16" sqref="$A1:$XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.90825688073394" defaultRowHeight="13.35" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="9.90384615384615" defaultRowHeight="16.8" outlineLevelCol="7"/>
   <cols>
-    <col min="1" max="1" width="11.7339449541284" customWidth="1"/>
-    <col min="2" max="2" width="17.9724770642202" customWidth="1"/>
-    <col min="3" max="3" width="12.0275229357798" customWidth="1"/>
+    <col min="1" max="1" width="11.7307692307692" customWidth="1"/>
+    <col min="2" max="2" width="17.9711538461538" customWidth="1"/>
+    <col min="3" max="3" width="12.0288461538462" customWidth="1"/>
     <col min="4" max="4" width="15" customWidth="1"/>
-    <col min="8" max="8" width="15.4862385321101" customWidth="1"/>
+    <col min="8" max="8" width="15.4903846153846" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -3390,8 +3404,8 @@
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="20"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="15"/>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="4" t="s">
@@ -3404,8 +3418,8 @@
       <c r="D2" s="6"/>
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
-      <c r="G2" s="21"/>
-      <c r="H2" s="22"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="17"/>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="7" t="s">
@@ -3437,21 +3451,21 @@
       <c r="A4" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="19"/>
       <c r="G4" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="H4" s="10"/>
+      <c r="H4" s="19"/>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="11"/>
-      <c r="B5" s="12"/>
+      <c r="A5" s="9"/>
+      <c r="B5" s="20"/>
       <c r="C5" s="13"/>
       <c r="D5" s="13" t="s">
         <v>81</v>
@@ -3464,8 +3478,8 @@
       <c r="H5" s="13"/>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="11"/>
-      <c r="B6" s="14"/>
+      <c r="A6" s="9"/>
+      <c r="B6" s="21"/>
       <c r="C6" s="13" t="s">
         <v>82</v>
       </c>
@@ -3478,8 +3492,8 @@
       <c r="H6" s="13"/>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="11"/>
-      <c r="B7" s="14" t="s">
+      <c r="A7" s="9"/>
+      <c r="B7" s="21" t="s">
         <v>83</v>
       </c>
       <c r="C7" s="13"/>
@@ -3492,8 +3506,8 @@
       <c r="H7" s="13"/>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="15"/>
-      <c r="B8" s="14"/>
+      <c r="A8" s="10"/>
+      <c r="B8" s="21"/>
       <c r="C8" s="13"/>
       <c r="D8" s="13"/>
       <c r="E8" s="13"/>
@@ -3504,7 +3518,7 @@
       <c r="A9" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="B9" s="12" t="s">
+      <c r="B9" s="20" t="s">
         <v>84</v>
       </c>
       <c r="C9" s="13"/>
@@ -3517,8 +3531,8 @@
       <c r="H9" s="13"/>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="11"/>
-      <c r="B10" s="14" t="s">
+      <c r="A10" s="9"/>
+      <c r="B10" s="21" t="s">
         <v>85</v>
       </c>
       <c r="C10" s="13"/>
@@ -3531,8 +3545,8 @@
       <c r="H10" s="13"/>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" s="15"/>
-      <c r="B11" s="14"/>
+      <c r="A11" s="10"/>
+      <c r="B11" s="21"/>
       <c r="C11" s="13"/>
       <c r="D11" s="13"/>
       <c r="E11" s="13"/>
@@ -3543,18 +3557,21 @@
       <c r="A12" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="B12" s="16" t="s">
+      <c r="B12" s="22" t="s">
         <v>86</v>
       </c>
       <c r="C12" s="13"/>
       <c r="D12" s="13"/>
       <c r="E12" s="13"/>
       <c r="F12" s="13"/>
+      <c r="G12" s="25" t="s">
+        <v>87</v>
+      </c>
       <c r="H12" s="13"/>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" s="11"/>
-      <c r="B13" s="14"/>
+      <c r="A13" s="9"/>
+      <c r="B13" s="21"/>
       <c r="C13" s="13"/>
       <c r="D13" s="13"/>
       <c r="E13" s="13"/>
@@ -3562,8 +3579,8 @@
       <c r="H13" s="13"/>
     </row>
     <row r="14" spans="1:8">
-      <c r="A14" s="15"/>
-      <c r="B14" s="14"/>
+      <c r="A14" s="10"/>
+      <c r="B14" s="21"/>
       <c r="C14" s="13"/>
       <c r="D14" s="13"/>
       <c r="E14" s="13"/>
@@ -3575,19 +3592,21 @@
       <c r="A15" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="B15" s="12" t="s">
+      <c r="B15" s="20" t="s">
         <v>86</v>
       </c>
       <c r="C15" s="13"/>
       <c r="D15" s="13"/>
       <c r="E15" s="13"/>
       <c r="F15" s="13"/>
-      <c r="G15" s="13"/>
+      <c r="G15" s="25" t="s">
+        <v>87</v>
+      </c>
       <c r="H15" s="13"/>
     </row>
     <row r="16" spans="1:8">
-      <c r="A16" s="11"/>
-      <c r="B16" s="12"/>
+      <c r="A16" s="9"/>
+      <c r="B16" s="20"/>
       <c r="C16" s="13"/>
       <c r="D16" s="13"/>
       <c r="E16" s="13"/>
@@ -3596,8 +3615,8 @@
       <c r="H16" s="13"/>
     </row>
     <row r="17" spans="1:8">
-      <c r="A17" s="15"/>
-      <c r="B17" s="14"/>
+      <c r="A17" s="10"/>
+      <c r="B17" s="21"/>
       <c r="C17" s="13"/>
       <c r="D17" s="13"/>
       <c r="E17" s="13"/>
@@ -3606,8 +3625,8 @@
       <c r="H17" s="13"/>
     </row>
     <row r="18" spans="1:8">
-      <c r="A18" s="17"/>
-      <c r="B18" s="18"/>
+      <c r="A18" s="11"/>
+      <c r="B18" s="12"/>
       <c r="C18" s="13"/>
       <c r="D18" s="13"/>
       <c r="E18" s="13"/>
@@ -3623,7 +3642,7 @@
     <mergeCell ref="A15:A17"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G4 G5 G6 G7 G12 G13">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G4 G5 G6 G7 G12 G13 G15">
       <formula1>"未进行,进行中,已暂停,已完成"</formula1>
     </dataValidation>
   </dataValidations>
@@ -3631,4 +3650,154 @@
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:H18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.90384615384615" defaultRowHeight="16.8" outlineLevelCol="7"/>
+  <cols>
+    <col min="1" max="1" width="11.7307692307692" customWidth="1"/>
+    <col min="2" max="2" width="17.9711538461538" customWidth="1"/>
+    <col min="3" max="3" width="12.0288461538462" customWidth="1"/>
+    <col min="4" max="4" width="15" customWidth="1"/>
+    <col min="8" max="8" width="15.4903846153846" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B1" s="2">
+        <v>20220601</v>
+      </c>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="15"/>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B2" s="5">
+        <v>20220630</v>
+      </c>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="17"/>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="B4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" s="9"/>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" s="9"/>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" s="9"/>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" s="10"/>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="B9" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10" s="9"/>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11" s="10"/>
+    </row>
+    <row r="12" spans="1:1">
+      <c r="A12" s="8" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1">
+      <c r="A13" s="9"/>
+    </row>
+    <row r="14" spans="1:1">
+      <c r="A14" s="10"/>
+    </row>
+    <row r="15" spans="1:1">
+      <c r="A15" s="8" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1">
+      <c r="A16" s="9"/>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" s="10"/>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" s="11"/>
+      <c r="B18" s="12"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="13"/>
+      <c r="H18" s="13"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A4:A8"/>
+    <mergeCell ref="A9:A11"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="A15:A17"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Site updated: 2022-06-19 17:11:30
</commit_message>
<xml_diff>
--- a/file/personal/roleImportant/角色要事记录表_2022.xlsx
+++ b/file/personal/roleImportant/角色要事记录表_2022.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27500" windowHeight="11860" activeTab="4"/>
+    <workbookView windowHeight="16360" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="角色目录" sheetId="2" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="89">
   <si>
     <t>角色</t>
   </si>
@@ -292,10 +292,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -306,6 +306,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
@@ -313,22 +320,7 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Helvetica Neue"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="Helvetica Neue"/>
       <charset val="134"/>
@@ -344,17 +336,47 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="3"/>
+      <name val="Helvetica Neue"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
       <name val="Helvetica Neue"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -366,9 +388,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <i/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -383,29 +405,8 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Helvetica Neue"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -419,8 +420,30 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -432,29 +455,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="44">
     <fill>
@@ -538,6 +538,108 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -550,13 +652,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -568,61 +694,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -634,91 +712,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -879,6 +879,21 @@
     </border>
     <border>
       <left style="thin">
+        <color indexed="13"/>
+      </left>
+      <right style="thin">
+        <color indexed="13"/>
+      </right>
+      <top style="thin">
+        <color indexed="18"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="13"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color indexed="17"/>
       </left>
       <right style="thin">
@@ -919,21 +934,6 @@
       </top>
       <bottom style="thin">
         <color indexed="17"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="13"/>
-      </left>
-      <right style="thin">
-        <color indexed="13"/>
-      </right>
-      <top style="thin">
-        <color indexed="18"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="13"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1031,8 +1031,17 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1052,6 +1061,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -1067,22 +1085,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1102,26 +1115,13 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1130,148 +1130,148 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="34" borderId="25" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="43" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="25" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="26" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="31" borderId="28" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="20" borderId="29" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="27" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="24" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="29" borderId="27" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="43" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="42" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="27" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="30" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="26" borderId="29" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="23" borderId="28" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="24" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="27" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="42" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="30" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="25" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="26" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1330,22 +1330,22 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1354,10 +1354,10 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -1387,13 +1387,13 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2622,8 +2622,8 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.90384615384615" defaultRowHeight="13.5" customHeight="1" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="9" style="18" customWidth="1"/>
-    <col min="2" max="16384" width="6" style="18" customWidth="1"/>
+    <col min="1" max="1" width="9" style="19" customWidth="1"/>
+    <col min="2" max="16384" width="6" style="19" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="14" customHeight="1" spans="1:5">
@@ -2855,9 +2855,9 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.90384615384615" defaultRowHeight="13" customHeight="1" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="1" width="16.3557692307692" style="18" customWidth="1"/>
+    <col min="1" max="1" width="16.3557692307692" style="19" customWidth="1"/>
     <col min="2" max="2" width="99.1153846153846" style="28" customWidth="1"/>
-    <col min="3" max="16384" width="16.3557692307692" style="18" customWidth="1"/>
+    <col min="3" max="16384" width="16.3557692307692" style="19" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.55" customHeight="1" spans="1:3">
@@ -2878,7 +2878,7 @@
       <c r="B2" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="23" t="s">
+      <c r="C2" s="18" t="s">
         <v>24</v>
       </c>
     </row>
@@ -2889,7 +2889,7 @@
       <c r="B3" s="35" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="23" t="s">
+      <c r="C3" s="18" t="s">
         <v>24</v>
       </c>
     </row>
@@ -2938,7 +2938,7 @@
         <v>34</v>
       </c>
       <c r="B8" s="38"/>
-      <c r="C8" s="23" t="s">
+      <c r="C8" s="18" t="s">
         <v>24</v>
       </c>
     </row>
@@ -2949,7 +2949,7 @@
       <c r="B9" s="35" t="s">
         <v>36</v>
       </c>
-      <c r="C9" s="23" t="s">
+      <c r="C9" s="18" t="s">
         <v>24</v>
       </c>
     </row>
@@ -3015,7 +3015,7 @@
       <c r="B15" s="35" t="s">
         <v>49</v>
       </c>
-      <c r="C15" s="23" t="s">
+      <c r="C15" s="18" t="s">
         <v>24</v>
       </c>
     </row>
@@ -3051,7 +3051,7 @@
       <c r="C18" s="13"/>
     </row>
     <row r="19" customHeight="1" spans="1:2">
-      <c r="A19" s="18" t="s">
+      <c r="A19" s="19" t="s">
         <v>56</v>
       </c>
       <c r="B19" s="28" t="s">
@@ -3059,7 +3059,7 @@
       </c>
     </row>
     <row r="20" customHeight="1" spans="1:2">
-      <c r="A20" s="18" t="s">
+      <c r="A20" s="19" t="s">
         <v>58</v>
       </c>
       <c r="B20" s="28" t="s">
@@ -3067,7 +3067,7 @@
       </c>
     </row>
     <row r="21" customHeight="1" spans="1:2">
-      <c r="A21" s="18" t="s">
+      <c r="A21" s="19" t="s">
         <v>58</v>
       </c>
       <c r="B21" s="28" t="s">
@@ -3075,7 +3075,7 @@
       </c>
     </row>
     <row r="22" customHeight="1" spans="1:2">
-      <c r="A22" s="18" t="s">
+      <c r="A22" s="19" t="s">
         <v>61</v>
       </c>
       <c r="B22" s="28" t="s">
@@ -3083,7 +3083,7 @@
       </c>
     </row>
     <row r="23" customHeight="1" spans="1:2">
-      <c r="A23" s="18" t="s">
+      <c r="A23" s="19" t="s">
         <v>63</v>
       </c>
       <c r="B23" s="28" t="s">
@@ -3119,7 +3119,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.90384615384615" defaultRowHeight="13" customHeight="1" outlineLevelCol="7"/>
   <cols>
-    <col min="1" max="16384" width="16.3557692307692" style="18" customWidth="1"/>
+    <col min="1" max="16384" width="16.3557692307692" style="19" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="14" customHeight="1" spans="1:8">
@@ -3180,58 +3180,58 @@
       <c r="A4" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="C4" s="19"/>
-      <c r="D4" s="19"/>
-      <c r="E4" s="19"/>
-      <c r="F4" s="19"/>
-      <c r="G4" s="19"/>
-      <c r="H4" s="19"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
     </row>
     <row r="5" ht="13.35" customHeight="1" spans="1:8">
       <c r="A5" s="9"/>
-      <c r="B5" s="20"/>
+      <c r="B5" s="21"/>
       <c r="C5" s="13"/>
       <c r="D5" s="13"/>
       <c r="E5" s="13" t="s">
         <v>71</v>
       </c>
       <c r="F5" s="13"/>
-      <c r="G5" s="23" t="s">
+      <c r="G5" s="18" t="s">
         <v>24</v>
       </c>
       <c r="H5" s="13"/>
     </row>
     <row r="6" ht="13.35" customHeight="1" spans="1:8">
       <c r="A6" s="9"/>
-      <c r="B6" s="21"/>
+      <c r="B6" s="22"/>
       <c r="C6" s="13"/>
       <c r="D6" s="13"/>
       <c r="E6" s="13" t="s">
         <v>72</v>
       </c>
       <c r="F6" s="13"/>
-      <c r="G6" s="23" t="s">
+      <c r="G6" s="18" t="s">
         <v>24</v>
       </c>
       <c r="H6" s="13"/>
     </row>
     <row r="7" ht="13.35" customHeight="1" spans="1:8">
       <c r="A7" s="9"/>
-      <c r="B7" s="21" t="s">
+      <c r="B7" s="22" t="s">
         <v>73</v>
       </c>
       <c r="C7" s="13"/>
       <c r="D7" s="13"/>
       <c r="E7" s="13"/>
       <c r="F7" s="13"/>
-      <c r="G7" s="23" t="s">
+      <c r="G7" s="18" t="s">
         <v>24</v>
       </c>
       <c r="H7" s="13"/>
     </row>
     <row r="8" ht="13.65" customHeight="1" spans="1:8">
       <c r="A8" s="10"/>
-      <c r="B8" s="21"/>
+      <c r="B8" s="22"/>
       <c r="C8" s="13"/>
       <c r="D8" s="13"/>
       <c r="E8" s="13"/>
@@ -3243,7 +3243,7 @@
       <c r="A9" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="B9" s="20"/>
+      <c r="B9" s="21"/>
       <c r="C9" s="13"/>
       <c r="D9" s="13"/>
       <c r="E9" s="13"/>
@@ -3253,7 +3253,7 @@
     </row>
     <row r="10" ht="13.35" customHeight="1" spans="1:8">
       <c r="A10" s="9"/>
-      <c r="B10" s="21"/>
+      <c r="B10" s="22"/>
       <c r="C10" s="13"/>
       <c r="D10" s="13"/>
       <c r="E10" s="13"/>
@@ -3263,7 +3263,7 @@
     </row>
     <row r="11" ht="13.65" customHeight="1" spans="1:8">
       <c r="A11" s="10"/>
-      <c r="B11" s="21"/>
+      <c r="B11" s="22"/>
       <c r="C11" s="13"/>
       <c r="D11" s="13"/>
       <c r="E11" s="13"/>
@@ -3275,7 +3275,7 @@
       <c r="A12" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="B12" s="22" t="s">
+      <c r="B12" s="23" t="s">
         <v>76</v>
       </c>
       <c r="C12" s="13"/>
@@ -3289,7 +3289,7 @@
     </row>
     <row r="13" ht="13.65" customHeight="1" spans="1:8">
       <c r="A13" s="9"/>
-      <c r="B13" s="21"/>
+      <c r="B13" s="22"/>
       <c r="C13" s="13" t="s">
         <v>55</v>
       </c>
@@ -3305,7 +3305,7 @@
     </row>
     <row r="14" ht="14" customHeight="1" spans="1:8">
       <c r="A14" s="10"/>
-      <c r="B14" s="21"/>
+      <c r="B14" s="22"/>
       <c r="C14" s="13"/>
       <c r="D14" s="13"/>
       <c r="E14" s="13"/>
@@ -3317,7 +3317,7 @@
       <c r="A15" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="B15" s="20"/>
+      <c r="B15" s="21"/>
       <c r="C15" s="13"/>
       <c r="D15" s="13"/>
       <c r="E15" s="13"/>
@@ -3327,7 +3327,7 @@
     </row>
     <row r="16" ht="13.35" customHeight="1" spans="1:8">
       <c r="A16" s="9"/>
-      <c r="B16" s="20"/>
+      <c r="B16" s="21"/>
       <c r="C16" s="13"/>
       <c r="D16" s="13"/>
       <c r="E16" s="13"/>
@@ -3337,7 +3337,7 @@
     </row>
     <row r="17" ht="13.65" customHeight="1" spans="1:8">
       <c r="A17" s="10"/>
-      <c r="B17" s="21"/>
+      <c r="B17" s="22"/>
       <c r="C17" s="13"/>
       <c r="D17" s="13"/>
       <c r="E17" s="13"/>
@@ -3381,7 +3381,7 @@
   <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D16" sqref="$A1:$XFD1048576"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.90384615384615" defaultRowHeight="16.8" outlineLevelCol="7"/>
@@ -3451,63 +3451,63 @@
       <c r="A4" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="B4" s="18" t="s">
+      <c r="B4" s="19" t="s">
         <v>80</v>
       </c>
-      <c r="C4" s="19"/>
-      <c r="D4" s="19"/>
-      <c r="E4" s="19"/>
-      <c r="F4" s="19"/>
-      <c r="G4" s="23" t="s">
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="H4" s="19"/>
+      <c r="H4" s="20"/>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="9"/>
-      <c r="B5" s="20"/>
+      <c r="B5" s="21"/>
       <c r="C5" s="13"/>
       <c r="D5" s="13" t="s">
         <v>81</v>
       </c>
       <c r="E5" s="13"/>
       <c r="F5" s="13"/>
-      <c r="G5" s="23" t="s">
+      <c r="G5" s="18" t="s">
         <v>24</v>
       </c>
       <c r="H5" s="13"/>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="9"/>
-      <c r="B6" s="21"/>
+      <c r="B6" s="22"/>
       <c r="C6" s="13" t="s">
         <v>82</v>
       </c>
       <c r="D6" s="13"/>
       <c r="E6" s="13"/>
       <c r="F6" s="13"/>
-      <c r="G6" s="23" t="s">
+      <c r="G6" s="18" t="s">
         <v>24</v>
       </c>
       <c r="H6" s="13"/>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="9"/>
-      <c r="B7" s="21" t="s">
+      <c r="B7" s="22" t="s">
         <v>83</v>
       </c>
       <c r="C7" s="13"/>
       <c r="D7" s="13"/>
       <c r="E7" s="13"/>
       <c r="F7" s="13"/>
-      <c r="G7" s="23" t="s">
+      <c r="G7" s="18" t="s">
         <v>24</v>
       </c>
       <c r="H7" s="13"/>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="10"/>
-      <c r="B8" s="21"/>
+      <c r="B8" s="22"/>
       <c r="C8" s="13"/>
       <c r="D8" s="13"/>
       <c r="E8" s="13"/>
@@ -3518,7 +3518,7 @@
       <c r="A9" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="B9" s="20" t="s">
+      <c r="B9" s="21" t="s">
         <v>84</v>
       </c>
       <c r="C9" s="13"/>
@@ -3532,7 +3532,7 @@
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="9"/>
-      <c r="B10" s="21" t="s">
+      <c r="B10" s="22" t="s">
         <v>85</v>
       </c>
       <c r="C10" s="13"/>
@@ -3546,7 +3546,7 @@
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="10"/>
-      <c r="B11" s="21"/>
+      <c r="B11" s="22"/>
       <c r="C11" s="13"/>
       <c r="D11" s="13"/>
       <c r="E11" s="13"/>
@@ -3557,7 +3557,7 @@
       <c r="A12" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="B12" s="22" t="s">
+      <c r="B12" s="23" t="s">
         <v>86</v>
       </c>
       <c r="C12" s="13"/>
@@ -3571,7 +3571,7 @@
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="9"/>
-      <c r="B13" s="21"/>
+      <c r="B13" s="22"/>
       <c r="C13" s="13"/>
       <c r="D13" s="13"/>
       <c r="E13" s="13"/>
@@ -3580,7 +3580,7 @@
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="10"/>
-      <c r="B14" s="21"/>
+      <c r="B14" s="22"/>
       <c r="C14" s="13"/>
       <c r="D14" s="13"/>
       <c r="E14" s="13"/>
@@ -3592,7 +3592,7 @@
       <c r="A15" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="B15" s="20" t="s">
+      <c r="B15" s="21" t="s">
         <v>86</v>
       </c>
       <c r="C15" s="13"/>
@@ -3606,7 +3606,7 @@
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="9"/>
-      <c r="B16" s="20"/>
+      <c r="B16" s="21"/>
       <c r="C16" s="13"/>
       <c r="D16" s="13"/>
       <c r="E16" s="13"/>
@@ -3616,7 +3616,7 @@
     </row>
     <row r="17" spans="1:8">
       <c r="A17" s="10"/>
-      <c r="B17" s="21"/>
+      <c r="B17" s="22"/>
       <c r="C17" s="13"/>
       <c r="D17" s="13"/>
       <c r="E17" s="13"/>
@@ -3658,7 +3658,7 @@
   <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.90384615384615" defaultRowHeight="16.8" outlineLevelCol="7"/>
@@ -3724,13 +3724,16 @@
         <v>69</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:7">
       <c r="A4" s="8" t="s">
         <v>70</v>
       </c>
       <c r="B4" t="s">
         <v>88</v>
       </c>
+      <c r="G4" s="18" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" s="9"/>
@@ -3744,12 +3747,15 @@
     <row r="8" spans="1:1">
       <c r="A8" s="10"/>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:7">
       <c r="A9" s="8" t="s">
         <v>74</v>
       </c>
       <c r="B9" t="s">
         <v>88</v>
+      </c>
+      <c r="G9" s="18" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:1">
@@ -3797,6 +3803,11 @@
     <mergeCell ref="A12:A13"/>
     <mergeCell ref="A15:A17"/>
   </mergeCells>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G4 G9">
+      <formula1>"未进行,进行中,已暂停,已完成"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>

</xml_diff>

<commit_message>
Site updated: 2022-07-12 23:38:08
</commit_message>
<xml_diff>
--- a/file/personal/roleImportant/角色要事记录表_2022.xlsx
+++ b/file/personal/roleImportant/角色要事记录表_2022.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="16360" activeTab="4"/>
+    <workbookView windowHeight="16360" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="角色目录" sheetId="2" r:id="rId1"/>
@@ -12,13 +12,14 @@
     <sheet name="四月" sheetId="10" r:id="rId3"/>
     <sheet name="五月" sheetId="11" r:id="rId4"/>
     <sheet name="六月" sheetId="12" r:id="rId5"/>
+    <sheet name="七月" sheetId="13" r:id="rId6"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="94">
   <si>
     <t>角色</t>
   </si>
@@ -285,6 +286,21 @@
   </si>
   <si>
     <t>印象笔记技术文档整理</t>
+  </si>
+  <si>
+    <t>eureka整理完成</t>
+  </si>
+  <si>
+    <t>面试资料过一遍</t>
+  </si>
+  <si>
+    <t>自己有所懈怠并且第一遍一定是耗时最长的</t>
+  </si>
+  <si>
+    <t>feign+ribbon梳理完成</t>
+  </si>
+  <si>
+    <t>feign+ribbon+eureka整理完成</t>
   </si>
 </sst>
 </file>
@@ -292,8 +308,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
@@ -319,23 +335,23 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Helvetica Neue"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Helvetica Neue"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="Helvetica Neue"/>
       <charset val="134"/>
@@ -351,7 +367,46 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="1"/>
+      <name val="Helvetica Neue"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Helvetica Neue"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Helvetica Neue"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -359,6 +414,13 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -372,71 +434,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Helvetica Neue"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Helvetica Neue"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -449,8 +449,24 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF800080"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Helvetica Neue"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -489,13 +505,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -544,19 +560,169 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -568,157 +734,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -813,6 +829,26 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right style="thin">
+        <color indexed="17"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="17"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="13"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color indexed="17"/>
       </left>
@@ -854,26 +890,6 @@
       </top>
       <bottom style="thin">
         <color indexed="17"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="17"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="17"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="13"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1039,6 +1055,17 @@
     <border>
       <left/>
       <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
       <bottom style="medium">
         <color theme="4"/>
@@ -1057,30 +1084,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1115,13 +1118,26 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1130,142 +1146,142 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="29" borderId="27" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="42" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="41" borderId="29" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="43" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="42" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="23" borderId="27" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="30" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="26" borderId="29" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="23" borderId="28" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="24" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="43" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="22" borderId="29" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="28" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="27" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="25" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="25" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="26" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="26" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="41" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="25" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="30" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1309,30 +1325,33 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1348,16 +1367,13 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -1381,7 +1397,7 @@
     <xf numFmtId="49" fontId="0" fillId="10" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1390,7 +1406,7 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2622,8 +2638,8 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.90384615384615" defaultRowHeight="13.5" customHeight="1" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="9" style="19" customWidth="1"/>
-    <col min="2" max="16384" width="6" style="19" customWidth="1"/>
+    <col min="1" max="1" width="9" style="20" customWidth="1"/>
+    <col min="2" max="16384" width="6" style="20" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="14" customHeight="1" spans="1:5">
@@ -2846,18 +2862,18 @@
   <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B9" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="B26" sqref="B26"/>
+      <selection pane="bottomRight" activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.90384615384615" defaultRowHeight="13" customHeight="1" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="1" width="16.3557692307692" style="19" customWidth="1"/>
+    <col min="1" max="1" width="16.3557692307692" style="20" customWidth="1"/>
     <col min="2" max="2" width="99.1153846153846" style="28" customWidth="1"/>
-    <col min="3" max="16384" width="16.3557692307692" style="19" customWidth="1"/>
+    <col min="3" max="16384" width="16.3557692307692" style="20" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.55" customHeight="1" spans="1:3">
@@ -3045,13 +3061,13 @@
       <c r="A18" s="40" t="s">
         <v>54</v>
       </c>
-      <c r="B18" s="13" t="s">
+      <c r="B18" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="C18" s="13"/>
+      <c r="C18" s="17"/>
     </row>
     <row r="19" customHeight="1" spans="1:2">
-      <c r="A19" s="19" t="s">
+      <c r="A19" s="20" t="s">
         <v>56</v>
       </c>
       <c r="B19" s="28" t="s">
@@ -3059,7 +3075,7 @@
       </c>
     </row>
     <row r="20" customHeight="1" spans="1:2">
-      <c r="A20" s="19" t="s">
+      <c r="A20" s="20" t="s">
         <v>58</v>
       </c>
       <c r="B20" s="28" t="s">
@@ -3067,7 +3083,7 @@
       </c>
     </row>
     <row r="21" customHeight="1" spans="1:2">
-      <c r="A21" s="19" t="s">
+      <c r="A21" s="20" t="s">
         <v>58</v>
       </c>
       <c r="B21" s="28" t="s">
@@ -3075,24 +3091,27 @@
       </c>
     </row>
     <row r="22" customHeight="1" spans="1:2">
-      <c r="A22" s="19" t="s">
+      <c r="A22" s="20" t="s">
         <v>61</v>
       </c>
       <c r="B22" s="28" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="23" customHeight="1" spans="1:2">
-      <c r="A23" s="19" t="s">
+    <row r="23" customHeight="1" spans="1:3">
+      <c r="A23" s="20" t="s">
         <v>63</v>
       </c>
       <c r="B23" s="28" t="s">
         <v>64</v>
       </c>
+      <c r="C23" s="18" t="s">
+        <v>24</v>
+      </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2 C3 C8 C9 C10 C11 C12 C13 C14 C15 C16 C17 C4:C7">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2 C3 C8 C9 C10 C11 C12 C13 C14 C15 C16 C17 C23 C4:C7">
       <formula1>"未进行,进行中,已暂停,已完成"</formula1>
     </dataValidation>
   </dataValidations>
@@ -3119,7 +3138,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.90384615384615" defaultRowHeight="13" customHeight="1" outlineLevelCol="7"/>
   <cols>
-    <col min="1" max="16384" width="16.3557692307692" style="19" customWidth="1"/>
+    <col min="1" max="16384" width="16.3557692307692" style="20" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="14" customHeight="1" spans="1:8">
@@ -3133,8 +3152,8 @@
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="15"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="12"/>
     </row>
     <row r="2" ht="14" customHeight="1" spans="1:8">
       <c r="A2" s="4" t="s">
@@ -3147,8 +3166,8 @@
       <c r="D2" s="6"/>
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="17"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="14"/>
     </row>
     <row r="3" ht="14" customHeight="1" spans="1:8">
       <c r="A3" s="7" t="s">
@@ -3180,180 +3199,180 @@
       <c r="A4" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="C4" s="20"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="20"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="20"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="21"/>
+      <c r="F4" s="21"/>
+      <c r="G4" s="21"/>
+      <c r="H4" s="21"/>
     </row>
     <row r="5" ht="13.35" customHeight="1" spans="1:8">
       <c r="A5" s="9"/>
-      <c r="B5" s="21"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13" t="s">
+      <c r="B5" s="22"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="17" t="s">
         <v>71</v>
       </c>
-      <c r="F5" s="13"/>
+      <c r="F5" s="17"/>
       <c r="G5" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="H5" s="13"/>
+      <c r="H5" s="17"/>
     </row>
     <row r="6" ht="13.35" customHeight="1" spans="1:8">
       <c r="A6" s="9"/>
-      <c r="B6" s="22"/>
-      <c r="C6" s="13"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13" t="s">
+      <c r="B6" s="23"/>
+      <c r="C6" s="17"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="F6" s="13"/>
+      <c r="F6" s="17"/>
       <c r="G6" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="H6" s="13"/>
+      <c r="H6" s="17"/>
     </row>
     <row r="7" ht="13.35" customHeight="1" spans="1:8">
       <c r="A7" s="9"/>
-      <c r="B7" s="22" t="s">
+      <c r="B7" s="23" t="s">
         <v>73</v>
       </c>
-      <c r="C7" s="13"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="13"/>
+      <c r="C7" s="17"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="17"/>
       <c r="G7" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="H7" s="13"/>
+      <c r="H7" s="17"/>
     </row>
     <row r="8" ht="13.65" customHeight="1" spans="1:8">
       <c r="A8" s="10"/>
-      <c r="B8" s="22"/>
-      <c r="C8" s="13"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
-      <c r="H8" s="13"/>
+      <c r="B8" s="23"/>
+      <c r="C8" s="17"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="17"/>
+      <c r="G8" s="17"/>
+      <c r="H8" s="17"/>
     </row>
     <row r="9" ht="13.65" customHeight="1" spans="1:8">
       <c r="A9" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="B9" s="21"/>
-      <c r="C9" s="13"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
-      <c r="H9" s="13"/>
+      <c r="B9" s="22"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="17"/>
+      <c r="H9" s="17"/>
     </row>
     <row r="10" ht="13.35" customHeight="1" spans="1:8">
       <c r="A10" s="9"/>
-      <c r="B10" s="22"/>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="13"/>
+      <c r="B10" s="23"/>
+      <c r="C10" s="17"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="17"/>
+      <c r="G10" s="17"/>
+      <c r="H10" s="17"/>
     </row>
     <row r="11" ht="13.65" customHeight="1" spans="1:8">
       <c r="A11" s="10"/>
-      <c r="B11" s="22"/>
-      <c r="C11" s="13"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="13"/>
-      <c r="H11" s="13"/>
+      <c r="B11" s="23"/>
+      <c r="C11" s="17"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="17"/>
+      <c r="G11" s="17"/>
+      <c r="H11" s="17"/>
     </row>
     <row r="12" ht="13.65" customHeight="1" spans="1:8">
       <c r="A12" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="B12" s="23" t="s">
+      <c r="B12" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="C12" s="13"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
+      <c r="C12" s="17"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="17"/>
       <c r="G12" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="H12" s="13"/>
+      <c r="H12" s="17"/>
     </row>
     <row r="13" ht="13.65" customHeight="1" spans="1:8">
       <c r="A13" s="9"/>
-      <c r="B13" s="22"/>
-      <c r="C13" s="13" t="s">
+      <c r="B13" s="23"/>
+      <c r="C13" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="17"/>
+      <c r="F13" s="17"/>
       <c r="G13" s="27" t="s">
         <v>77</v>
       </c>
-      <c r="H13" s="13" t="s">
+      <c r="H13" s="17" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="14" ht="14" customHeight="1" spans="1:8">
       <c r="A14" s="10"/>
-      <c r="B14" s="22"/>
-      <c r="C14" s="13"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="13"/>
-      <c r="H14" s="13"/>
+      <c r="B14" s="23"/>
+      <c r="C14" s="17"/>
+      <c r="D14" s="17"/>
+      <c r="E14" s="17"/>
+      <c r="F14" s="17"/>
+      <c r="G14" s="17"/>
+      <c r="H14" s="17"/>
     </row>
     <row r="15" ht="13.65" customHeight="1" spans="1:8">
       <c r="A15" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="B15" s="21"/>
-      <c r="C15" s="13"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="13"/>
-      <c r="H15" s="13"/>
+      <c r="B15" s="22"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="17"/>
+      <c r="E15" s="17"/>
+      <c r="F15" s="17"/>
+      <c r="G15" s="17"/>
+      <c r="H15" s="17"/>
     </row>
     <row r="16" ht="13.35" customHeight="1" spans="1:8">
       <c r="A16" s="9"/>
-      <c r="B16" s="21"/>
-      <c r="C16" s="13"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="13"/>
-      <c r="G16" s="13"/>
-      <c r="H16" s="13"/>
+      <c r="B16" s="22"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="17"/>
+      <c r="E16" s="17"/>
+      <c r="F16" s="17"/>
+      <c r="G16" s="17"/>
+      <c r="H16" s="17"/>
     </row>
     <row r="17" ht="13.65" customHeight="1" spans="1:8">
       <c r="A17" s="10"/>
-      <c r="B17" s="22"/>
-      <c r="C17" s="13"/>
-      <c r="D17" s="13"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="13"/>
-      <c r="H17" s="13"/>
+      <c r="B17" s="23"/>
+      <c r="C17" s="17"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="17"/>
+      <c r="F17" s="17"/>
+      <c r="G17" s="17"/>
+      <c r="H17" s="17"/>
     </row>
     <row r="18" ht="13.65" customHeight="1" spans="1:8">
-      <c r="A18" s="11"/>
-      <c r="B18" s="12"/>
-      <c r="C18" s="13"/>
-      <c r="D18" s="13"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="13"/>
-      <c r="H18" s="13"/>
+      <c r="A18" s="15"/>
+      <c r="B18" s="16"/>
+      <c r="C18" s="17"/>
+      <c r="D18" s="17"/>
+      <c r="E18" s="17"/>
+      <c r="F18" s="17"/>
+      <c r="G18" s="17"/>
+      <c r="H18" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -3381,7 +3400,7 @@
   <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.90384615384615" defaultRowHeight="16.8" outlineLevelCol="7"/>
@@ -3404,8 +3423,8 @@
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="15"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="12"/>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="4" t="s">
@@ -3418,8 +3437,8 @@
       <c r="D2" s="6"/>
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="17"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="14"/>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="7" t="s">
@@ -3451,188 +3470,188 @@
       <c r="A4" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="B4" s="19" t="s">
+      <c r="B4" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="C4" s="20"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="20"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="21"/>
+      <c r="F4" s="21"/>
       <c r="G4" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="H4" s="20"/>
+      <c r="H4" s="21"/>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="9"/>
-      <c r="B5" s="21"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13" t="s">
+      <c r="B5" s="22"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="17" t="s">
         <v>81</v>
       </c>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="17"/>
       <c r="G5" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="H5" s="13"/>
+      <c r="H5" s="17"/>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="9"/>
-      <c r="B6" s="22"/>
-      <c r="C6" s="13" t="s">
+      <c r="B6" s="23"/>
+      <c r="C6" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="13"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="17"/>
+      <c r="F6" s="17"/>
       <c r="G6" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="H6" s="13"/>
+      <c r="H6" s="17"/>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="9"/>
-      <c r="B7" s="22" t="s">
+      <c r="B7" s="23" t="s">
         <v>83</v>
       </c>
-      <c r="C7" s="13"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="13"/>
+      <c r="C7" s="17"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="17"/>
       <c r="G7" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="H7" s="13"/>
+      <c r="H7" s="17"/>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="10"/>
-      <c r="B8" s="22"/>
-      <c r="C8" s="13"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
-      <c r="H8" s="13"/>
+      <c r="B8" s="23"/>
+      <c r="C8" s="17"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="17"/>
+      <c r="H8" s="17"/>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="B9" s="21" t="s">
+      <c r="B9" s="22" t="s">
         <v>84</v>
       </c>
-      <c r="C9" s="13"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="24" t="s">
+      <c r="C9" s="17"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="H9" s="13"/>
+      <c r="H9" s="17"/>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="9"/>
-      <c r="B10" s="22" t="s">
+      <c r="B10" s="23" t="s">
         <v>85</v>
       </c>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="24" t="s">
+      <c r="C10" s="17"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="17"/>
+      <c r="G10" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="H10" s="13"/>
+      <c r="H10" s="17"/>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="10"/>
-      <c r="B11" s="22"/>
-      <c r="C11" s="13"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
-      <c r="H11" s="13"/>
+      <c r="B11" s="23"/>
+      <c r="C11" s="17"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="17"/>
+      <c r="H11" s="17"/>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="B12" s="23" t="s">
+      <c r="B12" s="24" t="s">
         <v>86</v>
       </c>
-      <c r="C12" s="13"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="25" t="s">
+      <c r="C12" s="17"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="17"/>
+      <c r="G12" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="H12" s="13"/>
+      <c r="H12" s="17"/>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="9"/>
-      <c r="B13" s="22"/>
-      <c r="C13" s="13"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
-      <c r="H13" s="13"/>
+      <c r="B13" s="23"/>
+      <c r="C13" s="17"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="17"/>
+      <c r="F13" s="17"/>
+      <c r="H13" s="17"/>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="10"/>
-      <c r="B14" s="22"/>
-      <c r="C14" s="13"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="13"/>
-      <c r="H14" s="13"/>
+      <c r="B14" s="23"/>
+      <c r="C14" s="17"/>
+      <c r="D14" s="17"/>
+      <c r="E14" s="17"/>
+      <c r="F14" s="17"/>
+      <c r="G14" s="17"/>
+      <c r="H14" s="17"/>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="B15" s="21" t="s">
+      <c r="B15" s="22" t="s">
         <v>86</v>
       </c>
-      <c r="C15" s="13"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="25" t="s">
+      <c r="C15" s="17"/>
+      <c r="D15" s="17"/>
+      <c r="E15" s="17"/>
+      <c r="F15" s="17"/>
+      <c r="G15" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="H15" s="13"/>
+      <c r="H15" s="17"/>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="9"/>
-      <c r="B16" s="21"/>
-      <c r="C16" s="13"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="13"/>
-      <c r="G16" s="13"/>
-      <c r="H16" s="13"/>
+      <c r="B16" s="22"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="17"/>
+      <c r="E16" s="17"/>
+      <c r="F16" s="17"/>
+      <c r="G16" s="17"/>
+      <c r="H16" s="17"/>
     </row>
     <row r="17" spans="1:8">
       <c r="A17" s="10"/>
-      <c r="B17" s="22"/>
-      <c r="C17" s="13"/>
-      <c r="D17" s="13"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="13"/>
-      <c r="H17" s="13"/>
+      <c r="B17" s="23"/>
+      <c r="C17" s="17"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="17"/>
+      <c r="F17" s="17"/>
+      <c r="G17" s="17"/>
+      <c r="H17" s="17"/>
     </row>
     <row r="18" spans="1:8">
-      <c r="A18" s="11"/>
-      <c r="B18" s="12"/>
-      <c r="C18" s="13"/>
-      <c r="D18" s="13"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="13"/>
-      <c r="H18" s="13"/>
+      <c r="A18" s="15"/>
+      <c r="B18" s="16"/>
+      <c r="C18" s="17"/>
+      <c r="D18" s="17"/>
+      <c r="E18" s="17"/>
+      <c r="F18" s="17"/>
+      <c r="G18" s="17"/>
+      <c r="H18" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -3657,8 +3676,8 @@
   <sheetPr/>
   <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.90384615384615" defaultRowHeight="16.8" outlineLevelCol="7"/>
@@ -3681,8 +3700,8 @@
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="15"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="12"/>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="4" t="s">
@@ -3695,8 +3714,8 @@
       <c r="D2" s="6"/>
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="17"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="14"/>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="7" t="s">
@@ -3764,37 +3783,64 @@
     <row r="11" spans="1:1">
       <c r="A11" s="10"/>
     </row>
-    <row r="12" spans="1:1">
+    <row r="12" spans="1:7">
       <c r="A12" s="8" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="13" spans="1:1">
+      <c r="B12" t="s">
+        <v>89</v>
+      </c>
+      <c r="G12" s="18" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
       <c r="A13" s="9"/>
+      <c r="B13" t="s">
+        <v>90</v>
+      </c>
+      <c r="G13" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="H13" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" s="10"/>
     </row>
-    <row r="15" spans="1:1">
+    <row r="15" spans="1:7">
       <c r="A15" s="8" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="16" spans="1:1">
+      <c r="B15" t="s">
+        <v>92</v>
+      </c>
+      <c r="G15" s="19" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
       <c r="A16" s="9"/>
+      <c r="B16" t="s">
+        <v>90</v>
+      </c>
+      <c r="G16" s="19" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" s="10"/>
     </row>
     <row r="18" spans="1:8">
-      <c r="A18" s="11"/>
-      <c r="B18" s="12"/>
-      <c r="C18" s="13"/>
-      <c r="D18" s="13"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="13"/>
-      <c r="H18" s="13"/>
+      <c r="A18" s="15"/>
+      <c r="B18" s="16"/>
+      <c r="C18" s="17"/>
+      <c r="D18" s="17"/>
+      <c r="E18" s="17"/>
+      <c r="F18" s="17"/>
+      <c r="G18" s="17"/>
+      <c r="H18" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -3804,11 +3850,147 @@
     <mergeCell ref="A15:A17"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G4 G9">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G4 G9 G12 G13 G15 G16">
       <formula1>"未进行,进行中,已暂停,已完成"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:H17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelCol="7"/>
+  <cols>
+    <col min="2" max="2" width="25.3173076923077" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B1" s="2">
+        <v>20220701</v>
+      </c>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="12"/>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B2" s="5">
+        <v>20220731</v>
+      </c>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="14"/>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="B4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="9"/>
+      <c r="B5" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" s="9"/>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" s="9"/>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" s="10"/>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" s="8" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10" s="9"/>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11" s="10"/>
+    </row>
+    <row r="12" spans="1:1">
+      <c r="A12" s="8" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1">
+      <c r="A13" s="9"/>
+    </row>
+    <row r="14" spans="1:1">
+      <c r="A14" s="10"/>
+    </row>
+    <row r="15" spans="1:1">
+      <c r="A15" s="8" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1">
+      <c r="A16" s="9"/>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" s="10"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A4:A8"/>
+    <mergeCell ref="A9:A11"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="A15:A17"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Site updated: 2022-11-03 20:31:59
</commit_message>
<xml_diff>
--- a/file/personal/roleImportant/角色要事记录表_2022.xlsx
+++ b/file/personal/roleImportant/角色要事记录表_2022.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="16360" activeTab="5"/>
+    <workbookView windowHeight="16860" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="角色目录" sheetId="2" r:id="rId1"/>
@@ -13,13 +13,15 @@
     <sheet name="五月" sheetId="11" r:id="rId4"/>
     <sheet name="六月" sheetId="12" r:id="rId5"/>
     <sheet name="七月" sheetId="13" r:id="rId6"/>
+    <sheet name="八月" sheetId="14" r:id="rId7"/>
+    <sheet name="九月" sheetId="16" r:id="rId8"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119">
   <si>
     <t>角色</t>
   </si>
@@ -301,6 +303,81 @@
   </si>
   <si>
     <t>feign+ribbon+eureka整理完成</t>
+  </si>
+  <si>
+    <t>面试资料再过一遍并筛选重点记忆内容</t>
+  </si>
+  <si>
+    <t>mybatis常见面试题整理</t>
+  </si>
+  <si>
+    <t>ES常见面试题整理</t>
+  </si>
+  <si>
+    <t>重要知识点过两遍</t>
+  </si>
+  <si>
+    <t>整体知识点过一遍</t>
+  </si>
+  <si>
+    <t>自己意愿不够强，没有动力去做</t>
+  </si>
+  <si>
+    <t>尝试投递6家公司</t>
+  </si>
+  <si>
+    <t>七夕节礼物</t>
+  </si>
+  <si>
+    <t>中午请闯闯吃个饭</t>
+  </si>
+  <si>
+    <t>Mq知识点补充整理</t>
+  </si>
+  <si>
+    <t>未能长期坚持</t>
+  </si>
+  <si>
+    <t>整体知识过一遍</t>
+  </si>
+  <si>
+    <t>刷20道面试题</t>
+  </si>
+  <si>
+    <t>刷10道面试题</t>
+  </si>
+  <si>
+    <t>刷30道面试题</t>
+  </si>
+  <si>
+    <t>复盘面试经验</t>
+  </si>
+  <si>
+    <t>第五周</t>
+  </si>
+  <si>
+    <t>重要知识过一遍</t>
+  </si>
+  <si>
+    <t>广度：刷题20</t>
+  </si>
+  <si>
+    <t>深度：rabbitmq客户端源码初步了解</t>
+  </si>
+  <si>
+    <t>温习一半知识点</t>
+  </si>
+  <si>
+    <t>投递公司3家</t>
+  </si>
+  <si>
+    <t>了解江苏考公基本情况</t>
+  </si>
+  <si>
+    <t>深度：rabbitmq客户端源码完全掌握</t>
+  </si>
+  <si>
+    <t>考公计划制定</t>
   </si>
 </sst>
 </file>
@@ -308,15 +385,21 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
+      <name val="SimSun"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="SimSun"/>
       <charset val="134"/>
     </font>
@@ -335,34 +418,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
       <color theme="3"/>
       <name val="Helvetica Neue"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -381,8 +441,30 @@
     </font>
     <font>
       <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Helvetica Neue"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF006100"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -390,17 +472,9 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Helvetica Neue"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Helvetica Neue"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -419,24 +493,17 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="1"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <u/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF0000FF"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -449,11 +516,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="Helvetica Neue"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -462,6 +529,22 @@
       <color theme="3"/>
       <name val="Helvetica Neue"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -493,12 +576,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="25"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.6"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -506,6 +583,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="25"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -560,13 +643,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -578,25 +661,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -608,7 +679,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -626,6 +703,24 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -638,7 +733,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -650,25 +763,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -680,61 +817,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -850,6 +933,21 @@
     </border>
     <border>
       <left style="thin">
+        <color indexed="13"/>
+      </left>
+      <right style="thin">
+        <color indexed="13"/>
+      </right>
+      <top style="thin">
+        <color indexed="18"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="13"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color indexed="17"/>
       </left>
       <right style="thin">
@@ -890,21 +988,6 @@
       </top>
       <bottom style="thin">
         <color indexed="17"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="13"/>
-      </left>
-      <right style="thin">
-        <color indexed="13"/>
-      </right>
-      <top style="thin">
-        <color indexed="18"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="13"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1055,11 +1138,9 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1069,21 +1150,6 @@
       <top/>
       <bottom style="medium">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1118,6 +1184,32 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -1132,166 +1224,157 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="43" borderId="30" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="42" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="41" borderId="29" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="30" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="43" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="22" borderId="29" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="28" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="27" borderId="27" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="26" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="25" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="34" borderId="29" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="25" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="24" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="25" borderId="28" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="27" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="25" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="26" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="25" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="30" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1319,37 +1402,49 @@
     <xf numFmtId="49" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -1370,10 +1465,7 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -1397,19 +1489,19 @@
     <xf numFmtId="49" fontId="0" fillId="10" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1551,11 +1643,6 @@
       <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -2624,11 +2711,12 @@
       </a:style>
     </a:txDef>
   </a:objectDefaults>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
   <dimension ref="A1:E23"/>
   <sheetViews>
@@ -2636,210 +2724,210 @@
       <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.90384615384615" defaultRowHeight="13.5" customHeight="1" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9.64285714285714" defaultRowHeight="13.5" customHeight="1" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="9" style="20" customWidth="1"/>
-    <col min="2" max="16384" width="6" style="20" customWidth="1"/>
+    <col min="1" max="1" width="9" style="24" customWidth="1"/>
+    <col min="2" max="16384" width="6" style="24" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="14" customHeight="1" spans="1:5">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
+      <c r="B1" s="44"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
     </row>
     <row r="2" ht="14" customHeight="1" spans="1:5">
-      <c r="A2" s="43" t="s">
+      <c r="A2" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="41"/>
-      <c r="C2" s="42"/>
-      <c r="D2" s="42"/>
-      <c r="E2" s="42"/>
+      <c r="B2" s="44"/>
+      <c r="C2" s="45"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="45"/>
     </row>
     <row r="3" ht="14" customHeight="1" spans="1:5">
-      <c r="A3" s="43" t="s">
+      <c r="A3" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="41"/>
-      <c r="C3" s="42"/>
-      <c r="D3" s="42"/>
-      <c r="E3" s="42"/>
+      <c r="B3" s="44"/>
+      <c r="C3" s="45"/>
+      <c r="D3" s="45"/>
+      <c r="E3" s="45"/>
     </row>
     <row r="4" ht="14" customHeight="1" spans="1:5">
-      <c r="A4" s="44" t="s">
+      <c r="A4" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="41"/>
-      <c r="C4" s="42"/>
-      <c r="D4" s="42"/>
-      <c r="E4" s="42"/>
+      <c r="B4" s="44"/>
+      <c r="C4" s="45"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
     </row>
     <row r="5" ht="14" customHeight="1" spans="1:5">
-      <c r="A5" s="45"/>
-      <c r="B5" s="41"/>
-      <c r="C5" s="42"/>
-      <c r="D5" s="42"/>
-      <c r="E5" s="42"/>
+      <c r="A5" s="48"/>
+      <c r="B5" s="44"/>
+      <c r="C5" s="45"/>
+      <c r="D5" s="45"/>
+      <c r="E5" s="45"/>
     </row>
     <row r="6" ht="14" customHeight="1" spans="1:5">
-      <c r="A6" s="45"/>
-      <c r="B6" s="41"/>
-      <c r="C6" s="42"/>
-      <c r="D6" s="42"/>
-      <c r="E6" s="42"/>
+      <c r="A6" s="48"/>
+      <c r="B6" s="44"/>
+      <c r="C6" s="45"/>
+      <c r="D6" s="45"/>
+      <c r="E6" s="45"/>
     </row>
     <row r="7" ht="14" customHeight="1" spans="1:5">
-      <c r="A7" s="44" t="s">
+      <c r="A7" s="47" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="41"/>
-      <c r="C7" s="42"/>
-      <c r="D7" s="42"/>
-      <c r="E7" s="42"/>
+      <c r="B7" s="44"/>
+      <c r="C7" s="45"/>
+      <c r="D7" s="45"/>
+      <c r="E7" s="45"/>
     </row>
     <row r="8" ht="14" customHeight="1" spans="1:5">
-      <c r="A8" s="45"/>
-      <c r="B8" s="41"/>
-      <c r="C8" s="42"/>
-      <c r="D8" s="42"/>
-      <c r="E8" s="42"/>
+      <c r="A8" s="48"/>
+      <c r="B8" s="44"/>
+      <c r="C8" s="45"/>
+      <c r="D8" s="45"/>
+      <c r="E8" s="45"/>
     </row>
     <row r="9" ht="14" customHeight="1" spans="1:5">
-      <c r="A9" s="45"/>
-      <c r="B9" s="41"/>
-      <c r="C9" s="42"/>
-      <c r="D9" s="42"/>
-      <c r="E9" s="42"/>
+      <c r="A9" s="48"/>
+      <c r="B9" s="44"/>
+      <c r="C9" s="45"/>
+      <c r="D9" s="45"/>
+      <c r="E9" s="45"/>
     </row>
     <row r="10" ht="14" customHeight="1" spans="1:5">
-      <c r="A10" s="44" t="s">
+      <c r="A10" s="47" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="41"/>
-      <c r="C10" s="42"/>
-      <c r="D10" s="42"/>
-      <c r="E10" s="42"/>
+      <c r="B10" s="44"/>
+      <c r="C10" s="45"/>
+      <c r="D10" s="45"/>
+      <c r="E10" s="45"/>
     </row>
     <row r="11" ht="14" customHeight="1" spans="1:5">
-      <c r="A11" s="44" t="s">
+      <c r="A11" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="41"/>
-      <c r="C11" s="42"/>
-      <c r="D11" s="42"/>
-      <c r="E11" s="42"/>
+      <c r="B11" s="44"/>
+      <c r="C11" s="45"/>
+      <c r="D11" s="45"/>
+      <c r="E11" s="45"/>
     </row>
     <row r="12" ht="14" customHeight="1" spans="1:5">
-      <c r="A12" s="44" t="s">
+      <c r="A12" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="B12" s="41"/>
-      <c r="C12" s="42"/>
-      <c r="D12" s="42"/>
-      <c r="E12" s="42"/>
+      <c r="B12" s="44"/>
+      <c r="C12" s="45"/>
+      <c r="D12" s="45"/>
+      <c r="E12" s="45"/>
     </row>
     <row r="13" ht="14" customHeight="1" spans="1:5">
-      <c r="A13" s="44" t="s">
+      <c r="A13" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="B13" s="41"/>
-      <c r="C13" s="42"/>
-      <c r="D13" s="42"/>
-      <c r="E13" s="42"/>
+      <c r="B13" s="44"/>
+      <c r="C13" s="45"/>
+      <c r="D13" s="45"/>
+      <c r="E13" s="45"/>
     </row>
     <row r="14" ht="14" customHeight="1" spans="1:5">
-      <c r="A14" s="44" t="s">
+      <c r="A14" s="47" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="41"/>
-      <c r="C14" s="42"/>
-      <c r="D14" s="42"/>
-      <c r="E14" s="42"/>
+      <c r="B14" s="44"/>
+      <c r="C14" s="45"/>
+      <c r="D14" s="45"/>
+      <c r="E14" s="45"/>
     </row>
     <row r="15" ht="14" customHeight="1" spans="1:5">
-      <c r="A15" s="44" t="s">
+      <c r="A15" s="47" t="s">
         <v>10</v>
       </c>
-      <c r="B15" s="41"/>
-      <c r="C15" s="42"/>
-      <c r="D15" s="42"/>
-      <c r="E15" s="42"/>
+      <c r="B15" s="44"/>
+      <c r="C15" s="45"/>
+      <c r="D15" s="45"/>
+      <c r="E15" s="45"/>
     </row>
     <row r="16" ht="14" customHeight="1" spans="1:5">
-      <c r="A16" s="44" t="s">
+      <c r="A16" s="47" t="s">
         <v>11</v>
       </c>
-      <c r="B16" s="41"/>
-      <c r="C16" s="42"/>
-      <c r="D16" s="42"/>
-      <c r="E16" s="42"/>
+      <c r="B16" s="44"/>
+      <c r="C16" s="45"/>
+      <c r="D16" s="45"/>
+      <c r="E16" s="45"/>
     </row>
     <row r="17" ht="14" customHeight="1" spans="1:5">
-      <c r="A17" s="44" t="s">
+      <c r="A17" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="B17" s="41"/>
-      <c r="C17" s="42"/>
-      <c r="D17" s="42"/>
-      <c r="E17" s="42"/>
+      <c r="B17" s="44"/>
+      <c r="C17" s="45"/>
+      <c r="D17" s="45"/>
+      <c r="E17" s="45"/>
     </row>
     <row r="18" ht="14" customHeight="1" spans="1:5">
-      <c r="A18" s="44" t="s">
+      <c r="A18" s="47" t="s">
         <v>13</v>
       </c>
-      <c r="B18" s="41"/>
-      <c r="C18" s="42"/>
-      <c r="D18" s="42"/>
-      <c r="E18" s="42"/>
+      <c r="B18" s="44"/>
+      <c r="C18" s="45"/>
+      <c r="D18" s="45"/>
+      <c r="E18" s="45"/>
     </row>
     <row r="19" ht="14" customHeight="1" spans="1:5">
-      <c r="A19" s="44" t="s">
+      <c r="A19" s="47" t="s">
         <v>14</v>
       </c>
-      <c r="B19" s="41"/>
-      <c r="C19" s="42"/>
-      <c r="D19" s="42"/>
-      <c r="E19" s="42"/>
+      <c r="B19" s="44"/>
+      <c r="C19" s="45"/>
+      <c r="D19" s="45"/>
+      <c r="E19" s="45"/>
     </row>
     <row r="20" ht="14" customHeight="1" spans="1:5">
-      <c r="A20" s="44" t="s">
+      <c r="A20" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="B20" s="41"/>
-      <c r="C20" s="42"/>
-      <c r="D20" s="42"/>
-      <c r="E20" s="42"/>
+      <c r="B20" s="44"/>
+      <c r="C20" s="45"/>
+      <c r="D20" s="45"/>
+      <c r="E20" s="45"/>
     </row>
     <row r="21" ht="14" customHeight="1" spans="1:5">
-      <c r="A21" s="44" t="s">
+      <c r="A21" s="47" t="s">
         <v>16</v>
       </c>
-      <c r="B21" s="41"/>
-      <c r="C21" s="42"/>
-      <c r="D21" s="42"/>
-      <c r="E21" s="42"/>
+      <c r="B21" s="44"/>
+      <c r="C21" s="45"/>
+      <c r="D21" s="45"/>
+      <c r="E21" s="45"/>
     </row>
     <row r="22" ht="14" customHeight="1" spans="1:5">
-      <c r="A22" s="44" t="s">
+      <c r="A22" s="47" t="s">
         <v>17</v>
       </c>
-      <c r="B22" s="41"/>
-      <c r="C22" s="42"/>
-      <c r="D22" s="42"/>
-      <c r="E22" s="42"/>
+      <c r="B22" s="44"/>
+      <c r="C22" s="45"/>
+      <c r="D22" s="45"/>
+      <c r="E22" s="45"/>
     </row>
     <row r="23" ht="14" customHeight="1" spans="1:5">
-      <c r="A23" s="43" t="s">
+      <c r="A23" s="46" t="s">
         <v>18</v>
       </c>
-      <c r="B23" s="41"/>
-      <c r="C23" s="42"/>
-      <c r="D23" s="42"/>
-      <c r="E23" s="42"/>
+      <c r="B23" s="44"/>
+      <c r="C23" s="45"/>
+      <c r="D23" s="45"/>
+      <c r="E23" s="45"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2855,7 +2943,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -2869,243 +2957,243 @@
       <selection pane="bottomRight" activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.90384615384615" defaultRowHeight="13" customHeight="1" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9.64285714285714" defaultRowHeight="13" customHeight="1" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="1" width="16.3557692307692" style="20" customWidth="1"/>
-    <col min="2" max="2" width="99.1153846153846" style="28" customWidth="1"/>
-    <col min="3" max="16384" width="16.3557692307692" style="20" customWidth="1"/>
+    <col min="1" max="1" width="16.3571428571429" style="24" customWidth="1"/>
+    <col min="2" max="2" width="99.1160714285714" style="31" customWidth="1"/>
+    <col min="3" max="16384" width="16.3571428571429" style="24" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.55" customHeight="1" spans="1:3">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="30" t="s">
+      <c r="B1" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="31" t="s">
+      <c r="C1" s="34" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="2" ht="13.55" customHeight="1" spans="1:3">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="33" t="s">
+      <c r="B2" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="18" t="s">
+      <c r="C2" s="15" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="3" ht="13.35" customHeight="1" spans="1:3">
-      <c r="A3" s="34" t="s">
+      <c r="A3" s="37" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="35" t="s">
+      <c r="B3" s="38" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="18" t="s">
+      <c r="C3" s="15" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="4" ht="13.35" customHeight="1" spans="1:3">
-      <c r="A4" s="36" t="s">
+      <c r="A4" s="39" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="35" t="s">
+      <c r="B4" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="C4" s="37" t="s">
+      <c r="C4" s="40" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="5" ht="13.35" customHeight="1" spans="1:3">
-      <c r="A5" s="36" t="s">
+      <c r="A5" s="39" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="35" t="s">
+      <c r="B5" s="38" t="s">
         <v>31</v>
       </c>
-      <c r="C5" s="37" t="s">
+      <c r="C5" s="40" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="6" ht="13.35" customHeight="1" spans="1:3">
-      <c r="A6" s="36" t="s">
+      <c r="A6" s="39" t="s">
         <v>32</v>
       </c>
-      <c r="B6" s="38"/>
-      <c r="C6" s="37" t="s">
+      <c r="B6" s="41"/>
+      <c r="C6" s="40" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="7" ht="13.35" customHeight="1" spans="1:3">
-      <c r="A7" s="36" t="s">
+      <c r="A7" s="39" t="s">
         <v>33</v>
       </c>
-      <c r="B7" s="38"/>
-      <c r="C7" s="37" t="s">
+      <c r="B7" s="41"/>
+      <c r="C7" s="40" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="8" ht="13.35" customHeight="1" spans="1:3">
-      <c r="A8" s="36" t="s">
+      <c r="A8" s="39" t="s">
         <v>34</v>
       </c>
-      <c r="B8" s="38"/>
-      <c r="C8" s="18" t="s">
+      <c r="B8" s="41"/>
+      <c r="C8" s="15" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="9" ht="13.35" customHeight="1" spans="1:3">
-      <c r="A9" s="36" t="s">
+      <c r="A9" s="39" t="s">
         <v>35</v>
       </c>
-      <c r="B9" s="35" t="s">
+      <c r="B9" s="38" t="s">
         <v>36</v>
       </c>
-      <c r="C9" s="18" t="s">
+      <c r="C9" s="15" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="10" ht="13.35" customHeight="1" spans="1:3">
-      <c r="A10" s="36" t="s">
+      <c r="A10" s="39" t="s">
         <v>37</v>
       </c>
-      <c r="B10" s="35" t="s">
+      <c r="B10" s="38" t="s">
         <v>38</v>
       </c>
-      <c r="C10" s="37" t="s">
+      <c r="C10" s="40" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="11" ht="13.35" customHeight="1" spans="1:3">
-      <c r="A11" s="34" t="s">
+      <c r="A11" s="37" t="s">
         <v>39</v>
       </c>
-      <c r="B11" s="35" t="s">
+      <c r="B11" s="38" t="s">
         <v>40</v>
       </c>
-      <c r="C11" s="39" t="s">
+      <c r="C11" s="42" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="12" ht="13.35" customHeight="1" spans="1:3">
-      <c r="A12" s="36" t="s">
+      <c r="A12" s="39" t="s">
         <v>42</v>
       </c>
-      <c r="B12" s="35" t="s">
+      <c r="B12" s="38" t="s">
         <v>43</v>
       </c>
-      <c r="C12" s="37" t="s">
+      <c r="C12" s="40" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="13" ht="13.35" customHeight="1" spans="1:3">
-      <c r="A13" s="36" t="s">
+      <c r="A13" s="39" t="s">
         <v>44</v>
       </c>
-      <c r="B13" s="35" t="s">
+      <c r="B13" s="38" t="s">
         <v>45</v>
       </c>
-      <c r="C13" s="37" t="s">
+      <c r="C13" s="40" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="14" ht="13.35" customHeight="1" spans="1:3">
-      <c r="A14" s="34" t="s">
+      <c r="A14" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="B14" s="35" t="s">
+      <c r="B14" s="38" t="s">
         <v>47</v>
       </c>
-      <c r="C14" s="39" t="s">
+      <c r="C14" s="42" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="15" ht="13.35" customHeight="1" spans="1:3">
-      <c r="A15" s="34" t="s">
+      <c r="A15" s="37" t="s">
         <v>48</v>
       </c>
-      <c r="B15" s="35" t="s">
+      <c r="B15" s="38" t="s">
         <v>49</v>
       </c>
-      <c r="C15" s="18" t="s">
+      <c r="C15" s="15" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="16" ht="13.35" customHeight="1" spans="1:3">
-      <c r="A16" s="34" t="s">
+      <c r="A16" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="B16" s="35" t="s">
+      <c r="B16" s="38" t="s">
         <v>51</v>
       </c>
-      <c r="C16" s="39" t="s">
+      <c r="C16" s="42" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="17" ht="13.35" customHeight="1" spans="1:3">
-      <c r="A17" s="34" t="s">
+      <c r="A17" s="37" t="s">
         <v>52</v>
       </c>
-      <c r="B17" s="35" t="s">
+      <c r="B17" s="38" t="s">
         <v>53</v>
       </c>
-      <c r="C17" s="37" t="s">
+      <c r="C17" s="40" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="18" ht="13.35" customHeight="1" spans="1:3">
-      <c r="A18" s="40" t="s">
+      <c r="A18" s="43" t="s">
         <v>54</v>
       </c>
-      <c r="B18" s="17" t="s">
+      <c r="B18" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="C18" s="17"/>
+      <c r="C18" s="22"/>
     </row>
     <row r="19" customHeight="1" spans="1:2">
-      <c r="A19" s="20" t="s">
+      <c r="A19" s="24" t="s">
         <v>56</v>
       </c>
-      <c r="B19" s="28" t="s">
+      <c r="B19" s="31" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="20" customHeight="1" spans="1:2">
-      <c r="A20" s="20" t="s">
+      <c r="A20" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="B20" s="28" t="s">
+      <c r="B20" s="31" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="21" customHeight="1" spans="1:2">
-      <c r="A21" s="20" t="s">
+      <c r="A21" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="B21" s="28" t="s">
+      <c r="B21" s="31" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="22" customHeight="1" spans="1:2">
-      <c r="A22" s="20" t="s">
+      <c r="A22" s="24" t="s">
         <v>61</v>
       </c>
-      <c r="B22" s="28" t="s">
+      <c r="B22" s="31" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="23" customHeight="1" spans="1:3">
-      <c r="A23" s="20" t="s">
+      <c r="A23" s="24" t="s">
         <v>63</v>
       </c>
-      <c r="B23" s="28" t="s">
+      <c r="B23" s="31" t="s">
         <v>64</v>
       </c>
-      <c r="C23" s="18" t="s">
+      <c r="C23" s="15" t="s">
         <v>24</v>
       </c>
     </row>
@@ -3124,7 +3212,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -3136,9 +3224,9 @@
       <selection pane="topRight" activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.90384615384615" defaultRowHeight="13" customHeight="1" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="9.64285714285714" defaultRowHeight="13" customHeight="1" outlineLevelCol="7"/>
   <cols>
-    <col min="1" max="16384" width="16.3557692307692" style="20" customWidth="1"/>
+    <col min="1" max="16384" width="16.3571428571429" style="24" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="14" customHeight="1" spans="1:8">
@@ -3199,180 +3287,180 @@
       <c r="A4" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="C4" s="21"/>
-      <c r="D4" s="21"/>
-      <c r="E4" s="21"/>
-      <c r="F4" s="21"/>
-      <c r="G4" s="21"/>
-      <c r="H4" s="21"/>
+      <c r="C4" s="25"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="25"/>
+      <c r="F4" s="25"/>
+      <c r="G4" s="25"/>
+      <c r="H4" s="25"/>
     </row>
     <row r="5" ht="13.35" customHeight="1" spans="1:8">
-      <c r="A5" s="9"/>
-      <c r="B5" s="22"/>
-      <c r="C5" s="17"/>
-      <c r="D5" s="17"/>
-      <c r="E5" s="17" t="s">
+      <c r="A5" s="17"/>
+      <c r="B5" s="26"/>
+      <c r="C5" s="22"/>
+      <c r="D5" s="22"/>
+      <c r="E5" s="22" t="s">
         <v>71</v>
       </c>
-      <c r="F5" s="17"/>
-      <c r="G5" s="18" t="s">
+      <c r="F5" s="22"/>
+      <c r="G5" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="H5" s="17"/>
+      <c r="H5" s="22"/>
     </row>
     <row r="6" ht="13.35" customHeight="1" spans="1:8">
-      <c r="A6" s="9"/>
-      <c r="B6" s="23"/>
-      <c r="C6" s="17"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17" t="s">
+      <c r="A6" s="17"/>
+      <c r="B6" s="27"/>
+      <c r="C6" s="22"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="22" t="s">
         <v>72</v>
       </c>
-      <c r="F6" s="17"/>
-      <c r="G6" s="18" t="s">
+      <c r="F6" s="22"/>
+      <c r="G6" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="H6" s="17"/>
+      <c r="H6" s="22"/>
     </row>
     <row r="7" ht="13.35" customHeight="1" spans="1:8">
-      <c r="A7" s="9"/>
-      <c r="B7" s="23" t="s">
+      <c r="A7" s="17"/>
+      <c r="B7" s="27" t="s">
         <v>73</v>
       </c>
-      <c r="C7" s="17"/>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="17"/>
-      <c r="G7" s="18" t="s">
+      <c r="C7" s="22"/>
+      <c r="D7" s="22"/>
+      <c r="E7" s="22"/>
+      <c r="F7" s="22"/>
+      <c r="G7" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="H7" s="17"/>
+      <c r="H7" s="22"/>
     </row>
     <row r="8" ht="13.65" customHeight="1" spans="1:8">
-      <c r="A8" s="10"/>
-      <c r="B8" s="23"/>
-      <c r="C8" s="17"/>
-      <c r="D8" s="17"/>
-      <c r="E8" s="17"/>
-      <c r="F8" s="17"/>
-      <c r="G8" s="17"/>
-      <c r="H8" s="17"/>
+      <c r="A8" s="18"/>
+      <c r="B8" s="27"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="22"/>
+      <c r="E8" s="22"/>
+      <c r="F8" s="22"/>
+      <c r="G8" s="22"/>
+      <c r="H8" s="22"/>
     </row>
     <row r="9" ht="13.65" customHeight="1" spans="1:8">
       <c r="A9" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="B9" s="22"/>
-      <c r="C9" s="17"/>
-      <c r="D9" s="17"/>
-      <c r="E9" s="17"/>
-      <c r="F9" s="17"/>
-      <c r="G9" s="17"/>
-      <c r="H9" s="17"/>
+      <c r="B9" s="26"/>
+      <c r="C9" s="22"/>
+      <c r="D9" s="22"/>
+      <c r="E9" s="22"/>
+      <c r="F9" s="22"/>
+      <c r="G9" s="22"/>
+      <c r="H9" s="22"/>
     </row>
     <row r="10" ht="13.35" customHeight="1" spans="1:8">
-      <c r="A10" s="9"/>
-      <c r="B10" s="23"/>
-      <c r="C10" s="17"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="17"/>
-      <c r="G10" s="17"/>
-      <c r="H10" s="17"/>
+      <c r="A10" s="17"/>
+      <c r="B10" s="27"/>
+      <c r="C10" s="22"/>
+      <c r="D10" s="22"/>
+      <c r="E10" s="22"/>
+      <c r="F10" s="22"/>
+      <c r="G10" s="22"/>
+      <c r="H10" s="22"/>
     </row>
     <row r="11" ht="13.65" customHeight="1" spans="1:8">
-      <c r="A11" s="10"/>
-      <c r="B11" s="23"/>
-      <c r="C11" s="17"/>
-      <c r="D11" s="17"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="17"/>
-      <c r="G11" s="17"/>
-      <c r="H11" s="17"/>
+      <c r="A11" s="18"/>
+      <c r="B11" s="27"/>
+      <c r="C11" s="22"/>
+      <c r="D11" s="22"/>
+      <c r="E11" s="22"/>
+      <c r="F11" s="22"/>
+      <c r="G11" s="22"/>
+      <c r="H11" s="22"/>
     </row>
     <row r="12" ht="13.65" customHeight="1" spans="1:8">
       <c r="A12" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="B12" s="24" t="s">
+      <c r="B12" s="28" t="s">
         <v>76</v>
       </c>
-      <c r="C12" s="17"/>
-      <c r="D12" s="17"/>
-      <c r="E12" s="17"/>
-      <c r="F12" s="17"/>
-      <c r="G12" s="26" t="s">
+      <c r="C12" s="22"/>
+      <c r="D12" s="22"/>
+      <c r="E12" s="22"/>
+      <c r="F12" s="22"/>
+      <c r="G12" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="H12" s="17"/>
+      <c r="H12" s="22"/>
     </row>
     <row r="13" ht="13.65" customHeight="1" spans="1:8">
-      <c r="A13" s="9"/>
-      <c r="B13" s="23"/>
-      <c r="C13" s="17" t="s">
+      <c r="A13" s="17"/>
+      <c r="B13" s="27"/>
+      <c r="C13" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="D13" s="17"/>
-      <c r="E13" s="17"/>
-      <c r="F13" s="17"/>
-      <c r="G13" s="27" t="s">
+      <c r="D13" s="22"/>
+      <c r="E13" s="22"/>
+      <c r="F13" s="22"/>
+      <c r="G13" s="19" t="s">
         <v>77</v>
       </c>
-      <c r="H13" s="17" t="s">
+      <c r="H13" s="22" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="14" ht="14" customHeight="1" spans="1:8">
-      <c r="A14" s="10"/>
-      <c r="B14" s="23"/>
-      <c r="C14" s="17"/>
-      <c r="D14" s="17"/>
-      <c r="E14" s="17"/>
-      <c r="F14" s="17"/>
-      <c r="G14" s="17"/>
-      <c r="H14" s="17"/>
+      <c r="A14" s="18"/>
+      <c r="B14" s="27"/>
+      <c r="C14" s="22"/>
+      <c r="D14" s="22"/>
+      <c r="E14" s="22"/>
+      <c r="F14" s="22"/>
+      <c r="G14" s="22"/>
+      <c r="H14" s="22"/>
     </row>
     <row r="15" ht="13.65" customHeight="1" spans="1:8">
       <c r="A15" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="B15" s="22"/>
-      <c r="C15" s="17"/>
-      <c r="D15" s="17"/>
-      <c r="E15" s="17"/>
-      <c r="F15" s="17"/>
-      <c r="G15" s="17"/>
-      <c r="H15" s="17"/>
+      <c r="B15" s="26"/>
+      <c r="C15" s="22"/>
+      <c r="D15" s="22"/>
+      <c r="E15" s="22"/>
+      <c r="F15" s="22"/>
+      <c r="G15" s="22"/>
+      <c r="H15" s="22"/>
     </row>
     <row r="16" ht="13.35" customHeight="1" spans="1:8">
-      <c r="A16" s="9"/>
-      <c r="B16" s="22"/>
-      <c r="C16" s="17"/>
-      <c r="D16" s="17"/>
-      <c r="E16" s="17"/>
-      <c r="F16" s="17"/>
-      <c r="G16" s="17"/>
-      <c r="H16" s="17"/>
+      <c r="A16" s="17"/>
+      <c r="B16" s="26"/>
+      <c r="C16" s="22"/>
+      <c r="D16" s="22"/>
+      <c r="E16" s="22"/>
+      <c r="F16" s="22"/>
+      <c r="G16" s="22"/>
+      <c r="H16" s="22"/>
     </row>
     <row r="17" ht="13.65" customHeight="1" spans="1:8">
-      <c r="A17" s="10"/>
-      <c r="B17" s="23"/>
-      <c r="C17" s="17"/>
-      <c r="D17" s="17"/>
-      <c r="E17" s="17"/>
-      <c r="F17" s="17"/>
-      <c r="G17" s="17"/>
-      <c r="H17" s="17"/>
+      <c r="A17" s="18"/>
+      <c r="B17" s="27"/>
+      <c r="C17" s="22"/>
+      <c r="D17" s="22"/>
+      <c r="E17" s="22"/>
+      <c r="F17" s="22"/>
+      <c r="G17" s="22"/>
+      <c r="H17" s="22"/>
     </row>
     <row r="18" ht="13.65" customHeight="1" spans="1:8">
-      <c r="A18" s="15"/>
-      <c r="B18" s="16"/>
-      <c r="C18" s="17"/>
-      <c r="D18" s="17"/>
-      <c r="E18" s="17"/>
-      <c r="F18" s="17"/>
-      <c r="G18" s="17"/>
-      <c r="H18" s="17"/>
+      <c r="A18" s="20"/>
+      <c r="B18" s="21"/>
+      <c r="C18" s="22"/>
+      <c r="D18" s="22"/>
+      <c r="E18" s="22"/>
+      <c r="F18" s="22"/>
+      <c r="G18" s="22"/>
+      <c r="H18" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -3395,7 +3483,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
   <dimension ref="A1:H18"/>
   <sheetViews>
@@ -3403,13 +3491,13 @@
       <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.90384615384615" defaultRowHeight="16.8" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="9.64285714285714" defaultRowHeight="13.1" outlineLevelCol="7"/>
   <cols>
-    <col min="1" max="1" width="11.7307692307692" customWidth="1"/>
-    <col min="2" max="2" width="17.9711538461538" customWidth="1"/>
-    <col min="3" max="3" width="12.0288461538462" customWidth="1"/>
+    <col min="1" max="1" width="11.7321428571429" customWidth="1"/>
+    <col min="2" max="2" width="17.9732142857143" customWidth="1"/>
+    <col min="3" max="3" width="12.0267857142857" customWidth="1"/>
     <col min="4" max="4" width="15" customWidth="1"/>
-    <col min="8" max="8" width="15.4903846153846" customWidth="1"/>
+    <col min="8" max="8" width="15.4910714285714" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -3470,188 +3558,188 @@
       <c r="A4" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="B4" s="20" t="s">
+      <c r="B4" s="24" t="s">
         <v>80</v>
       </c>
-      <c r="C4" s="21"/>
-      <c r="D4" s="21"/>
-      <c r="E4" s="21"/>
-      <c r="F4" s="21"/>
-      <c r="G4" s="18" t="s">
+      <c r="C4" s="25"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="25"/>
+      <c r="F4" s="25"/>
+      <c r="G4" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="H4" s="21"/>
+      <c r="H4" s="25"/>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="9"/>
-      <c r="B5" s="22"/>
-      <c r="C5" s="17"/>
-      <c r="D5" s="17" t="s">
+      <c r="A5" s="17"/>
+      <c r="B5" s="26"/>
+      <c r="C5" s="22"/>
+      <c r="D5" s="22" t="s">
         <v>81</v>
       </c>
-      <c r="E5" s="17"/>
-      <c r="F5" s="17"/>
-      <c r="G5" s="18" t="s">
+      <c r="E5" s="22"/>
+      <c r="F5" s="22"/>
+      <c r="G5" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="H5" s="17"/>
+      <c r="H5" s="22"/>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="9"/>
-      <c r="B6" s="23"/>
-      <c r="C6" s="17" t="s">
+      <c r="A6" s="17"/>
+      <c r="B6" s="27"/>
+      <c r="C6" s="22" t="s">
         <v>82</v>
       </c>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="17"/>
-      <c r="G6" s="18" t="s">
+      <c r="D6" s="22"/>
+      <c r="E6" s="22"/>
+      <c r="F6" s="22"/>
+      <c r="G6" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="H6" s="17"/>
+      <c r="H6" s="22"/>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="9"/>
-      <c r="B7" s="23" t="s">
+      <c r="A7" s="17"/>
+      <c r="B7" s="27" t="s">
         <v>83</v>
       </c>
-      <c r="C7" s="17"/>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="17"/>
-      <c r="G7" s="18" t="s">
+      <c r="C7" s="22"/>
+      <c r="D7" s="22"/>
+      <c r="E7" s="22"/>
+      <c r="F7" s="22"/>
+      <c r="G7" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="H7" s="17"/>
+      <c r="H7" s="22"/>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="10"/>
-      <c r="B8" s="23"/>
-      <c r="C8" s="17"/>
-      <c r="D8" s="17"/>
-      <c r="E8" s="17"/>
-      <c r="F8" s="17"/>
-      <c r="H8" s="17"/>
+      <c r="A8" s="18"/>
+      <c r="B8" s="27"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="22"/>
+      <c r="E8" s="22"/>
+      <c r="F8" s="22"/>
+      <c r="H8" s="22"/>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="B9" s="22" t="s">
+      <c r="B9" s="26" t="s">
         <v>84</v>
       </c>
-      <c r="C9" s="17"/>
-      <c r="D9" s="17"/>
-      <c r="E9" s="17"/>
-      <c r="F9" s="17"/>
-      <c r="G9" s="25" t="s">
+      <c r="C9" s="22"/>
+      <c r="D9" s="22"/>
+      <c r="E9" s="22"/>
+      <c r="F9" s="22"/>
+      <c r="G9" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="H9" s="17"/>
+      <c r="H9" s="22"/>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="9"/>
-      <c r="B10" s="23" t="s">
+      <c r="A10" s="17"/>
+      <c r="B10" s="27" t="s">
         <v>85</v>
       </c>
-      <c r="C10" s="17"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="17"/>
-      <c r="G10" s="25" t="s">
+      <c r="C10" s="22"/>
+      <c r="D10" s="22"/>
+      <c r="E10" s="22"/>
+      <c r="F10" s="22"/>
+      <c r="G10" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="H10" s="17"/>
+      <c r="H10" s="22"/>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" s="10"/>
-      <c r="B11" s="23"/>
-      <c r="C11" s="17"/>
-      <c r="D11" s="17"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="17"/>
-      <c r="H11" s="17"/>
+      <c r="A11" s="18"/>
+      <c r="B11" s="27"/>
+      <c r="C11" s="22"/>
+      <c r="D11" s="22"/>
+      <c r="E11" s="22"/>
+      <c r="F11" s="22"/>
+      <c r="H11" s="22"/>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="B12" s="24" t="s">
+      <c r="B12" s="28" t="s">
         <v>86</v>
       </c>
-      <c r="C12" s="17"/>
-      <c r="D12" s="17"/>
-      <c r="E12" s="17"/>
-      <c r="F12" s="17"/>
-      <c r="G12" s="19" t="s">
+      <c r="C12" s="22"/>
+      <c r="D12" s="22"/>
+      <c r="E12" s="22"/>
+      <c r="F12" s="22"/>
+      <c r="G12" s="23" t="s">
         <v>87</v>
       </c>
-      <c r="H12" s="17"/>
+      <c r="H12" s="22"/>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" s="9"/>
-      <c r="B13" s="23"/>
-      <c r="C13" s="17"/>
-      <c r="D13" s="17"/>
-      <c r="E13" s="17"/>
-      <c r="F13" s="17"/>
-      <c r="H13" s="17"/>
+      <c r="A13" s="17"/>
+      <c r="B13" s="27"/>
+      <c r="C13" s="22"/>
+      <c r="D13" s="22"/>
+      <c r="E13" s="22"/>
+      <c r="F13" s="22"/>
+      <c r="H13" s="22"/>
     </row>
     <row r="14" spans="1:8">
-      <c r="A14" s="10"/>
-      <c r="B14" s="23"/>
-      <c r="C14" s="17"/>
-      <c r="D14" s="17"/>
-      <c r="E14" s="17"/>
-      <c r="F14" s="17"/>
-      <c r="G14" s="17"/>
-      <c r="H14" s="17"/>
+      <c r="A14" s="18"/>
+      <c r="B14" s="27"/>
+      <c r="C14" s="22"/>
+      <c r="D14" s="22"/>
+      <c r="E14" s="22"/>
+      <c r="F14" s="22"/>
+      <c r="G14" s="22"/>
+      <c r="H14" s="22"/>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="B15" s="22" t="s">
+      <c r="B15" s="26" t="s">
         <v>86</v>
       </c>
-      <c r="C15" s="17"/>
-      <c r="D15" s="17"/>
-      <c r="E15" s="17"/>
-      <c r="F15" s="17"/>
-      <c r="G15" s="19" t="s">
+      <c r="C15" s="22"/>
+      <c r="D15" s="22"/>
+      <c r="E15" s="22"/>
+      <c r="F15" s="22"/>
+      <c r="G15" s="23" t="s">
         <v>87</v>
       </c>
-      <c r="H15" s="17"/>
+      <c r="H15" s="22"/>
     </row>
     <row r="16" spans="1:8">
-      <c r="A16" s="9"/>
-      <c r="B16" s="22"/>
-      <c r="C16" s="17"/>
-      <c r="D16" s="17"/>
-      <c r="E16" s="17"/>
-      <c r="F16" s="17"/>
-      <c r="G16" s="17"/>
-      <c r="H16" s="17"/>
+      <c r="A16" s="17"/>
+      <c r="B16" s="26"/>
+      <c r="C16" s="22"/>
+      <c r="D16" s="22"/>
+      <c r="E16" s="22"/>
+      <c r="F16" s="22"/>
+      <c r="G16" s="22"/>
+      <c r="H16" s="22"/>
     </row>
     <row r="17" spans="1:8">
-      <c r="A17" s="10"/>
-      <c r="B17" s="23"/>
-      <c r="C17" s="17"/>
-      <c r="D17" s="17"/>
-      <c r="E17" s="17"/>
-      <c r="F17" s="17"/>
-      <c r="G17" s="17"/>
-      <c r="H17" s="17"/>
+      <c r="A17" s="18"/>
+      <c r="B17" s="27"/>
+      <c r="C17" s="22"/>
+      <c r="D17" s="22"/>
+      <c r="E17" s="22"/>
+      <c r="F17" s="22"/>
+      <c r="G17" s="22"/>
+      <c r="H17" s="22"/>
     </row>
     <row r="18" spans="1:8">
-      <c r="A18" s="15"/>
-      <c r="B18" s="16"/>
-      <c r="C18" s="17"/>
-      <c r="D18" s="17"/>
-      <c r="E18" s="17"/>
-      <c r="F18" s="17"/>
-      <c r="G18" s="17"/>
-      <c r="H18" s="17"/>
+      <c r="A18" s="20"/>
+      <c r="B18" s="21"/>
+      <c r="C18" s="22"/>
+      <c r="D18" s="22"/>
+      <c r="E18" s="22"/>
+      <c r="F18" s="22"/>
+      <c r="G18" s="22"/>
+      <c r="H18" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -3672,21 +3760,21 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
   <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.90384615384615" defaultRowHeight="16.8" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="9.64285714285714" defaultRowHeight="13.1" outlineLevelCol="7"/>
   <cols>
-    <col min="1" max="1" width="11.7307692307692" customWidth="1"/>
-    <col min="2" max="2" width="17.9711538461538" customWidth="1"/>
-    <col min="3" max="3" width="12.0288461538462" customWidth="1"/>
+    <col min="1" max="1" width="11.7321428571429" customWidth="1"/>
+    <col min="2" max="2" width="17.9732142857143" customWidth="1"/>
+    <col min="3" max="3" width="12.0267857142857" customWidth="1"/>
     <col min="4" max="4" width="15" customWidth="1"/>
-    <col min="8" max="8" width="15.4903846153846" customWidth="1"/>
+    <col min="8" max="8" width="15.4910714285714" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -3750,21 +3838,21 @@
       <c r="B4" t="s">
         <v>88</v>
       </c>
-      <c r="G4" s="18" t="s">
+      <c r="G4" s="15" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:1">
-      <c r="A5" s="9"/>
+      <c r="A5" s="17"/>
     </row>
     <row r="6" spans="1:1">
-      <c r="A6" s="9"/>
+      <c r="A6" s="17"/>
     </row>
     <row r="7" spans="1:1">
-      <c r="A7" s="9"/>
+      <c r="A7" s="17"/>
     </row>
     <row r="8" spans="1:1">
-      <c r="A8" s="10"/>
+      <c r="A8" s="18"/>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="8" t="s">
@@ -3773,15 +3861,15 @@
       <c r="B9" t="s">
         <v>88</v>
       </c>
-      <c r="G9" s="18" t="s">
+      <c r="G9" s="15" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:1">
-      <c r="A10" s="9"/>
+      <c r="A10" s="17"/>
     </row>
     <row r="11" spans="1:1">
-      <c r="A11" s="10"/>
+      <c r="A11" s="18"/>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="8" t="s">
@@ -3790,16 +3878,16 @@
       <c r="B12" t="s">
         <v>89</v>
       </c>
-      <c r="G12" s="18" t="s">
+      <c r="G12" s="15" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" s="9"/>
+      <c r="A13" s="17"/>
       <c r="B13" t="s">
         <v>90</v>
       </c>
-      <c r="G13" s="19" t="s">
+      <c r="G13" s="23" t="s">
         <v>87</v>
       </c>
       <c r="H13" t="s">
@@ -3807,7 +3895,7 @@
       </c>
     </row>
     <row r="14" spans="1:1">
-      <c r="A14" s="10"/>
+      <c r="A14" s="18"/>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="8" t="s">
@@ -3816,31 +3904,31 @@
       <c r="B15" t="s">
         <v>92</v>
       </c>
-      <c r="G15" s="19" t="s">
+      <c r="G15" s="23" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="16" spans="1:7">
-      <c r="A16" s="9"/>
+      <c r="A16" s="17"/>
       <c r="B16" t="s">
         <v>90</v>
       </c>
-      <c r="G16" s="19" t="s">
+      <c r="G16" s="23" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="17" spans="1:1">
-      <c r="A17" s="10"/>
+      <c r="A17" s="18"/>
     </row>
     <row r="18" spans="1:8">
-      <c r="A18" s="15"/>
-      <c r="B18" s="16"/>
-      <c r="C18" s="17"/>
-      <c r="D18" s="17"/>
-      <c r="E18" s="17"/>
-      <c r="F18" s="17"/>
-      <c r="G18" s="17"/>
-      <c r="H18" s="17"/>
+      <c r="A18" s="20"/>
+      <c r="B18" s="21"/>
+      <c r="C18" s="22"/>
+      <c r="D18" s="22"/>
+      <c r="E18" s="22"/>
+      <c r="F18" s="22"/>
+      <c r="G18" s="22"/>
+      <c r="H18" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -3860,17 +3948,17 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
   <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="9.64285714285714" defaultRowHeight="13.1" outlineLevelCol="7"/>
   <cols>
-    <col min="2" max="2" width="25.3173076923077" customWidth="1"/>
+    <col min="2" max="2" width="25.3214285714286" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -3927,39 +4015,63 @@
         <v>69</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:7">
       <c r="A4" s="8" t="s">
         <v>70</v>
       </c>
       <c r="B4" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="9"/>
+      <c r="G4" s="15" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="17"/>
       <c r="B5" t="s">
         <v>90</v>
       </c>
+      <c r="G5" s="15" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="6" spans="1:1">
-      <c r="A6" s="9"/>
+      <c r="A6" s="17"/>
     </row>
     <row r="7" spans="1:1">
-      <c r="A7" s="9"/>
+      <c r="A7" s="17"/>
     </row>
     <row r="8" spans="1:1">
-      <c r="A8" s="10"/>
-    </row>
-    <row r="9" spans="1:1">
+      <c r="A8" s="18"/>
+    </row>
+    <row r="9" spans="1:7">
       <c r="A9" s="8" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="10" spans="1:1">
-      <c r="A10" s="9"/>
-    </row>
-    <row r="11" spans="1:1">
-      <c r="A11" s="10"/>
+      <c r="B9" t="s">
+        <v>94</v>
+      </c>
+      <c r="G9" s="15" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="17"/>
+      <c r="B10" t="s">
+        <v>95</v>
+      </c>
+      <c r="G10" s="15" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" s="18"/>
+      <c r="B11" t="s">
+        <v>96</v>
+      </c>
+      <c r="G11" s="15" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" s="8" t="s">
@@ -3967,10 +4079,10 @@
       </c>
     </row>
     <row r="13" spans="1:1">
-      <c r="A13" s="9"/>
+      <c r="A13" s="17"/>
     </row>
     <row r="14" spans="1:1">
-      <c r="A14" s="10"/>
+      <c r="A14" s="18"/>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" s="8" t="s">
@@ -3978,10 +4090,10 @@
       </c>
     </row>
     <row r="16" spans="1:1">
-      <c r="A16" s="9"/>
+      <c r="A16" s="17"/>
     </row>
     <row r="17" spans="1:1">
-      <c r="A17" s="10"/>
+      <c r="A17" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -3990,6 +4102,553 @@
     <mergeCell ref="A12:A13"/>
     <mergeCell ref="A15:A17"/>
   </mergeCells>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G4 G5 G9 G10 G11">
+      <formula1>"未进行,进行中,已暂停,已完成"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
+  <dimension ref="A1:H27"/>
+  <sheetViews>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.64285714285714" defaultRowHeight="13.1" outlineLevelCol="7"/>
+  <cols>
+    <col min="2" max="2" width="20.0267857142857" customWidth="1"/>
+    <col min="4" max="4" width="13.2857142857143" customWidth="1"/>
+    <col min="5" max="5" width="9.77678571428571" customWidth="1"/>
+    <col min="6" max="6" width="19.5446428571429" customWidth="1"/>
+    <col min="8" max="8" width="19.8660714285714" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B1" s="2">
+        <v>20220801</v>
+      </c>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="12"/>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B2" s="5">
+        <v>20220831</v>
+      </c>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="14"/>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="B4" t="s">
+        <v>97</v>
+      </c>
+      <c r="G4" s="15" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="9"/>
+      <c r="B5" t="s">
+        <v>98</v>
+      </c>
+      <c r="G5" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="H5" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="9"/>
+      <c r="B6" t="s">
+        <v>100</v>
+      </c>
+      <c r="G6" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="H6" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="9"/>
+      <c r="D7" t="s">
+        <v>101</v>
+      </c>
+      <c r="G7" s="15" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="9"/>
+      <c r="F8" t="s">
+        <v>102</v>
+      </c>
+      <c r="G8" s="15" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="B9" t="s">
+        <v>103</v>
+      </c>
+      <c r="G9" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="H9" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="9"/>
+      <c r="B10" t="s">
+        <v>105</v>
+      </c>
+      <c r="G10" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="H10" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="10"/>
+      <c r="B11" t="s">
+        <v>100</v>
+      </c>
+      <c r="G11" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="H11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="9"/>
+      <c r="B12" t="s">
+        <v>106</v>
+      </c>
+      <c r="G12" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="H12" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="B13" t="s">
+        <v>103</v>
+      </c>
+      <c r="G13" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="H13" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" s="9"/>
+      <c r="B14" t="s">
+        <v>105</v>
+      </c>
+      <c r="G14" s="15" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" s="10"/>
+      <c r="B15" t="s">
+        <v>100</v>
+      </c>
+      <c r="G15" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="H15" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" s="9"/>
+      <c r="B16" t="s">
+        <v>107</v>
+      </c>
+      <c r="G16" s="15" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" s="9"/>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="B18" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="9"/>
+      <c r="B19" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="10"/>
+      <c r="B20" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="9"/>
+      <c r="B21" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" s="9"/>
+      <c r="B22" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="B23" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" s="17"/>
+      <c r="B24" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" s="17"/>
+      <c r="B25" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" s="17"/>
+      <c r="B26" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" s="18"/>
+      <c r="B27" t="s">
+        <v>109</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A4:A8"/>
+    <mergeCell ref="A9:A12"/>
+    <mergeCell ref="A13:A17"/>
+    <mergeCell ref="A18:A21"/>
+    <mergeCell ref="A23:A27"/>
+  </mergeCells>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G5 G6 G9 G10 G11 G12 G13 G15">
+      <formula1>"未进行,进行中,已暂停,已完成,未完成"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G4 G14 G16 G7:G8">
+      <formula1>"未进行,进行中,已暂停,已完成"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
+  <dimension ref="A1:H23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="B17" sqref="17:17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.64285714285714" defaultRowHeight="13.1" outlineLevelCol="7"/>
+  <cols>
+    <col min="2" max="2" width="20.0267857142857" customWidth="1"/>
+    <col min="4" max="4" width="13.2857142857143" customWidth="1"/>
+    <col min="5" max="5" width="9.77678571428571" customWidth="1"/>
+    <col min="6" max="6" width="19.5446428571429" customWidth="1"/>
+    <col min="8" max="8" width="19.8660714285714" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B1" s="2">
+        <v>20220901</v>
+      </c>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="12"/>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B2" s="5">
+        <v>20220930</v>
+      </c>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="14"/>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" s="8" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" s="9"/>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" s="9"/>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" s="9"/>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" s="9"/>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="B9" t="s">
+        <v>112</v>
+      </c>
+      <c r="G9" s="15" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="9"/>
+      <c r="B10" t="s">
+        <v>113</v>
+      </c>
+      <c r="G10" s="16" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" s="10"/>
+      <c r="B11" t="s">
+        <v>114</v>
+      </c>
+      <c r="G11" s="16" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" s="9"/>
+      <c r="B12" t="s">
+        <v>115</v>
+      </c>
+      <c r="G12" s="15" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" s="9"/>
+      <c r="C13" t="s">
+        <v>116</v>
+      </c>
+      <c r="G13" s="16" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="B14" t="s">
+        <v>112</v>
+      </c>
+      <c r="G14" s="15" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" s="9"/>
+      <c r="B15" t="s">
+        <v>113</v>
+      </c>
+      <c r="G15" s="15" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" s="10"/>
+      <c r="B16" t="s">
+        <v>114</v>
+      </c>
+      <c r="G16" s="16" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" s="9"/>
+      <c r="B17" t="s">
+        <v>115</v>
+      </c>
+      <c r="G17" s="15" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" s="9"/>
+      <c r="C18" t="s">
+        <v>116</v>
+      </c>
+      <c r="G18" s="16" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="B19" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="9"/>
+      <c r="B20" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="10"/>
+      <c r="B21" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" s="9"/>
+      <c r="B22" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="9"/>
+      <c r="C23" t="s">
+        <v>118</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A4:A8"/>
+    <mergeCell ref="A9:A12"/>
+    <mergeCell ref="A14:A18"/>
+    <mergeCell ref="A19:A22"/>
+  </mergeCells>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G5 G6 G10 G11 G13 G16 G18">
+      <formula1>"未进行,进行中,已暂停,已完成,未完成"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G4 G9 G12 G14 G15 G17 G7:G8">
+      <formula1>"未进行,进行中,已暂停,已完成"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>

</xml_diff>

<commit_message>
Site updated: 2023-01-01 00:30:46
</commit_message>
<xml_diff>
--- a/file/personal/roleImportant/角色要事记录表_2022.xlsx
+++ b/file/personal/roleImportant/角色要事记录表_2022.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="16860" activeTab="7"/>
+    <workbookView windowWidth="27400" windowHeight="14700" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="角色目录" sheetId="2" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="119">
   <si>
     <t>角色</t>
   </si>
@@ -146,9 +146,6 @@
     <t>登记已经完成半年后正式办理</t>
   </si>
   <si>
-    <t>进行中</t>
-  </si>
-  <si>
     <t>如何抵御通货膨胀</t>
   </si>
   <si>
@@ -378,6 +375,9 @@
   </si>
   <si>
     <t>考公计划制定</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -385,10 +385,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -405,14 +405,22 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Helvetica Neue"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="0"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -426,22 +434,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Helvetica Neue"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
-      <sz val="15"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Helvetica Neue"/>
       <charset val="134"/>
@@ -449,22 +443,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFA7D00"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -478,9 +457,46 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Helvetica Neue"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -501,9 +517,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FFFF0000"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -516,25 +531,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Helvetica Neue"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Helvetica Neue"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF800080"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -548,14 +547,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="Helvetica Neue"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="44">
+  <fills count="43">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -631,13 +631,79 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.6"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -649,109 +715,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -769,7 +733,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -781,43 +793,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1130,8 +1124,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1148,8 +1142,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1184,13 +1178,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FF7F7F7F"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1210,17 +1208,13 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1229,152 +1223,152 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="43" borderId="30" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="42" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="26" borderId="30" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="28" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="27" borderId="27" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="26" borderId="26" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="26" borderId="28" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="42" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="28" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="30" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="27" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="26" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="23" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="29" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="24" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="25" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="34" borderId="29" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="25" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1500,9 +1494,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1643,6 +1634,11 @@
       <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -2711,12 +2707,11 @@
       </a:style>
     </a:txDef>
   </a:objectDefaults>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:E23"/>
   <sheetViews>
@@ -2724,7 +2719,7 @@
       <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.64285714285714" defaultRowHeight="13.5" customHeight="1" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9.64423076923077" defaultRowHeight="13.5" customHeight="1" outlineLevelCol="4"/>
   <cols>
     <col min="1" max="1" width="9" style="24" customWidth="1"/>
     <col min="2" max="16384" width="6" style="24" customWidth="1"/>
@@ -2734,200 +2729,200 @@
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="44"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
+      <c r="B1" s="43"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
     </row>
     <row r="2" ht="14" customHeight="1" spans="1:5">
-      <c r="A2" s="46" t="s">
+      <c r="A2" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="44"/>
-      <c r="C2" s="45"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="45"/>
+      <c r="B2" s="43"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
     </row>
     <row r="3" ht="14" customHeight="1" spans="1:5">
-      <c r="A3" s="46" t="s">
+      <c r="A3" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="44"/>
-      <c r="C3" s="45"/>
-      <c r="D3" s="45"/>
-      <c r="E3" s="45"/>
+      <c r="B3" s="43"/>
+      <c r="C3" s="44"/>
+      <c r="D3" s="44"/>
+      <c r="E3" s="44"/>
     </row>
     <row r="4" ht="14" customHeight="1" spans="1:5">
-      <c r="A4" s="47" t="s">
+      <c r="A4" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="44"/>
-      <c r="C4" s="45"/>
-      <c r="D4" s="45"/>
-      <c r="E4" s="45"/>
+      <c r="B4" s="43"/>
+      <c r="C4" s="44"/>
+      <c r="D4" s="44"/>
+      <c r="E4" s="44"/>
     </row>
     <row r="5" ht="14" customHeight="1" spans="1:5">
-      <c r="A5" s="48"/>
-      <c r="B5" s="44"/>
-      <c r="C5" s="45"/>
-      <c r="D5" s="45"/>
-      <c r="E5" s="45"/>
+      <c r="A5" s="47"/>
+      <c r="B5" s="43"/>
+      <c r="C5" s="44"/>
+      <c r="D5" s="44"/>
+      <c r="E5" s="44"/>
     </row>
     <row r="6" ht="14" customHeight="1" spans="1:5">
-      <c r="A6" s="48"/>
-      <c r="B6" s="44"/>
-      <c r="C6" s="45"/>
-      <c r="D6" s="45"/>
-      <c r="E6" s="45"/>
+      <c r="A6" s="47"/>
+      <c r="B6" s="43"/>
+      <c r="C6" s="44"/>
+      <c r="D6" s="44"/>
+      <c r="E6" s="44"/>
     </row>
     <row r="7" ht="14" customHeight="1" spans="1:5">
-      <c r="A7" s="47" t="s">
+      <c r="A7" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="44"/>
-      <c r="C7" s="45"/>
-      <c r="D7" s="45"/>
-      <c r="E7" s="45"/>
+      <c r="B7" s="43"/>
+      <c r="C7" s="44"/>
+      <c r="D7" s="44"/>
+      <c r="E7" s="44"/>
     </row>
     <row r="8" ht="14" customHeight="1" spans="1:5">
-      <c r="A8" s="48"/>
-      <c r="B8" s="44"/>
-      <c r="C8" s="45"/>
-      <c r="D8" s="45"/>
-      <c r="E8" s="45"/>
+      <c r="A8" s="47"/>
+      <c r="B8" s="43"/>
+      <c r="C8" s="44"/>
+      <c r="D8" s="44"/>
+      <c r="E8" s="44"/>
     </row>
     <row r="9" ht="14" customHeight="1" spans="1:5">
-      <c r="A9" s="48"/>
-      <c r="B9" s="44"/>
-      <c r="C9" s="45"/>
-      <c r="D9" s="45"/>
-      <c r="E9" s="45"/>
+      <c r="A9" s="47"/>
+      <c r="B9" s="43"/>
+      <c r="C9" s="44"/>
+      <c r="D9" s="44"/>
+      <c r="E9" s="44"/>
     </row>
     <row r="10" ht="14" customHeight="1" spans="1:5">
-      <c r="A10" s="47" t="s">
+      <c r="A10" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="44"/>
-      <c r="C10" s="45"/>
-      <c r="D10" s="45"/>
-      <c r="E10" s="45"/>
+      <c r="B10" s="43"/>
+      <c r="C10" s="44"/>
+      <c r="D10" s="44"/>
+      <c r="E10" s="44"/>
     </row>
     <row r="11" ht="14" customHeight="1" spans="1:5">
-      <c r="A11" s="47" t="s">
+      <c r="A11" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="44"/>
-      <c r="C11" s="45"/>
-      <c r="D11" s="45"/>
-      <c r="E11" s="45"/>
+      <c r="B11" s="43"/>
+      <c r="C11" s="44"/>
+      <c r="D11" s="44"/>
+      <c r="E11" s="44"/>
     </row>
     <row r="12" ht="14" customHeight="1" spans="1:5">
-      <c r="A12" s="47" t="s">
+      <c r="A12" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="B12" s="44"/>
-      <c r="C12" s="45"/>
-      <c r="D12" s="45"/>
-      <c r="E12" s="45"/>
+      <c r="B12" s="43"/>
+      <c r="C12" s="44"/>
+      <c r="D12" s="44"/>
+      <c r="E12" s="44"/>
     </row>
     <row r="13" ht="14" customHeight="1" spans="1:5">
-      <c r="A13" s="47" t="s">
+      <c r="A13" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="B13" s="44"/>
-      <c r="C13" s="45"/>
-      <c r="D13" s="45"/>
-      <c r="E13" s="45"/>
+      <c r="B13" s="43"/>
+      <c r="C13" s="44"/>
+      <c r="D13" s="44"/>
+      <c r="E13" s="44"/>
     </row>
     <row r="14" ht="14" customHeight="1" spans="1:5">
-      <c r="A14" s="47" t="s">
+      <c r="A14" s="46" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="44"/>
-      <c r="C14" s="45"/>
-      <c r="D14" s="45"/>
-      <c r="E14" s="45"/>
+      <c r="B14" s="43"/>
+      <c r="C14" s="44"/>
+      <c r="D14" s="44"/>
+      <c r="E14" s="44"/>
     </row>
     <row r="15" ht="14" customHeight="1" spans="1:5">
-      <c r="A15" s="47" t="s">
+      <c r="A15" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="B15" s="44"/>
-      <c r="C15" s="45"/>
-      <c r="D15" s="45"/>
-      <c r="E15" s="45"/>
+      <c r="B15" s="43"/>
+      <c r="C15" s="44"/>
+      <c r="D15" s="44"/>
+      <c r="E15" s="44"/>
     </row>
     <row r="16" ht="14" customHeight="1" spans="1:5">
-      <c r="A16" s="47" t="s">
+      <c r="A16" s="46" t="s">
         <v>11</v>
       </c>
-      <c r="B16" s="44"/>
-      <c r="C16" s="45"/>
-      <c r="D16" s="45"/>
-      <c r="E16" s="45"/>
+      <c r="B16" s="43"/>
+      <c r="C16" s="44"/>
+      <c r="D16" s="44"/>
+      <c r="E16" s="44"/>
     </row>
     <row r="17" ht="14" customHeight="1" spans="1:5">
-      <c r="A17" s="47" t="s">
+      <c r="A17" s="46" t="s">
         <v>12</v>
       </c>
-      <c r="B17" s="44"/>
-      <c r="C17" s="45"/>
-      <c r="D17" s="45"/>
-      <c r="E17" s="45"/>
+      <c r="B17" s="43"/>
+      <c r="C17" s="44"/>
+      <c r="D17" s="44"/>
+      <c r="E17" s="44"/>
     </row>
     <row r="18" ht="14" customHeight="1" spans="1:5">
-      <c r="A18" s="47" t="s">
+      <c r="A18" s="46" t="s">
         <v>13</v>
       </c>
-      <c r="B18" s="44"/>
-      <c r="C18" s="45"/>
-      <c r="D18" s="45"/>
-      <c r="E18" s="45"/>
+      <c r="B18" s="43"/>
+      <c r="C18" s="44"/>
+      <c r="D18" s="44"/>
+      <c r="E18" s="44"/>
     </row>
     <row r="19" ht="14" customHeight="1" spans="1:5">
-      <c r="A19" s="47" t="s">
+      <c r="A19" s="46" t="s">
         <v>14</v>
       </c>
-      <c r="B19" s="44"/>
-      <c r="C19" s="45"/>
-      <c r="D19" s="45"/>
-      <c r="E19" s="45"/>
+      <c r="B19" s="43"/>
+      <c r="C19" s="44"/>
+      <c r="D19" s="44"/>
+      <c r="E19" s="44"/>
     </row>
     <row r="20" ht="14" customHeight="1" spans="1:5">
-      <c r="A20" s="47" t="s">
+      <c r="A20" s="46" t="s">
         <v>15</v>
       </c>
-      <c r="B20" s="44"/>
-      <c r="C20" s="45"/>
-      <c r="D20" s="45"/>
-      <c r="E20" s="45"/>
+      <c r="B20" s="43"/>
+      <c r="C20" s="44"/>
+      <c r="D20" s="44"/>
+      <c r="E20" s="44"/>
     </row>
     <row r="21" ht="14" customHeight="1" spans="1:5">
-      <c r="A21" s="47" t="s">
+      <c r="A21" s="46" t="s">
         <v>16</v>
       </c>
-      <c r="B21" s="44"/>
-      <c r="C21" s="45"/>
-      <c r="D21" s="45"/>
-      <c r="E21" s="45"/>
+      <c r="B21" s="43"/>
+      <c r="C21" s="44"/>
+      <c r="D21" s="44"/>
+      <c r="E21" s="44"/>
     </row>
     <row r="22" ht="14" customHeight="1" spans="1:5">
-      <c r="A22" s="47" t="s">
+      <c r="A22" s="46" t="s">
         <v>17</v>
       </c>
-      <c r="B22" s="44"/>
-      <c r="C22" s="45"/>
-      <c r="D22" s="45"/>
-      <c r="E22" s="45"/>
+      <c r="B22" s="43"/>
+      <c r="C22" s="44"/>
+      <c r="D22" s="44"/>
+      <c r="E22" s="44"/>
     </row>
     <row r="23" ht="14" customHeight="1" spans="1:5">
-      <c r="A23" s="46" t="s">
+      <c r="A23" s="45" t="s">
         <v>18</v>
       </c>
-      <c r="B23" s="44"/>
-      <c r="C23" s="45"/>
-      <c r="D23" s="45"/>
-      <c r="E23" s="45"/>
+      <c r="B23" s="43"/>
+      <c r="C23" s="44"/>
+      <c r="D23" s="44"/>
+      <c r="E23" s="44"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2943,25 +2938,25 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="D21" sqref="D21"/>
+      <selection pane="bottomRight" activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.64285714285714" defaultRowHeight="13" customHeight="1" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9.64423076923077" defaultRowHeight="13" customHeight="1" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="1" width="16.3571428571429" style="24" customWidth="1"/>
-    <col min="2" max="2" width="99.1160714285714" style="31" customWidth="1"/>
-    <col min="3" max="16384" width="16.3571428571429" style="24" customWidth="1"/>
+    <col min="1" max="1" width="16.3557692307692" style="24" customWidth="1"/>
+    <col min="2" max="2" width="99.1153846153846" style="31" customWidth="1"/>
+    <col min="3" max="16384" width="16.3557692307692" style="24" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.55" customHeight="1" spans="1:3">
@@ -3075,16 +3070,16 @@
       <c r="B11" s="38" t="s">
         <v>40</v>
       </c>
-      <c r="C11" s="42" t="s">
-        <v>41</v>
+      <c r="C11" s="15" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="12" ht="13.35" customHeight="1" spans="1:3">
       <c r="A12" s="39" t="s">
+        <v>41</v>
+      </c>
+      <c r="B12" s="38" t="s">
         <v>42</v>
-      </c>
-      <c r="B12" s="38" t="s">
-        <v>43</v>
       </c>
       <c r="C12" s="40" t="s">
         <v>29</v>
@@ -3092,10 +3087,10 @@
     </row>
     <row r="13" ht="13.35" customHeight="1" spans="1:3">
       <c r="A13" s="39" t="s">
+        <v>43</v>
+      </c>
+      <c r="B13" s="38" t="s">
         <v>44</v>
-      </c>
-      <c r="B13" s="38" t="s">
-        <v>45</v>
       </c>
       <c r="C13" s="40" t="s">
         <v>29</v>
@@ -3103,21 +3098,21 @@
     </row>
     <row r="14" ht="13.35" customHeight="1" spans="1:3">
       <c r="A14" s="37" t="s">
+        <v>45</v>
+      </c>
+      <c r="B14" s="38" t="s">
         <v>46</v>
       </c>
-      <c r="B14" s="38" t="s">
-        <v>47</v>
-      </c>
-      <c r="C14" s="42" t="s">
-        <v>41</v>
+      <c r="C14" s="15" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="15" ht="13.35" customHeight="1" spans="1:3">
       <c r="A15" s="37" t="s">
+        <v>47</v>
+      </c>
+      <c r="B15" s="38" t="s">
         <v>48</v>
-      </c>
-      <c r="B15" s="38" t="s">
-        <v>49</v>
       </c>
       <c r="C15" s="15" t="s">
         <v>24</v>
@@ -3125,73 +3120,73 @@
     </row>
     <row r="16" ht="13.35" customHeight="1" spans="1:3">
       <c r="A16" s="37" t="s">
+        <v>49</v>
+      </c>
+      <c r="B16" s="38" t="s">
         <v>50</v>
       </c>
-      <c r="B16" s="38" t="s">
-        <v>51</v>
-      </c>
-      <c r="C16" s="42" t="s">
-        <v>41</v>
+      <c r="C16" s="15" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="17" ht="13.35" customHeight="1" spans="1:3">
       <c r="A17" s="37" t="s">
+        <v>51</v>
+      </c>
+      <c r="B17" s="38" t="s">
         <v>52</v>
-      </c>
-      <c r="B17" s="38" t="s">
-        <v>53</v>
       </c>
       <c r="C17" s="40" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="18" ht="13.35" customHeight="1" spans="1:3">
-      <c r="A18" s="43" t="s">
+      <c r="A18" s="42" t="s">
+        <v>53</v>
+      </c>
+      <c r="B18" s="22" t="s">
         <v>54</v>
-      </c>
-      <c r="B18" s="22" t="s">
-        <v>55</v>
       </c>
       <c r="C18" s="22"/>
     </row>
     <row r="19" customHeight="1" spans="1:2">
       <c r="A19" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="B19" s="31" t="s">
         <v>56</v>
-      </c>
-      <c r="B19" s="31" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="20" customHeight="1" spans="1:2">
       <c r="A20" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="B20" s="31" t="s">
         <v>58</v>
-      </c>
-      <c r="B20" s="31" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="21" customHeight="1" spans="1:2">
       <c r="A21" s="24" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B21" s="31" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="22" customHeight="1" spans="1:2">
       <c r="A22" s="24" t="s">
+        <v>60</v>
+      </c>
+      <c r="B22" s="31" t="s">
         <v>61</v>
-      </c>
-      <c r="B22" s="31" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="23" customHeight="1" spans="1:3">
       <c r="A23" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="B23" s="31" t="s">
         <v>63</v>
-      </c>
-      <c r="B23" s="31" t="s">
-        <v>64</v>
       </c>
       <c r="C23" s="15" t="s">
         <v>24</v>
@@ -3212,7 +3207,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -3224,14 +3219,14 @@
       <selection pane="topRight" activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.64285714285714" defaultRowHeight="13" customHeight="1" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="9.64423076923077" defaultRowHeight="13" customHeight="1" outlineLevelCol="7"/>
   <cols>
-    <col min="1" max="16384" width="16.3571428571429" style="24" customWidth="1"/>
+    <col min="1" max="16384" width="16.3557692307692" style="24" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="14" customHeight="1" spans="1:8">
       <c r="A1" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B1" s="2">
         <v>20220401</v>
@@ -3245,7 +3240,7 @@
     </row>
     <row r="2" ht="14" customHeight="1" spans="1:8">
       <c r="A2" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B2" s="5">
         <v>20220430</v>
@@ -3259,7 +3254,7 @@
     </row>
     <row r="3" ht="14" customHeight="1" spans="1:8">
       <c r="A3" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>1</v>
@@ -3277,15 +3272,15 @@
         <v>14</v>
       </c>
       <c r="G3" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="H3" s="7" t="s">
         <v>68</v>
-      </c>
-      <c r="H3" s="7" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="4" ht="13.65" customHeight="1" spans="1:8">
       <c r="A4" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C4" s="25"/>
       <c r="D4" s="25"/>
@@ -3300,7 +3295,7 @@
       <c r="C5" s="22"/>
       <c r="D5" s="22"/>
       <c r="E5" s="22" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F5" s="22"/>
       <c r="G5" s="15" t="s">
@@ -3314,7 +3309,7 @@
       <c r="C6" s="22"/>
       <c r="D6" s="22"/>
       <c r="E6" s="22" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F6" s="22"/>
       <c r="G6" s="15" t="s">
@@ -3325,7 +3320,7 @@
     <row r="7" ht="13.35" customHeight="1" spans="1:8">
       <c r="A7" s="17"/>
       <c r="B7" s="27" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C7" s="22"/>
       <c r="D7" s="22"/>
@@ -3348,7 +3343,7 @@
     </row>
     <row r="9" ht="13.65" customHeight="1" spans="1:8">
       <c r="A9" s="8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B9" s="26"/>
       <c r="C9" s="22"/>
@@ -3380,10 +3375,10 @@
     </row>
     <row r="12" ht="13.65" customHeight="1" spans="1:8">
       <c r="A12" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="B12" s="28" t="s">
         <v>75</v>
-      </c>
-      <c r="B12" s="28" t="s">
-        <v>76</v>
       </c>
       <c r="C12" s="22"/>
       <c r="D12" s="22"/>
@@ -3398,16 +3393,16 @@
       <c r="A13" s="17"/>
       <c r="B13" s="27"/>
       <c r="C13" s="22" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D13" s="22"/>
       <c r="E13" s="22"/>
       <c r="F13" s="22"/>
       <c r="G13" s="19" t="s">
+        <v>76</v>
+      </c>
+      <c r="H13" s="22" t="s">
         <v>77</v>
-      </c>
-      <c r="H13" s="22" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="14" ht="14" customHeight="1" spans="1:8">
@@ -3422,7 +3417,7 @@
     </row>
     <row r="15" ht="13.65" customHeight="1" spans="1:8">
       <c r="A15" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B15" s="26"/>
       <c r="C15" s="22"/>
@@ -3483,7 +3478,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:H18"/>
   <sheetViews>
@@ -3491,18 +3486,18 @@
       <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.64285714285714" defaultRowHeight="13.1" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="9.64423076923077" defaultRowHeight="16.8" outlineLevelCol="7"/>
   <cols>
-    <col min="1" max="1" width="11.7321428571429" customWidth="1"/>
-    <col min="2" max="2" width="17.9732142857143" customWidth="1"/>
-    <col min="3" max="3" width="12.0267857142857" customWidth="1"/>
+    <col min="1" max="1" width="11.7307692307692" customWidth="1"/>
+    <col min="2" max="2" width="17.9711538461538" customWidth="1"/>
+    <col min="3" max="3" width="12.0288461538462" customWidth="1"/>
     <col min="4" max="4" width="15" customWidth="1"/>
-    <col min="8" max="8" width="15.4910714285714" customWidth="1"/>
+    <col min="8" max="8" width="15.4903846153846" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B1" s="2">
         <v>20220501</v>
@@ -3516,7 +3511,7 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B2" s="5">
         <v>20220531</v>
@@ -3530,7 +3525,7 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>1</v>
@@ -3548,18 +3543,18 @@
         <v>14</v>
       </c>
       <c r="G3" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="H3" s="7" t="s">
         <v>68</v>
-      </c>
-      <c r="H3" s="7" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B4" s="24" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C4" s="25"/>
       <c r="D4" s="25"/>
@@ -3575,7 +3570,7 @@
       <c r="B5" s="26"/>
       <c r="C5" s="22"/>
       <c r="D5" s="22" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E5" s="22"/>
       <c r="F5" s="22"/>
@@ -3588,7 +3583,7 @@
       <c r="A6" s="17"/>
       <c r="B6" s="27"/>
       <c r="C6" s="22" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D6" s="22"/>
       <c r="E6" s="22"/>
@@ -3601,7 +3596,7 @@
     <row r="7" spans="1:8">
       <c r="A7" s="17"/>
       <c r="B7" s="27" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C7" s="22"/>
       <c r="D7" s="22"/>
@@ -3623,10 +3618,10 @@
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B9" s="26" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C9" s="22"/>
       <c r="D9" s="22"/>
@@ -3640,7 +3635,7 @@
     <row r="10" spans="1:8">
       <c r="A10" s="17"/>
       <c r="B10" s="27" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C10" s="22"/>
       <c r="D10" s="22"/>
@@ -3662,17 +3657,17 @@
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B12" s="28" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C12" s="22"/>
       <c r="D12" s="22"/>
       <c r="E12" s="22"/>
       <c r="F12" s="22"/>
       <c r="G12" s="23" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H12" s="22"/>
     </row>
@@ -3697,17 +3692,17 @@
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B15" s="26" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C15" s="22"/>
       <c r="D15" s="22"/>
       <c r="E15" s="22"/>
       <c r="F15" s="22"/>
       <c r="G15" s="23" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H15" s="22"/>
     </row>
@@ -3760,7 +3755,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:H18"/>
   <sheetViews>
@@ -3768,18 +3763,18 @@
       <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.64285714285714" defaultRowHeight="13.1" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="9.64423076923077" defaultRowHeight="16.8" outlineLevelCol="7"/>
   <cols>
-    <col min="1" max="1" width="11.7321428571429" customWidth="1"/>
-    <col min="2" max="2" width="17.9732142857143" customWidth="1"/>
-    <col min="3" max="3" width="12.0267857142857" customWidth="1"/>
+    <col min="1" max="1" width="11.7307692307692" customWidth="1"/>
+    <col min="2" max="2" width="17.9711538461538" customWidth="1"/>
+    <col min="3" max="3" width="12.0288461538462" customWidth="1"/>
     <col min="4" max="4" width="15" customWidth="1"/>
-    <col min="8" max="8" width="15.4910714285714" customWidth="1"/>
+    <col min="8" max="8" width="15.4903846153846" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B1" s="2">
         <v>20220601</v>
@@ -3793,7 +3788,7 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B2" s="5">
         <v>20220630</v>
@@ -3807,7 +3802,7 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>1</v>
@@ -3825,18 +3820,18 @@
         <v>14</v>
       </c>
       <c r="G3" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="H3" s="7" t="s">
         <v>68</v>
-      </c>
-      <c r="H3" s="7" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G4" s="15" t="s">
         <v>24</v>
@@ -3856,10 +3851,10 @@
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G9" s="15" t="s">
         <v>24</v>
@@ -3873,10 +3868,10 @@
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B12" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G12" s="15" t="s">
         <v>24</v>
@@ -3885,13 +3880,13 @@
     <row r="13" spans="1:8">
       <c r="A13" s="17"/>
       <c r="B13" t="s">
+        <v>89</v>
+      </c>
+      <c r="G13" s="23" t="s">
+        <v>86</v>
+      </c>
+      <c r="H13" t="s">
         <v>90</v>
-      </c>
-      <c r="G13" s="23" t="s">
-        <v>87</v>
-      </c>
-      <c r="H13" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="14" spans="1:1">
@@ -3899,22 +3894,22 @@
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B15" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G15" s="23" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" s="17"/>
       <c r="B16" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G16" s="23" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="17" spans="1:1">
@@ -3948,7 +3943,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:H17"/>
   <sheetViews>
@@ -3956,14 +3951,14 @@
       <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.64285714285714" defaultRowHeight="13.1" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="9.64423076923077" defaultRowHeight="16.8" outlineLevelCol="7"/>
   <cols>
-    <col min="2" max="2" width="25.3214285714286" customWidth="1"/>
+    <col min="2" max="2" width="25.3173076923077" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B1" s="2">
         <v>20220701</v>
@@ -3977,7 +3972,7 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B2" s="5">
         <v>20220731</v>
@@ -3991,7 +3986,7 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>1</v>
@@ -4009,18 +4004,18 @@
         <v>14</v>
       </c>
       <c r="G3" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="H3" s="7" t="s">
         <v>68</v>
-      </c>
-      <c r="H3" s="7" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G4" s="15" t="s">
         <v>24</v>
@@ -4029,7 +4024,7 @@
     <row r="5" spans="1:7">
       <c r="A5" s="17"/>
       <c r="B5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G5" s="15" t="s">
         <v>24</v>
@@ -4046,10 +4041,10 @@
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G9" s="15" t="s">
         <v>24</v>
@@ -4058,7 +4053,7 @@
     <row r="10" spans="1:7">
       <c r="A10" s="17"/>
       <c r="B10" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G10" s="15" t="s">
         <v>24</v>
@@ -4067,7 +4062,7 @@
     <row r="11" spans="1:7">
       <c r="A11" s="18"/>
       <c r="B11" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G11" s="15" t="s">
         <v>24</v>
@@ -4075,7 +4070,7 @@
     </row>
     <row r="12" spans="1:1">
       <c r="A12" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:1">
@@ -4086,7 +4081,7 @@
     </row>
     <row r="15" spans="1:1">
       <c r="A15" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="16" spans="1:1">
@@ -4113,26 +4108,26 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.64285714285714" defaultRowHeight="13.1" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="9.64423076923077" defaultRowHeight="16.8" outlineLevelCol="7"/>
   <cols>
-    <col min="2" max="2" width="20.0267857142857" customWidth="1"/>
-    <col min="4" max="4" width="13.2857142857143" customWidth="1"/>
-    <col min="5" max="5" width="9.77678571428571" customWidth="1"/>
-    <col min="6" max="6" width="19.5446428571429" customWidth="1"/>
-    <col min="8" max="8" width="19.8660714285714" customWidth="1"/>
+    <col min="2" max="2" width="20.0288461538462" customWidth="1"/>
+    <col min="4" max="4" width="13.2884615384615" customWidth="1"/>
+    <col min="5" max="5" width="9.77884615384615" customWidth="1"/>
+    <col min="6" max="6" width="19.5480769230769" customWidth="1"/>
+    <col min="8" max="8" width="19.8653846153846" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B1" s="2">
         <v>20220801</v>
@@ -4146,7 +4141,7 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B2" s="5">
         <v>20220831</v>
@@ -4160,7 +4155,7 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>1</v>
@@ -4178,18 +4173,18 @@
         <v>14</v>
       </c>
       <c r="G3" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="H3" s="7" t="s">
         <v>68</v>
-      </c>
-      <c r="H3" s="7" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G4" s="15" t="s">
         <v>24</v>
@@ -4198,31 +4193,31 @@
     <row r="5" spans="1:8">
       <c r="A5" s="9"/>
       <c r="B5" t="s">
+        <v>97</v>
+      </c>
+      <c r="G5" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="H5" t="s">
         <v>98</v>
-      </c>
-      <c r="G5" s="16" t="s">
-        <v>87</v>
-      </c>
-      <c r="H5" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="9"/>
       <c r="B6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G6" s="19" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="9"/>
       <c r="D7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G7" s="15" t="s">
         <v>24</v>
@@ -4231,7 +4226,7 @@
     <row r="8" spans="1:7">
       <c r="A8" s="9"/>
       <c r="F8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G8" s="15" t="s">
         <v>24</v>
@@ -4239,72 +4234,72 @@
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B9" t="s">
+        <v>102</v>
+      </c>
+      <c r="G9" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="H9" t="s">
         <v>103</v>
-      </c>
-      <c r="G9" s="16" t="s">
-        <v>87</v>
-      </c>
-      <c r="H9" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="9"/>
       <c r="B10" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G10" s="16" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H10" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="10"/>
       <c r="B11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G11" s="16" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H11" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="9"/>
       <c r="B12" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G12" s="16" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B13" t="s">
+        <v>102</v>
+      </c>
+      <c r="G13" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="H13" t="s">
         <v>103</v>
-      </c>
-      <c r="G13" s="16" t="s">
-        <v>87</v>
-      </c>
-      <c r="H13" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="9"/>
       <c r="B14" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G14" s="15" t="s">
         <v>24</v>
@@ -4313,19 +4308,19 @@
     <row r="15" spans="1:8">
       <c r="A15" s="10"/>
       <c r="B15" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G15" s="16" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H15" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" s="9"/>
       <c r="B16" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G16" s="15" t="s">
         <v>24</v>
@@ -4336,66 +4331,66 @@
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B18" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="9"/>
       <c r="B19" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="10"/>
       <c r="B20" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="9"/>
       <c r="B21" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" s="9"/>
       <c r="B22" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="B23" t="s">
         <v>110</v>
-      </c>
-      <c r="B23" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" s="17"/>
       <c r="B24" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" s="17"/>
       <c r="B25" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" s="17"/>
       <c r="B26" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" s="18"/>
       <c r="B27" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
   </sheetData>
@@ -4420,26 +4415,26 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:H23"/>
+  <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="B17" sqref="17:17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.64285714285714" defaultRowHeight="13.1" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="9.64423076923077" defaultRowHeight="16.8" outlineLevelCol="7"/>
   <cols>
-    <col min="2" max="2" width="20.0267857142857" customWidth="1"/>
-    <col min="4" max="4" width="13.2857142857143" customWidth="1"/>
-    <col min="5" max="5" width="9.77678571428571" customWidth="1"/>
-    <col min="6" max="6" width="19.5446428571429" customWidth="1"/>
-    <col min="8" max="8" width="19.8660714285714" customWidth="1"/>
+    <col min="2" max="2" width="20.0288461538462" customWidth="1"/>
+    <col min="4" max="4" width="13.2884615384615" customWidth="1"/>
+    <col min="5" max="5" width="9.77884615384615" customWidth="1"/>
+    <col min="6" max="6" width="19.5480769230769" customWidth="1"/>
+    <col min="8" max="8" width="19.8653846153846" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B1" s="2">
         <v>20220901</v>
@@ -4453,7 +4448,7 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B2" s="5">
         <v>20220930</v>
@@ -4467,7 +4462,7 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>1</v>
@@ -4485,15 +4480,15 @@
         <v>14</v>
       </c>
       <c r="G3" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="H3" s="7" t="s">
         <v>68</v>
-      </c>
-      <c r="H3" s="7" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="5" spans="1:1">
@@ -4510,10 +4505,10 @@
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B9" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G9" s="15" t="s">
         <v>24</v>
@@ -4522,25 +4517,25 @@
     <row r="10" spans="1:7">
       <c r="A10" s="9"/>
       <c r="B10" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G10" s="16" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="10"/>
       <c r="B11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G11" s="16" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="9"/>
       <c r="B12" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G12" s="15" t="s">
         <v>24</v>
@@ -4549,18 +4544,18 @@
     <row r="13" spans="1:7">
       <c r="A13" s="9"/>
       <c r="C13" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G13" s="16" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B14" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G14" s="15" t="s">
         <v>24</v>
@@ -4569,7 +4564,7 @@
     <row r="15" spans="1:7">
       <c r="A15" s="9"/>
       <c r="B15" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G15" s="15" t="s">
         <v>24</v>
@@ -4578,16 +4573,16 @@
     <row r="16" spans="1:7">
       <c r="A16" s="10"/>
       <c r="B16" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G16" s="16" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="17" spans="1:7">
       <c r="A17" s="9"/>
       <c r="B17" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G17" s="15" t="s">
         <v>24</v>
@@ -4596,41 +4591,46 @@
     <row r="18" spans="1:7">
       <c r="A18" s="9"/>
       <c r="C18" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G18" s="16" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B19" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="9"/>
       <c r="B20" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="10"/>
       <c r="B21" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" s="9"/>
       <c r="B22" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" s="9"/>
       <c r="C23" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="26" spans="7:7">
+      <c r="G26" t="s">
         <v>118</v>
       </c>
     </row>

</xml_diff>